<commit_message>
Some changes made to Generic plotter and tvDataFeed usage.
</commit_message>
<xml_diff>
--- a/Generic_Macro/Control.xlsx
+++ b/Generic_Macro/Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimmi\OneDrive\Documents\Documents\Scripts\VenV\Plebs_Macro\Generic_Macro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/TempVenv/Plebs_Macro/Generic_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4B83F4-1FBA-46DC-9B7A-00025FB8B938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC430E67-7267-7D43-A5F5-2090231A2F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_Input" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="364">
   <si>
     <t>Index</t>
   </si>
@@ -1295,26 +1295,17 @@
     <t>1970-01-01</t>
   </si>
   <si>
-    <t>WALCL</t>
-  </si>
-  <si>
-    <t>fedBal</t>
-  </si>
-  <si>
-    <t>Fed balance sheet</t>
-  </si>
-  <si>
     <t>Soft &amp; Hard money</t>
   </si>
   <si>
-    <t>Millions of US $</t>
+    <t>Bil. of US $</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2108,26 +2099,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="9" width="44" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="15.5" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" customWidth="1"/>
+    <col min="15" max="15" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2165,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2182,7 +2173,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>145</v>
@@ -2214,30 +2205,30 @@
         <v>1000000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="18">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>362</v>
+        <v>106</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>145</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>363</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>364</v>
+        <v>88</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>30</v>
@@ -2249,33 +2240,33 @@
       <c r="N3" s="9"/>
       <c r="O3" s="10"/>
     </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="18">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>106</v>
+        <v>169</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>145</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>90</v>
+        <v>170</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>88</v>
+        <v>360</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>30</v>
+        <v>172</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
@@ -2284,80 +2275,63 @@
       <c r="N4" s="9"/>
       <c r="O4" s="10"/>
     </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="18">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>145</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>170</v>
+        <v>23</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>360</v>
+        <v>165</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>172</v>
+        <v>363</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="O5" s="10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>366</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10">
-        <f>10^6</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" ht="16">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2372,7 +2346,7 @@
       <c r="L7" s="14"/>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="16">
       <c r="A8" s="16" t="s">
         <v>31</v>
       </c>
@@ -2392,7 +2366,7 @@
       <c r="K8" s="18"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="16">
       <c r="A9" s="16" t="s">
         <v>33</v>
       </c>
@@ -2410,7 +2384,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="16">
       <c r="A10" s="13"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -2424,7 +2398,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="16">
       <c r="A11" s="20" t="s">
         <v>35</v>
       </c>
@@ -2442,12 +2416,12 @@
       <c r="K11" s="18"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="16">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
@@ -2460,7 +2434,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="16">
       <c r="A13" s="21" t="s">
         <v>38</v>
       </c>
@@ -2478,7 +2452,7 @@
       <c r="K13" s="18"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="16">
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -2490,7 +2464,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="16">
       <c r="A15" s="21" t="s">
         <v>353</v>
       </c>
@@ -2508,7 +2482,7 @@
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="16">
       <c r="A16" s="51" t="s">
         <v>355</v>
       </c>
@@ -2524,7 +2498,7 @@
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16">
       <c r="A17" s="51" t="s">
         <v>354</v>
       </c>
@@ -2540,7 +2514,7 @@
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
     </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="16">
       <c r="A18" s="13"/>
       <c r="B18" s="23"/>
       <c r="C18" s="18"/>
@@ -2554,7 +2528,7 @@
       <c r="K18" s="18"/>
       <c r="L18" s="19"/>
     </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="16">
       <c r="A19" s="13"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -2568,7 +2542,7 @@
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -2579,7 +2553,7 @@
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -2592,7 +2566,7 @@
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="24"/>
       <c r="B22" s="25"/>
       <c r="C22" s="26"/>
@@ -2603,7 +2577,7 @@
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
@@ -2614,7 +2588,7 @@
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="24"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
@@ -2625,7 +2599,7 @@
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
     </row>
-    <row r="25" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="14">
       <c r="A25" s="24"/>
       <c r="B25" s="53"/>
       <c r="C25" s="54"/>
@@ -2639,7 +2613,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="24"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="24"/>
       <c r="B26" s="25"/>
       <c r="C26" s="25"/>
@@ -2652,32 +2626,32 @@
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="16">
       <c r="A27" s="15"/>
       <c r="E27" s="23"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="15"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="15"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="15"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="15"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="15"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="15"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="15"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="15"/>
     </row>
   </sheetData>
@@ -2761,22 +2735,22 @@
       <selection activeCell="I34" sqref="B34:I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="46.7109375" customWidth="1"/>
-    <col min="9" max="9" width="35.28515625" customWidth="1"/>
-    <col min="10" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" customWidth="1"/>
+    <col min="10" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="25.5" customWidth="1"/>
     <col min="14" max="14" width="119" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="D1" s="27" t="s">
         <v>39</v>
       </c>
@@ -2797,7 +2771,7 @@
       <c r="R1" s="31"/>
       <c r="S1" s="31"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
@@ -2839,7 +2813,7 @@
       <c r="R2" s="36"/>
       <c r="S2" s="37"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="B3" s="34" t="s">
         <v>14</v>
       </c>
@@ -2875,7 +2849,7 @@
       <c r="R3" s="35"/>
       <c r="S3" s="35"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="B4" s="34" t="s">
         <v>46</v>
       </c>
@@ -2911,7 +2885,7 @@
       <c r="R4" s="35"/>
       <c r="S4" s="35"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="B5" s="10" t="s">
         <v>51</v>
       </c>
@@ -2947,7 +2921,7 @@
       <c r="R5" s="35"/>
       <c r="S5" s="35"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="B6" s="34" t="s">
         <v>57</v>
       </c>
@@ -2983,7 +2957,7 @@
       <c r="R6" s="35"/>
       <c r="S6" s="35"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="B7" s="34" t="s">
         <v>63</v>
       </c>
@@ -3019,7 +2993,7 @@
       <c r="R7" s="35"/>
       <c r="S7" s="35"/>
     </row>
-    <row r="8" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="14">
       <c r="B8" s="39" t="s">
         <v>69</v>
       </c>
@@ -3050,7 +3024,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19">
       <c r="B9" s="34" t="s">
         <v>75</v>
       </c>
@@ -3081,7 +3055,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19">
       <c r="B10" s="10" t="s">
         <v>80</v>
       </c>
@@ -3115,7 +3089,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19">
       <c r="B11" s="10" t="s">
         <v>86</v>
       </c>
@@ -3145,7 +3119,7 @@
       </c>
       <c r="N11" s="35"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="B12" s="10" t="s">
         <v>51</v>
       </c>
@@ -3177,7 +3151,7 @@
       </c>
       <c r="N12" s="35"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="B13" s="10" t="s">
         <v>94</v>
       </c>
@@ -3209,7 +3183,7 @@
       </c>
       <c r="N13" s="35"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19">
       <c r="B14" s="10" t="s">
         <v>98</v>
       </c>
@@ -3238,7 +3212,7 @@
       </c>
       <c r="N14" s="35"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19">
       <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
@@ -3262,7 +3236,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19">
       <c r="B16" s="34" t="s">
         <v>51</v>
       </c>
@@ -3296,7 +3270,7 @@
       </c>
       <c r="N16" s="35"/>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:28">
       <c r="B17" s="34" t="s">
         <v>106</v>
       </c>
@@ -3331,7 +3305,7 @@
       </c>
       <c r="N17" s="35"/>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:28">
       <c r="B18" s="34" t="s">
         <v>109</v>
       </c>
@@ -3365,7 +3339,7 @@
       </c>
       <c r="N18" s="35"/>
     </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:28">
       <c r="B19" s="34" t="s">
         <v>113</v>
       </c>
@@ -3399,7 +3373,7 @@
       </c>
       <c r="N19" s="35"/>
     </row>
-    <row r="20" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:28" ht="12.75" customHeight="1">
       <c r="B20" s="34" t="s">
         <v>117</v>
       </c>
@@ -3445,7 +3419,7 @@
       <c r="AA20" s="43"/>
       <c r="AB20" s="43"/>
     </row>
-    <row r="21" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:28" ht="12.75" customHeight="1">
       <c r="B21" s="34" t="s">
         <v>122</v>
       </c>
@@ -3481,7 +3455,7 @@
       <c r="AA21" s="43"/>
       <c r="AB21" s="43"/>
     </row>
-    <row r="22" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:28" ht="12.75" customHeight="1">
       <c r="B22" s="10" t="s">
         <v>125</v>
       </c>
@@ -3517,7 +3491,7 @@
       <c r="AA22" s="43"/>
       <c r="AB22" s="43"/>
     </row>
-    <row r="23" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:28" ht="12.75" customHeight="1">
       <c r="B23" s="34" t="s">
         <v>128</v>
       </c>
@@ -3563,7 +3537,7 @@
       <c r="AA23" s="43"/>
       <c r="AB23" s="43"/>
     </row>
-    <row r="24" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:28" ht="12.75" customHeight="1">
       <c r="B24" s="10" t="s">
         <v>132</v>
       </c>
@@ -3599,7 +3573,7 @@
       <c r="AA24" s="43"/>
       <c r="AB24" s="43"/>
     </row>
-    <row r="25" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:28" ht="12.75" customHeight="1">
       <c r="B25" s="34" t="s">
         <v>135</v>
       </c>
@@ -3646,7 +3620,7 @@
       <c r="AA25" s="43"/>
       <c r="AB25" s="43"/>
     </row>
-    <row r="26" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:28" ht="12.75" customHeight="1">
       <c r="B26" s="34" t="s">
         <v>140</v>
       </c>
@@ -3693,7 +3667,7 @@
       <c r="AA26" s="43"/>
       <c r="AB26" s="43"/>
     </row>
-    <row r="27" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:28" ht="12.75" customHeight="1">
       <c r="B27" s="17" t="s">
         <v>144</v>
       </c>
@@ -3738,7 +3712,7 @@
       <c r="AA27" s="43"/>
       <c r="AB27" s="43"/>
     </row>
-    <row r="28" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:28" ht="12.75" customHeight="1">
       <c r="B28" s="10" t="s">
         <v>135</v>
       </c>
@@ -3785,7 +3759,7 @@
       <c r="AA28" s="43"/>
       <c r="AB28" s="43"/>
     </row>
-    <row r="29" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:28" ht="12.75" customHeight="1">
       <c r="B29" s="10" t="s">
         <v>153</v>
       </c>
@@ -3828,7 +3802,7 @@
       <c r="AA29" s="43"/>
       <c r="AB29" s="43"/>
     </row>
-    <row r="30" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:28" ht="12.75" customHeight="1">
       <c r="B30" s="10" t="s">
         <v>157</v>
       </c>
@@ -3875,7 +3849,7 @@
       <c r="AA30" s="43"/>
       <c r="AB30" s="43"/>
     </row>
-    <row r="31" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:28" ht="12.75" customHeight="1">
       <c r="B31" s="34" t="s">
         <v>106</v>
       </c>
@@ -3920,7 +3894,7 @@
       <c r="AA31" s="43"/>
       <c r="AB31" s="43"/>
     </row>
-    <row r="32" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:28" ht="12.75" customHeight="1">
       <c r="B32" s="34" t="s">
         <v>160</v>
       </c>
@@ -3953,7 +3927,7 @@
       <c r="AA32" s="43"/>
       <c r="AB32" s="43"/>
     </row>
-    <row r="33" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:28" ht="12.75" customHeight="1">
       <c r="B33" s="34" t="s">
         <v>162</v>
       </c>
@@ -4000,7 +3974,7 @@
       <c r="AA33" s="43"/>
       <c r="AB33" s="43"/>
     </row>
-    <row r="34" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:28" ht="12.75" customHeight="1">
       <c r="B34" s="34" t="s">
         <v>14</v>
       </c>
@@ -4047,7 +4021,7 @@
       <c r="AA34" s="43"/>
       <c r="AB34" s="43"/>
     </row>
-    <row r="35" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:28" ht="12.75" customHeight="1">
       <c r="B35" s="34" t="s">
         <v>22</v>
       </c>
@@ -4092,7 +4066,7 @@
       <c r="AA35" s="43"/>
       <c r="AB35" s="43"/>
     </row>
-    <row r="36" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:28" ht="12.75" customHeight="1">
       <c r="B36" s="34" t="s">
         <v>169</v>
       </c>
@@ -4139,7 +4113,7 @@
       <c r="AA36" s="43"/>
       <c r="AB36" s="43"/>
     </row>
-    <row r="37" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:28" ht="12.75" customHeight="1">
       <c r="B37" s="10" t="s">
         <v>153</v>
       </c>
@@ -4186,7 +4160,7 @@
       <c r="AA37" s="43"/>
       <c r="AB37" s="43"/>
     </row>
-    <row r="38" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:28" ht="12.75" customHeight="1">
       <c r="B38" s="34" t="s">
         <v>178</v>
       </c>
@@ -4233,7 +4207,7 @@
       <c r="AA38" s="43"/>
       <c r="AB38" s="43"/>
     </row>
-    <row r="39" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:28" ht="12.75" customHeight="1">
       <c r="B39" s="10" t="s">
         <v>182</v>
       </c>
@@ -4270,7 +4244,7 @@
       <c r="AA39" s="43"/>
       <c r="AB39" s="43"/>
     </row>
-    <row r="40" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:28" ht="12.75" customHeight="1">
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
@@ -4300,7 +4274,7 @@
       <c r="AA40" s="43"/>
       <c r="AB40" s="43"/>
     </row>
-    <row r="41" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:28" ht="12.75" customHeight="1">
       <c r="B41" s="34" t="s">
         <v>14</v>
       </c>
@@ -4332,7 +4306,7 @@
       <c r="AA41" s="43"/>
       <c r="AB41" s="43"/>
     </row>
-    <row r="42" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:28" ht="12.75" customHeight="1">
       <c r="B42" s="10" t="s">
         <v>22</v>
       </c>
@@ -4362,7 +4336,7 @@
       <c r="AA42" s="43"/>
       <c r="AB42" s="43"/>
     </row>
-    <row r="43" spans="2:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:28" ht="27.75" customHeight="1">
       <c r="B43" s="10" t="s">
         <v>169</v>
       </c>
@@ -4395,7 +4369,7 @@
       <c r="AA43" s="43"/>
       <c r="AB43" s="43"/>
     </row>
-    <row r="44" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:28" ht="12.75" customHeight="1">
       <c r="B44" s="10" t="s">
         <v>27</v>
       </c>
@@ -4436,7 +4410,7 @@
       <c r="AA44" s="43"/>
       <c r="AB44" s="43"/>
     </row>
-    <row r="45" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:28" ht="12.75" customHeight="1">
       <c r="B45" s="10" t="s">
         <v>14</v>
       </c>
@@ -4475,7 +4449,7 @@
       <c r="AA45" s="43"/>
       <c r="AB45" s="43"/>
     </row>
-    <row r="46" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:28" ht="12.75" customHeight="1">
       <c r="B46" s="10" t="s">
         <v>122</v>
       </c>
@@ -4514,7 +4488,7 @@
       <c r="AA46" s="43"/>
       <c r="AB46" s="43"/>
     </row>
-    <row r="47" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:28" ht="12.75" customHeight="1">
       <c r="B47" s="10" t="s">
         <v>125</v>
       </c>
@@ -4553,7 +4527,7 @@
       <c r="AA47" s="43"/>
       <c r="AB47" s="43"/>
     </row>
-    <row r="48" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:28" ht="12.75" customHeight="1">
       <c r="B48" s="10" t="s">
         <v>75</v>
       </c>
@@ -4584,7 +4558,7 @@
       <c r="AA48" s="43"/>
       <c r="AB48" s="43"/>
     </row>
-    <row r="49" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:28" ht="12.75" customHeight="1">
       <c r="B49" s="10" t="s">
         <v>356</v>
       </c>
@@ -4629,7 +4603,7 @@
       <c r="AA49" s="43"/>
       <c r="AB49" s="43"/>
     </row>
-    <row r="50" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:28" ht="12.75" customHeight="1">
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
@@ -4658,7 +4632,7 @@
       <c r="AA50" s="43"/>
       <c r="AB50" s="43"/>
     </row>
-    <row r="51" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:28" ht="12.75" customHeight="1">
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
@@ -4687,7 +4661,7 @@
       <c r="AA51" s="43"/>
       <c r="AB51" s="43"/>
     </row>
-    <row r="52" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:28" ht="12.75" customHeight="1">
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="10"/>
@@ -4716,7 +4690,7 @@
       <c r="AA52" s="43"/>
       <c r="AB52" s="43"/>
     </row>
-    <row r="53" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:28" ht="12.75" customHeight="1">
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="10"/>
@@ -4745,7 +4719,7 @@
       <c r="AA53" s="43"/>
       <c r="AB53" s="43"/>
     </row>
-    <row r="54" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:28" ht="12.75" customHeight="1">
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
@@ -4774,7 +4748,7 @@
       <c r="AA54" s="43"/>
       <c r="AB54" s="43"/>
     </row>
-    <row r="55" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:28" ht="12.75" customHeight="1">
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -4803,7 +4777,7 @@
       <c r="AA55" s="43"/>
       <c r="AB55" s="43"/>
     </row>
-    <row r="56" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:28" ht="12.75" customHeight="1">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -4832,7 +4806,7 @@
       <c r="AA56" s="43"/>
       <c r="AB56" s="43"/>
     </row>
-    <row r="57" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:28" ht="12.75" customHeight="1">
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -4861,7 +4835,7 @@
       <c r="AA57" s="43"/>
       <c r="AB57" s="43"/>
     </row>
-    <row r="58" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:28" ht="12.75" customHeight="1">
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -4890,7 +4864,7 @@
       <c r="AA58" s="43"/>
       <c r="AB58" s="43"/>
     </row>
-    <row r="59" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:28" ht="12.75" customHeight="1">
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -4919,7 +4893,7 @@
       <c r="AA59" s="43"/>
       <c r="AB59" s="43"/>
     </row>
-    <row r="60" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:28" ht="12.75" customHeight="1">
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -4948,7 +4922,7 @@
       <c r="AA60" s="43"/>
       <c r="AB60" s="43"/>
     </row>
-    <row r="61" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:28" ht="12.75" customHeight="1">
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -4977,7 +4951,7 @@
       <c r="AA61" s="43"/>
       <c r="AB61" s="43"/>
     </row>
-    <row r="62" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:28" ht="12.75" customHeight="1">
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -5006,7 +4980,7 @@
       <c r="AA62" s="43"/>
       <c r="AB62" s="43"/>
     </row>
-    <row r="63" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:28" ht="12.75" customHeight="1">
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -5035,7 +5009,7 @@
       <c r="AA63" s="43"/>
       <c r="AB63" s="43"/>
     </row>
-    <row r="64" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:28" ht="12.75" customHeight="1">
       <c r="B64" s="38"/>
       <c r="C64" s="38"/>
       <c r="D64" s="38"/>
@@ -5062,7 +5036,7 @@
       <c r="AA64" s="43"/>
       <c r="AB64" s="43"/>
     </row>
-    <row r="65" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:28" ht="12.75" customHeight="1">
       <c r="B65" s="38"/>
       <c r="C65" s="38"/>
       <c r="D65" s="38"/>
@@ -5089,7 +5063,7 @@
       <c r="AA65" s="43"/>
       <c r="AB65" s="43"/>
     </row>
-    <row r="66" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:28" ht="12.75" customHeight="1">
       <c r="B66" s="38"/>
       <c r="C66" s="38"/>
       <c r="D66" s="38"/>
@@ -5116,7 +5090,7 @@
       <c r="AA66" s="43"/>
       <c r="AB66" s="43"/>
     </row>
-    <row r="67" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:28" ht="12.75" customHeight="1">
       <c r="B67" s="38"/>
       <c r="C67" s="38"/>
       <c r="D67" s="38"/>
@@ -5143,7 +5117,7 @@
       <c r="AA67" s="43"/>
       <c r="AB67" s="43"/>
     </row>
-    <row r="68" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:28" ht="12.75" customHeight="1">
       <c r="B68" s="38"/>
       <c r="C68" s="38"/>
       <c r="D68" s="38"/>
@@ -5170,7 +5144,7 @@
       <c r="AA68" s="43"/>
       <c r="AB68" s="43"/>
     </row>
-    <row r="69" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:28" ht="12.75" customHeight="1">
       <c r="B69" s="38"/>
       <c r="C69" s="38"/>
       <c r="D69" s="38"/>
@@ -5197,7 +5171,7 @@
       <c r="AA69" s="43"/>
       <c r="AB69" s="43"/>
     </row>
-    <row r="70" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:28" ht="12.75" customHeight="1">
       <c r="B70" s="38"/>
       <c r="C70" s="38"/>
       <c r="D70" s="38"/>
@@ -5224,7 +5198,7 @@
       <c r="AA70" s="43"/>
       <c r="AB70" s="43"/>
     </row>
-    <row r="71" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:28" ht="12.75" customHeight="1">
       <c r="B71" s="38"/>
       <c r="C71" s="38"/>
       <c r="D71" s="38"/>
@@ -5251,7 +5225,7 @@
       <c r="AA71" s="43"/>
       <c r="AB71" s="43"/>
     </row>
-    <row r="72" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:28" ht="12.75" customHeight="1">
       <c r="B72" s="38"/>
       <c r="C72" s="38"/>
       <c r="D72" s="38"/>
@@ -5278,7 +5252,7 @@
       <c r="AA72" s="43"/>
       <c r="AB72" s="43"/>
     </row>
-    <row r="73" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:28" ht="12.75" customHeight="1">
       <c r="B73" s="38"/>
       <c r="C73" s="38"/>
       <c r="D73" s="38"/>
@@ -5305,7 +5279,7 @@
       <c r="AA73" s="43"/>
       <c r="AB73" s="43"/>
     </row>
-    <row r="74" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:28" ht="12.75" customHeight="1">
       <c r="B74" s="38"/>
       <c r="C74" s="38"/>
       <c r="D74" s="38"/>
@@ -5332,7 +5306,7 @@
       <c r="AA74" s="43"/>
       <c r="AB74" s="43"/>
     </row>
-    <row r="75" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:28" ht="12.75" customHeight="1">
       <c r="B75" s="35"/>
       <c r="C75" s="35"/>
       <c r="D75" s="35"/>
@@ -5359,7 +5333,7 @@
       <c r="AA75" s="43"/>
       <c r="AB75" s="43"/>
     </row>
-    <row r="76" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:28" ht="12.75" customHeight="1">
       <c r="B76" s="35"/>
       <c r="C76" s="35"/>
       <c r="D76" s="35"/>
@@ -5386,7 +5360,7 @@
       <c r="AA76" s="43"/>
       <c r="AB76" s="43"/>
     </row>
-    <row r="77" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:28" ht="12.75" customHeight="1">
       <c r="B77" s="35"/>
       <c r="C77" s="35"/>
       <c r="D77" s="35"/>
@@ -5413,7 +5387,7 @@
       <c r="AA77" s="43"/>
       <c r="AB77" s="43"/>
     </row>
-    <row r="78" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:28" ht="12.75" customHeight="1">
       <c r="M78" s="61"/>
       <c r="N78" s="61"/>
       <c r="O78" s="61"/>
@@ -5431,7 +5405,7 @@
       <c r="AA78" s="43"/>
       <c r="AB78" s="43"/>
     </row>
-    <row r="79" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:28" ht="12.75" customHeight="1">
       <c r="M79" s="61"/>
       <c r="N79" s="61"/>
       <c r="O79" s="61"/>
@@ -5449,7 +5423,7 @@
       <c r="AA79" s="43"/>
       <c r="AB79" s="43"/>
     </row>
-    <row r="80" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:28" ht="12.75" customHeight="1">
       <c r="M80" s="61"/>
       <c r="N80" s="61"/>
       <c r="O80" s="61"/>
@@ -5467,7 +5441,7 @@
       <c r="AA80" s="43"/>
       <c r="AB80" s="43"/>
     </row>
-    <row r="81" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="13:28" ht="12.75" customHeight="1">
       <c r="M81" s="61"/>
       <c r="N81" s="61"/>
       <c r="O81" s="61"/>
@@ -5485,7 +5459,7 @@
       <c r="AA81" s="43"/>
       <c r="AB81" s="43"/>
     </row>
-    <row r="82" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="13:28" ht="12.75" customHeight="1">
       <c r="M82" s="61"/>
       <c r="N82" s="61"/>
       <c r="O82" s="61"/>
@@ -5503,7 +5477,7 @@
       <c r="AA82" s="43"/>
       <c r="AB82" s="43"/>
     </row>
-    <row r="83" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="13:28" ht="12.75" customHeight="1">
       <c r="M83" s="61"/>
       <c r="N83" s="61"/>
       <c r="O83" s="61"/>
@@ -5521,7 +5495,7 @@
       <c r="AA83" s="43"/>
       <c r="AB83" s="43"/>
     </row>
-    <row r="84" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="13:28" ht="12.75" customHeight="1">
       <c r="M84" s="61"/>
       <c r="N84" s="61"/>
       <c r="O84" s="61"/>
@@ -5539,7 +5513,7 @@
       <c r="AA84" s="43"/>
       <c r="AB84" s="43"/>
     </row>
-    <row r="85" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="13:28" ht="12.75" customHeight="1">
       <c r="M85" s="61"/>
       <c r="N85" s="61"/>
       <c r="O85" s="61"/>
@@ -5557,7 +5531,7 @@
       <c r="AA85" s="43"/>
       <c r="AB85" s="43"/>
     </row>
-    <row r="86" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="13:28" ht="12.75" customHeight="1">
       <c r="M86" s="61"/>
       <c r="N86" s="61"/>
       <c r="O86" s="61"/>
@@ -5575,7 +5549,7 @@
       <c r="AA86" s="43"/>
       <c r="AB86" s="43"/>
     </row>
-    <row r="87" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="13:28" ht="12.75" customHeight="1">
       <c r="M87" s="61"/>
       <c r="N87" s="61"/>
       <c r="O87" s="61"/>
@@ -5653,19 +5627,19 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="88.7109375" customWidth="1"/>
+    <col min="5" max="5" width="88.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21">
       <c r="B2" s="28" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" ht="12.75" customHeight="1">
       <c r="B3" s="62" t="s">
         <v>188</v>
       </c>
@@ -5689,7 +5663,7 @@
       <c r="T3" s="62"/>
       <c r="U3" s="62"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21">
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -5711,7 +5685,7 @@
       <c r="T4" s="62"/>
       <c r="U4" s="62"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21">
       <c r="B5" s="62"/>
       <c r="C5" s="62"/>
       <c r="D5" s="62"/>
@@ -5733,7 +5707,7 @@
       <c r="T5" s="62"/>
       <c r="U5" s="62"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21">
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -5755,7 +5729,7 @@
       <c r="T6" s="62"/>
       <c r="U6" s="62"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:21">
       <c r="B7" s="62"/>
       <c r="C7" s="62"/>
       <c r="D7" s="62"/>
@@ -5777,7 +5751,7 @@
       <c r="T7" s="62"/>
       <c r="U7" s="62"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:21">
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
       <c r="D8" s="62"/>
@@ -5799,7 +5773,7 @@
       <c r="T8" s="62"/>
       <c r="U8" s="62"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21">
       <c r="B9" s="62"/>
       <c r="C9" s="62"/>
       <c r="D9" s="62"/>
@@ -5821,7 +5795,7 @@
       <c r="T9" s="62"/>
       <c r="U9" s="62"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21">
       <c r="B10" s="62"/>
       <c r="C10" s="62"/>
       <c r="D10" s="62"/>
@@ -5843,7 +5817,7 @@
       <c r="T10" s="62"/>
       <c r="U10" s="62"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:21">
       <c r="B11" s="62"/>
       <c r="C11" s="62"/>
       <c r="D11" s="62"/>
@@ -5865,7 +5839,7 @@
       <c r="T11" s="62"/>
       <c r="U11" s="62"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21">
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
       <c r="D12" s="62"/>
@@ -5887,7 +5861,7 @@
       <c r="T12" s="62"/>
       <c r="U12" s="62"/>
     </row>
-    <row r="15" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:21" ht="12.75" customHeight="1">
       <c r="B15" t="s">
         <v>189</v>
       </c>
@@ -5904,7 +5878,7 @@
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21">
       <c r="F16" s="61"/>
       <c r="G16" s="61"/>
       <c r="H16" s="61"/>
@@ -5916,7 +5890,7 @@
       <c r="N16" s="61"/>
       <c r="O16" s="61"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15">
       <c r="F17" s="61"/>
       <c r="G17" s="61"/>
       <c r="H17" s="61"/>
@@ -5928,7 +5902,7 @@
       <c r="N17" s="61"/>
       <c r="O17" s="61"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15">
       <c r="B18" s="28" t="s">
         <v>191</v>
       </c>
@@ -5952,7 +5926,7 @@
       <c r="N18" s="61"/>
       <c r="O18" s="61"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15">
       <c r="B19" t="s">
         <v>193</v>
       </c>
@@ -5976,7 +5950,7 @@
       <c r="N19" s="61"/>
       <c r="O19" s="61"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15">
       <c r="C20" t="s">
         <v>196</v>
       </c>
@@ -5997,7 +5971,7 @@
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15">
       <c r="B21" t="s">
         <v>199</v>
       </c>
@@ -6018,7 +5992,7 @@
       <c r="N21" s="61"/>
       <c r="O21" s="61"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15">
       <c r="C22" t="s">
         <v>61</v>
       </c>
@@ -6039,7 +6013,7 @@
       <c r="N22" s="61"/>
       <c r="O22" s="61"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15">
       <c r="B23" t="s">
         <v>203</v>
       </c>
@@ -6057,7 +6031,7 @@
       <c r="N23" s="61"/>
       <c r="O23" s="61"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15">
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
       <c r="H24" s="61"/>
@@ -6069,7 +6043,7 @@
       <c r="N24" s="61"/>
       <c r="O24" s="61"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15">
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
       <c r="H25" s="61"/>
@@ -6081,7 +6055,7 @@
       <c r="N25" s="61"/>
       <c r="O25" s="61"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15">
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
       <c r="H26" s="61"/>
@@ -6093,7 +6067,7 @@
       <c r="N26" s="61"/>
       <c r="O26" s="61"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15">
       <c r="F27" s="61"/>
       <c r="G27" s="61"/>
       <c r="H27" s="61"/>
@@ -6105,7 +6079,7 @@
       <c r="N27" s="61"/>
       <c r="O27" s="61"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15">
       <c r="F28" s="61"/>
       <c r="G28" s="61"/>
       <c r="H28" s="61"/>
@@ -6117,7 +6091,7 @@
       <c r="N28" s="61"/>
       <c r="O28" s="61"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15">
       <c r="F29" s="61"/>
       <c r="G29" s="61"/>
       <c r="H29" s="61"/>
@@ -6129,7 +6103,7 @@
       <c r="N29" s="61"/>
       <c r="O29" s="61"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15">
       <c r="F30" s="61"/>
       <c r="G30" s="61"/>
       <c r="H30" s="61"/>
@@ -6141,7 +6115,7 @@
       <c r="N30" s="61"/>
       <c r="O30" s="61"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15">
       <c r="F31" s="61"/>
       <c r="G31" s="61"/>
       <c r="H31" s="61"/>
@@ -6153,7 +6127,7 @@
       <c r="N31" s="61"/>
       <c r="O31" s="61"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15">
       <c r="F32" s="61"/>
       <c r="G32" s="61"/>
       <c r="H32" s="61"/>
@@ -6165,7 +6139,7 @@
       <c r="N32" s="61"/>
       <c r="O32" s="61"/>
     </row>
-    <row r="33" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:15">
       <c r="F33" s="61"/>
       <c r="G33" s="61"/>
       <c r="H33" s="61"/>
@@ -6177,7 +6151,7 @@
       <c r="N33" s="61"/>
       <c r="O33" s="61"/>
     </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:15">
       <c r="F34" s="61"/>
       <c r="G34" s="61"/>
       <c r="H34" s="61"/>
@@ -6189,7 +6163,7 @@
       <c r="N34" s="61"/>
       <c r="O34" s="61"/>
     </row>
-    <row r="35" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:15">
       <c r="F35" s="61"/>
       <c r="G35" s="61"/>
       <c r="H35" s="61"/>
@@ -6201,7 +6175,7 @@
       <c r="N35" s="61"/>
       <c r="O35" s="61"/>
     </row>
-    <row r="36" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:15">
       <c r="F36" s="61"/>
       <c r="G36" s="61"/>
       <c r="H36" s="61"/>
@@ -6213,7 +6187,7 @@
       <c r="N36" s="61"/>
       <c r="O36" s="61"/>
     </row>
-    <row r="37" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:15">
       <c r="F37" s="61"/>
       <c r="G37" s="61"/>
       <c r="H37" s="61"/>
@@ -6225,7 +6199,7 @@
       <c r="N37" s="61"/>
       <c r="O37" s="61"/>
     </row>
-    <row r="38" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:15">
       <c r="F38" s="61"/>
       <c r="G38" s="61"/>
       <c r="H38" s="61"/>
@@ -6237,7 +6211,7 @@
       <c r="N38" s="61"/>
       <c r="O38" s="61"/>
     </row>
-    <row r="39" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:15">
       <c r="F39" s="61"/>
       <c r="G39" s="61"/>
       <c r="H39" s="61"/>
@@ -6249,7 +6223,7 @@
       <c r="N39" s="61"/>
       <c r="O39" s="61"/>
     </row>
-    <row r="40" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:15">
       <c r="F40" s="61"/>
       <c r="G40" s="61"/>
       <c r="H40" s="61"/>
@@ -6261,7 +6235,7 @@
       <c r="N40" s="61"/>
       <c r="O40" s="61"/>
     </row>
-    <row r="41" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:15">
       <c r="F41" s="61"/>
       <c r="G41" s="61"/>
       <c r="H41" s="61"/>
@@ -6273,7 +6247,7 @@
       <c r="N41" s="61"/>
       <c r="O41" s="61"/>
     </row>
-    <row r="42" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:15">
       <c r="F42" s="61"/>
       <c r="G42" s="61"/>
       <c r="H42" s="61"/>
@@ -6285,7 +6259,7 @@
       <c r="N42" s="61"/>
       <c r="O42" s="61"/>
     </row>
-    <row r="43" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:15">
       <c r="F43" s="61"/>
       <c r="G43" s="61"/>
       <c r="H43" s="61"/>
@@ -6297,7 +6271,7 @@
       <c r="N43" s="61"/>
       <c r="O43" s="61"/>
     </row>
-    <row r="44" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:15">
       <c r="F44" s="61"/>
       <c r="G44" s="61"/>
       <c r="H44" s="61"/>
@@ -6309,7 +6283,7 @@
       <c r="N44" s="61"/>
       <c r="O44" s="61"/>
     </row>
-    <row r="45" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:15">
       <c r="F45" s="61"/>
       <c r="G45" s="61"/>
       <c r="H45" s="61"/>
@@ -6321,7 +6295,7 @@
       <c r="N45" s="61"/>
       <c r="O45" s="61"/>
     </row>
-    <row r="46" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:15">
       <c r="F46" s="61"/>
       <c r="G46" s="61"/>
       <c r="H46" s="61"/>
@@ -6333,7 +6307,7 @@
       <c r="N46" s="61"/>
       <c r="O46" s="61"/>
     </row>
-    <row r="47" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:15">
       <c r="F47" s="61"/>
       <c r="G47" s="61"/>
       <c r="H47" s="61"/>
@@ -6345,7 +6319,7 @@
       <c r="N47" s="61"/>
       <c r="O47" s="61"/>
     </row>
-    <row r="48" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="6:15">
       <c r="F48" s="61"/>
       <c r="G48" s="61"/>
       <c r="H48" s="61"/>
@@ -6357,7 +6331,7 @@
       <c r="N48" s="61"/>
       <c r="O48" s="61"/>
     </row>
-    <row r="49" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:15">
       <c r="F49" s="61"/>
       <c r="G49" s="61"/>
       <c r="H49" s="61"/>
@@ -6369,7 +6343,7 @@
       <c r="N49" s="61"/>
       <c r="O49" s="61"/>
     </row>
-    <row r="50" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:15">
       <c r="F50" s="61"/>
       <c r="G50" s="61"/>
       <c r="H50" s="61"/>
@@ -6381,7 +6355,7 @@
       <c r="N50" s="61"/>
       <c r="O50" s="61"/>
     </row>
-    <row r="51" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:15">
       <c r="F51" s="61"/>
       <c r="G51" s="61"/>
       <c r="H51" s="61"/>
@@ -6393,7 +6367,7 @@
       <c r="N51" s="61"/>
       <c r="O51" s="61"/>
     </row>
-    <row r="52" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:15">
       <c r="F52" s="61"/>
       <c r="G52" s="61"/>
       <c r="H52" s="61"/>
@@ -6423,21 +6397,21 @@
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="33.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -6472,7 +6446,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="46" t="s">
         <v>205</v>
       </c>
@@ -6487,7 +6461,7 @@
       <c r="J2" s="40"/>
       <c r="K2" s="40"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="46">
         <v>1</v>
       </c>
@@ -6514,7 +6488,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="46">
         <v>2</v>
       </c>
@@ -6541,7 +6515,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="46">
         <v>3</v>
       </c>
@@ -6562,7 +6536,7 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="46">
         <v>4</v>
       </c>
@@ -6583,7 +6557,7 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="46">
         <v>5</v>
       </c>
@@ -6604,7 +6578,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="C8" s="34" t="s">
         <v>73</v>
       </c>
@@ -6615,7 +6589,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="C9" s="34" t="s">
         <v>78</v>
       </c>
@@ -6623,7 +6597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="C10" s="10" t="s">
         <v>84</v>
       </c>
@@ -6631,7 +6605,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="C11" s="10" t="s">
         <v>89</v>
       </c>
@@ -6639,7 +6613,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="C12" s="10" t="s">
         <v>93</v>
       </c>
@@ -6647,7 +6621,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="C13" s="10" t="s">
         <v>97</v>
       </c>
@@ -6655,7 +6629,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="C14" s="10" t="s">
         <v>97</v>
       </c>
@@ -6663,7 +6637,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="C15" s="10" t="s">
         <v>101</v>
       </c>
@@ -6671,7 +6645,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="C16" s="10" t="s">
         <v>105</v>
       </c>
@@ -6679,7 +6653,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5">
       <c r="C17" s="10" t="s">
         <v>108</v>
       </c>
@@ -6687,7 +6661,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5">
       <c r="C18" s="10" t="s">
         <v>112</v>
       </c>
@@ -6695,7 +6669,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:5">
       <c r="C19" s="10" t="s">
         <v>61</v>
       </c>
@@ -6703,7 +6677,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5">
       <c r="C20" s="10" t="s">
         <v>121</v>
       </c>
@@ -6711,7 +6685,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:5">
       <c r="C21" s="10" t="s">
         <v>124</v>
       </c>
@@ -6719,7 +6693,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:5">
       <c r="C22" s="10" t="s">
         <v>127</v>
       </c>
@@ -6727,7 +6701,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:5">
       <c r="C23" s="10" t="s">
         <v>131</v>
       </c>
@@ -6735,7 +6709,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:5">
       <c r="C24" s="10" t="s">
         <v>134</v>
       </c>
@@ -6743,7 +6717,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:5">
       <c r="C25" s="10" t="s">
         <v>139</v>
       </c>
@@ -6751,7 +6725,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:5">
       <c r="C26" s="10" t="s">
         <v>143</v>
       </c>
@@ -6759,7 +6733,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:5">
       <c r="C27" s="10" t="s">
         <v>149</v>
       </c>
@@ -6767,7 +6741,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:5">
       <c r="C28" s="10" t="s">
         <v>152</v>
       </c>
@@ -6775,7 +6749,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:5">
       <c r="C29" s="10" t="s">
         <v>156</v>
       </c>
@@ -6783,7 +6757,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:5">
       <c r="C30" s="10" t="s">
         <v>158</v>
       </c>
@@ -6791,7 +6765,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:5">
       <c r="C31" s="10" t="s">
         <v>159</v>
       </c>
@@ -6799,7 +6773,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:5">
       <c r="C32" s="10" t="s">
         <v>235</v>
       </c>
@@ -6807,7 +6781,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:5">
       <c r="C33" s="10" t="s">
         <v>166</v>
       </c>
@@ -6815,7 +6789,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:5">
       <c r="C34" s="10" t="s">
         <v>167</v>
       </c>
@@ -6823,7 +6797,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:5">
       <c r="C35" s="10" t="s">
         <v>168</v>
       </c>
@@ -6831,7 +6805,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:5">
       <c r="C36" s="10" t="s">
         <v>173</v>
       </c>
@@ -6839,7 +6813,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:5">
       <c r="C37" s="10" t="s">
         <v>177</v>
       </c>
@@ -6847,7 +6821,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:5">
       <c r="C38" s="10" t="s">
         <v>181</v>
       </c>
@@ -6855,7 +6829,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:5">
       <c r="C39" s="10" t="s">
         <v>184</v>
       </c>
@@ -6863,557 +6837,557 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:5">
       <c r="E40" s="10" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:5">
       <c r="E41" s="10" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:5">
       <c r="E42" s="10" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:5">
       <c r="E43" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:5">
       <c r="E44" s="10" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:5">
       <c r="E45" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:5">
       <c r="E46" s="10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:5">
       <c r="E47" s="10" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:5">
       <c r="E48" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5">
       <c r="E49" s="10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:5">
       <c r="E50" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:5">
       <c r="E51" s="10" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:5">
       <c r="E52" s="10" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:5">
       <c r="E53" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:5">
       <c r="E54" s="10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:5">
       <c r="E55" s="10" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:5">
       <c r="E56" s="10" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:5">
       <c r="E57" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:5">
       <c r="E58" s="10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:5">
       <c r="E59" s="10" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:5">
       <c r="E60" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:5">
       <c r="E61" s="10" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:5">
       <c r="E62" s="10" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:5">
       <c r="E63" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:5">
       <c r="E64" s="10" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:5">
       <c r="E65" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:5">
       <c r="E66" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:5">
       <c r="E67" s="10" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:5">
       <c r="E68" s="10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:5">
       <c r="E69" s="10" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:5">
       <c r="E70" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:5">
       <c r="E71" s="10" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:5">
       <c r="E72" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:5">
       <c r="E73" s="10" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:5">
       <c r="E74" s="10" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:5">
       <c r="E75" s="10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="5:5">
       <c r="E76" s="10" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="5:5">
       <c r="E77" s="10" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="5:5">
       <c r="E78" s="10" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="5:5">
       <c r="E79" s="10" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:5">
       <c r="E80" s="10" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="5:5">
       <c r="E81" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="5:5">
       <c r="E82" s="10" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="5:5">
       <c r="E83" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="5:5">
       <c r="E84" s="10" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="5:5">
       <c r="E85" s="10" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="5:5">
       <c r="E86" s="10" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="5:5">
       <c r="E87" s="10" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="5:5">
       <c r="E88" s="10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="5:5">
       <c r="E89" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="5:5">
       <c r="E90" s="10" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="5:5">
       <c r="E91" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="5:5">
       <c r="E92" s="10" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="5:5">
       <c r="E93" s="10" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="5:5">
       <c r="E94" s="10" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="5:5">
       <c r="E95" s="10" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="5:5">
       <c r="E96" s="10" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:5">
       <c r="E97" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:5">
       <c r="E98" s="10" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:5">
       <c r="E99" s="10" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:5">
       <c r="E100" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:5">
       <c r="E101" s="10" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:5">
       <c r="E102" s="10" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:5">
       <c r="E103" s="10" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:5">
       <c r="E104" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:5">
       <c r="E105" s="10" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:5">
       <c r="E106" s="10" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:5">
       <c r="E107" s="10" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:5">
       <c r="E108" s="10" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:5">
       <c r="E109" s="10" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="5:5">
       <c r="E110" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="5:5">
       <c r="E111" s="10" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="5:5">
       <c r="E112" s="10" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:5">
       <c r="E113" s="10" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:5">
       <c r="E114" s="10" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:5">
       <c r="E115" s="10" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:5">
       <c r="E116" s="10" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:5">
       <c r="E117" s="10" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="5:5">
       <c r="E118" s="10" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="5:5">
       <c r="E119" s="10" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="5:5">
       <c r="E120" s="10" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="5:5">
       <c r="E121" s="10" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="5:5">
       <c r="E122" s="10" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="5:5">
       <c r="E123" s="10" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="5:5">
       <c r="E124" s="10" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="5:5">
       <c r="E125" s="10" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="5:5">
       <c r="E126" s="10" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="5:5">
       <c r="E127" s="10" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="5:5">
       <c r="E128" s="10" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="5:5">
       <c r="E129" s="10" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="5:5">
       <c r="E130" s="10" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="5:5">
       <c r="E131" s="10" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="5:5">
       <c r="E132" s="10" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="5:5">
       <c r="E133" s="10" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="5:5">
       <c r="E134" s="10" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="5:5">
       <c r="E135" s="10" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="5:5">
       <c r="E136" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="5:5">
       <c r="E137" s="10" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="5:5">
       <c r="E138" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="5:5">
       <c r="E139" s="10" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="5:5">
       <c r="E140" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="5:5">
       <c r="E141" s="10" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="5:5">
       <c r="E142" s="10" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="5:5">
       <c r="E143" s="10" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="5:5">
       <c r="E144" s="10" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="5:5">
       <c r="E145" s="10" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="5:5">
       <c r="E146" s="10" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="5:5">
       <c r="E147" s="10" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="5:5">
       <c r="E148" s="10" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="5:5">
       <c r="E149" s="10" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="5:5">
       <c r="E150" s="10" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Fixed some little bugs in NetLiquidity script.
</commit_message>
<xml_diff>
--- a/Generic_Macro/Control.xlsx
+++ b/Generic_Macro/Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/TempVenv/Plebs_Macro/Generic_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC430E67-7267-7D43-A5F5-2090231A2F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82E6059-3522-9A42-A22D-A1B25FB7285F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2100,7 +2100,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
Added gitignore to not track downloaded datafiles and such. Also working on BEA data downloader tool, that is cool....
</commit_message>
<xml_diff>
--- a/Generic_Macro/Control.xlsx
+++ b/Generic_Macro/Control.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/TempVenv/Plebs_Macro/Generic_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82E6059-3522-9A42-A22D-A1B25FB7285F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D7EA93-CB7D-3144-A439-D476A8B02349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="367">
   <si>
     <t>Index</t>
   </si>
@@ -1289,16 +1289,25 @@
     <t>Mining difficulty (x 10$^{20}$)</t>
   </si>
   <si>
-    <t xml:space="preserve">Gold </t>
-  </si>
-  <si>
-    <t>1970-01-01</t>
-  </si>
-  <si>
-    <t>Soft &amp; Hard money</t>
-  </si>
-  <si>
-    <t>Bil. of US $</t>
+    <t>ODSACBW027SBOG</t>
+  </si>
+  <si>
+    <t>Other Deposits, All Commercial Banks</t>
+  </si>
+  <si>
+    <t>TOTBKCRNSA</t>
+  </si>
+  <si>
+    <t>Bank credit, all commercial banks</t>
+  </si>
+  <si>
+    <t>2010-01-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Bitty: dawg…</t>
   </si>
 </sst>
 </file>
@@ -2099,8 +2108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -2170,10 +2179,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>145</v>
@@ -2188,10 +2197,10 @@
         <v>19</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -2200,39 +2209,20 @@
       <c r="N2" s="9">
         <v>2</v>
       </c>
-      <c r="O2" s="10">
-        <f>10^12</f>
-        <v>1000000000000</v>
-      </c>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="1:15" ht="18">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="7"/>
@@ -2244,30 +2234,14 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>172</v>
-      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="7"/>
@@ -2279,38 +2253,20 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>363</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
-      <c r="O5" s="10">
-        <v>1000</v>
-      </c>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:15" ht="18">
       <c r="A6" s="4">
@@ -2351,7 +2307,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="C8" s="56" t="s">
         <v>32</v>
@@ -2421,7 +2377,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
@@ -2645,13 +2601,16 @@
     <row r="32" spans="1:12">
       <c r="A32" s="15"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:9">
       <c r="A33" s="15"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:9">
       <c r="A34" s="15"/>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="I34" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="15"/>
     </row>
   </sheetData>
@@ -2731,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB87"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I34" sqref="B34:I34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -4604,13 +4563,19 @@
       <c r="AB49" s="43"/>
     </row>
     <row r="50" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
+      <c r="B50" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
       <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
+      <c r="H50" s="10" t="s">
+        <v>361</v>
+      </c>
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
       <c r="K50" s="15"/>
@@ -4633,13 +4598,19 @@
       <c r="AB50" s="43"/>
     </row>
     <row r="51" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
+      <c r="B51" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
       <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
+      <c r="H51" s="10" t="s">
+        <v>363</v>
+      </c>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
       <c r="K51" s="15"/>
@@ -5624,7 +5595,7 @@
   <dimension ref="B2:U52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F15" sqref="F15:O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
Got rid of a whole bunch of files that should not be tracked...
</commit_message>
<xml_diff>
--- a/Generic_Macro/Control.xlsx
+++ b/Generic_Macro/Control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/TempVenv/Plebs_Macro/Generic_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D7EA93-CB7D-3144-A439-D476A8B02349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D88711-32D9-F249-95BE-BC11EE523D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Notes" sheetId="3" r:id="rId3"/>
     <sheet name="DropDownValues" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="373">
   <si>
     <t>Index</t>
   </si>
@@ -1301,13 +1301,31 @@
     <t>Bank credit, all commercial banks</t>
   </si>
   <si>
-    <t>2010-01-01</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Bitty: dawg…</t>
+  </si>
+  <si>
+    <t>Gov_CurrentReceipts_Q</t>
+  </si>
+  <si>
+    <t>Gov_TotalExpenditures_Q</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>expense</t>
+  </si>
+  <si>
+    <t>US Gov total current income receipts</t>
+  </si>
+  <si>
+    <t>US Gov total expenditures</t>
+  </si>
+  <si>
+    <t>1950-01-01</t>
   </si>
 </sst>
 </file>
@@ -2109,7 +2127,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -2179,25 +2197,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>106</v>
+        <v>366</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>145</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>18</v>
+        <v>368</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>54</v>
+        <v>370</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>30</v>
@@ -2215,19 +2233,37 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
+      <c r="N3" s="9">
+        <v>2</v>
+      </c>
       <c r="O3" s="10"/>
     </row>
     <row r="4" spans="1:15" ht="18">
@@ -2307,7 +2343,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="C8" s="56" t="s">
         <v>32</v>
@@ -2377,7 +2413,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
@@ -2607,7 +2643,7 @@
     <row r="34" spans="1:9">
       <c r="A34" s="15"/>
       <c r="I34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="35" spans="1:9">

</xml_diff>

<commit_message>
Fixed a couple little buigs..
</commit_message>
<xml_diff>
--- a/Generic_Macro/Control.xlsx
+++ b/Generic_Macro/Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/TempVenv/Plebs_Macro/Generic_Macro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimmi\OneDrive\Documents\Documents\Scripts\VenV\Plebs_Macro\Generic_Macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D88711-32D9-F249-95BE-BC11EE523D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB8111D-017F-404D-9ED8-BA0173E02F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_Input" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="373">
   <si>
     <t>Index</t>
   </si>
@@ -1304,35 +1304,35 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Bitty: dawg…</t>
-  </si>
-  <si>
-    <t>Gov_CurrentReceipts_Q</t>
-  </si>
-  <si>
-    <t>Gov_TotalExpenditures_Q</t>
-  </si>
-  <si>
-    <t>income</t>
-  </si>
-  <si>
-    <t>expense</t>
-  </si>
-  <si>
-    <t>US Gov total current income receipts</t>
-  </si>
-  <si>
-    <t>US Gov total expenditures</t>
-  </si>
-  <si>
-    <t>1950-01-01</t>
+    <t>odl</t>
+  </si>
+  <si>
+    <t>2010-01-01</t>
+  </si>
+  <si>
+    <t>M2 money supply (U.S)</t>
+  </si>
+  <si>
+    <t>Trillions of U.S $</t>
+  </si>
+  <si>
+    <t>btc</t>
+  </si>
+  <si>
+    <t>Top50GM2</t>
+  </si>
+  <si>
+    <t>Global M2 (top 50)</t>
+  </si>
+  <si>
+    <t>Monetary Aggregates, Bitcoin &amp; Equities.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2127,25 +2127,25 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
     <col min="8" max="9" width="44" customWidth="1"/>
-    <col min="12" max="12" width="18.5" customWidth="1"/>
-    <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" customWidth="1"/>
-    <col min="15" max="15" width="18.5" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18">
+    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2192,58 +2192,56 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18">
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>30</v>
+        <v>368</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
-      <c r="N2" s="9">
-        <v>2</v>
-      </c>
+      <c r="N2" s="9"/>
       <c r="O2" s="10"/>
     </row>
-    <row r="3" spans="1:15" ht="18">
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>367</v>
+        <v>106</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>369</v>
@@ -2252,32 +2250,46 @@
         <v>19</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="O3" s="10"/>
     </row>
-    <row r="4" spans="1:15" ht="18">
+    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="7"/>
@@ -2285,26 +2297,42 @@
       <c r="N4" s="9"/>
       <c r="O4" s="10"/>
     </row>
-    <row r="5" spans="1:15" ht="18">
+    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>371</v>
+      </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
+      <c r="N5" s="9">
+        <v>2.5</v>
+      </c>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:15" ht="18">
+    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2323,7 +2351,7 @@
       <c r="N6" s="9"/>
       <c r="O6" s="10"/>
     </row>
-    <row r="7" spans="1:15" ht="16">
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2338,12 +2366,12 @@
       <c r="L7" s="14"/>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:15" ht="16">
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C8" s="56" t="s">
         <v>32</v>
@@ -2358,7 +2386,7 @@
       <c r="K8" s="18"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:15" ht="16">
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>33</v>
       </c>
@@ -2376,7 +2404,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:15" ht="16">
+    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -2390,7 +2418,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:15" ht="16">
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>35</v>
       </c>
@@ -2408,12 +2436,12 @@
       <c r="K11" s="18"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:15" ht="16">
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
@@ -2426,7 +2454,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="1:15" ht="16">
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>38</v>
       </c>
@@ -2444,7 +2472,7 @@
       <c r="K13" s="18"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="1:15" ht="16">
+    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -2456,7 +2484,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="1:15" ht="16">
+    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>353</v>
       </c>
@@ -2474,7 +2502,7 @@
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="1:15" ht="16">
+    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="51" t="s">
         <v>355</v>
       </c>
@@ -2490,7 +2518,7 @@
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="1:12" ht="16">
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="51" t="s">
         <v>354</v>
       </c>
@@ -2506,7 +2534,7 @@
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
     </row>
-    <row r="18" spans="1:12" ht="16">
+    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="23"/>
       <c r="C18" s="18"/>
@@ -2520,7 +2548,7 @@
       <c r="K18" s="18"/>
       <c r="L18" s="19"/>
     </row>
-    <row r="19" spans="1:12" ht="16">
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -2534,7 +2562,7 @@
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -2545,7 +2573,7 @@
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -2558,7 +2586,7 @@
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="24"/>
       <c r="B22" s="25"/>
       <c r="C22" s="26"/>
@@ -2569,7 +2597,7 @@
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
@@ -2580,7 +2608,7 @@
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="24"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
@@ -2591,7 +2619,7 @@
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
     </row>
-    <row r="25" spans="1:12" ht="14">
+    <row r="25" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="24"/>
       <c r="B25" s="53"/>
       <c r="C25" s="54"/>
@@ -2605,7 +2633,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="24"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="24"/>
       <c r="B26" s="25"/>
       <c r="C26" s="25"/>
@@ -2618,35 +2646,35 @@
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
     </row>
-    <row r="27" spans="1:12" ht="16">
+    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
       <c r="E27" s="23"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="15"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="15"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="15"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="15"/>
       <c r="I34" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
     </row>
   </sheetData>
@@ -2726,26 +2754,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB87"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="46.6640625" customWidth="1"/>
-    <col min="9" max="9" width="35.33203125" customWidth="1"/>
-    <col min="10" max="12" width="12.33203125" customWidth="1"/>
-    <col min="13" max="13" width="25.5" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="46.7109375" customWidth="1"/>
+    <col min="9" max="9" width="35.28515625" customWidth="1"/>
+    <col min="10" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="25.42578125" customWidth="1"/>
     <col min="14" max="14" width="119" customWidth="1"/>
-    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D1" s="27" t="s">
         <v>39</v>
       </c>
@@ -2766,7 +2794,7 @@
       <c r="R1" s="31"/>
       <c r="S1" s="31"/>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
@@ -2808,7 +2836,7 @@
       <c r="R2" s="36"/>
       <c r="S2" s="37"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3" s="34" t="s">
         <v>14</v>
       </c>
@@ -2844,7 +2872,7 @@
       <c r="R3" s="35"/>
       <c r="S3" s="35"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B4" s="34" t="s">
         <v>46</v>
       </c>
@@ -2880,7 +2908,7 @@
       <c r="R4" s="35"/>
       <c r="S4" s="35"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>51</v>
       </c>
@@ -2916,7 +2944,7 @@
       <c r="R5" s="35"/>
       <c r="S5" s="35"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="34" t="s">
         <v>57</v>
       </c>
@@ -2952,7 +2980,7 @@
       <c r="R6" s="35"/>
       <c r="S6" s="35"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B7" s="34" t="s">
         <v>63</v>
       </c>
@@ -2988,7 +3016,7 @@
       <c r="R7" s="35"/>
       <c r="S7" s="35"/>
     </row>
-    <row r="8" spans="1:19" ht="14">
+    <row r="8" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B8" s="39" t="s">
         <v>69</v>
       </c>
@@ -3019,7 +3047,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9" s="34" t="s">
         <v>75</v>
       </c>
@@ -3050,7 +3078,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
         <v>80</v>
       </c>
@@ -3084,7 +3112,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
         <v>86</v>
       </c>
@@ -3114,7 +3142,7 @@
       </c>
       <c r="N11" s="35"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>51</v>
       </c>
@@ -3146,7 +3174,7 @@
       </c>
       <c r="N12" s="35"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
         <v>94</v>
       </c>
@@ -3178,7 +3206,7 @@
       </c>
       <c r="N13" s="35"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
         <v>98</v>
       </c>
@@ -3207,7 +3235,7 @@
       </c>
       <c r="N14" s="35"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
@@ -3231,7 +3259,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B16" s="34" t="s">
         <v>51</v>
       </c>
@@ -3265,7 +3293,7 @@
       </c>
       <c r="N16" s="35"/>
     </row>
-    <row r="17" spans="2:28">
+    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B17" s="34" t="s">
         <v>106</v>
       </c>
@@ -3300,7 +3328,7 @@
       </c>
       <c r="N17" s="35"/>
     </row>
-    <row r="18" spans="2:28">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B18" s="34" t="s">
         <v>109</v>
       </c>
@@ -3334,7 +3362,7 @@
       </c>
       <c r="N18" s="35"/>
     </row>
-    <row r="19" spans="2:28">
+    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B19" s="34" t="s">
         <v>113</v>
       </c>
@@ -3368,7 +3396,7 @@
       </c>
       <c r="N19" s="35"/>
     </row>
-    <row r="20" spans="2:28" ht="12.75" customHeight="1">
+    <row r="20" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="34" t="s">
         <v>117</v>
       </c>
@@ -3414,7 +3442,7 @@
       <c r="AA20" s="43"/>
       <c r="AB20" s="43"/>
     </row>
-    <row r="21" spans="2:28" ht="12.75" customHeight="1">
+    <row r="21" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="34" t="s">
         <v>122</v>
       </c>
@@ -3450,7 +3478,7 @@
       <c r="AA21" s="43"/>
       <c r="AB21" s="43"/>
     </row>
-    <row r="22" spans="2:28" ht="12.75" customHeight="1">
+    <row r="22" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
         <v>125</v>
       </c>
@@ -3486,7 +3514,7 @@
       <c r="AA22" s="43"/>
       <c r="AB22" s="43"/>
     </row>
-    <row r="23" spans="2:28" ht="12.75" customHeight="1">
+    <row r="23" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="34" t="s">
         <v>128</v>
       </c>
@@ -3532,7 +3560,7 @@
       <c r="AA23" s="43"/>
       <c r="AB23" s="43"/>
     </row>
-    <row r="24" spans="2:28" ht="12.75" customHeight="1">
+    <row r="24" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
         <v>132</v>
       </c>
@@ -3568,7 +3596,7 @@
       <c r="AA24" s="43"/>
       <c r="AB24" s="43"/>
     </row>
-    <row r="25" spans="2:28" ht="12.75" customHeight="1">
+    <row r="25" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="34" t="s">
         <v>135</v>
       </c>
@@ -3615,7 +3643,7 @@
       <c r="AA25" s="43"/>
       <c r="AB25" s="43"/>
     </row>
-    <row r="26" spans="2:28" ht="12.75" customHeight="1">
+    <row r="26" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="34" t="s">
         <v>140</v>
       </c>
@@ -3662,7 +3690,7 @@
       <c r="AA26" s="43"/>
       <c r="AB26" s="43"/>
     </row>
-    <row r="27" spans="2:28" ht="12.75" customHeight="1">
+    <row r="27" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="17" t="s">
         <v>144</v>
       </c>
@@ -3707,7 +3735,7 @@
       <c r="AA27" s="43"/>
       <c r="AB27" s="43"/>
     </row>
-    <row r="28" spans="2:28" ht="12.75" customHeight="1">
+    <row r="28" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
         <v>135</v>
       </c>
@@ -3754,7 +3782,7 @@
       <c r="AA28" s="43"/>
       <c r="AB28" s="43"/>
     </row>
-    <row r="29" spans="2:28" ht="12.75" customHeight="1">
+    <row r="29" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
         <v>153</v>
       </c>
@@ -3797,7 +3825,7 @@
       <c r="AA29" s="43"/>
       <c r="AB29" s="43"/>
     </row>
-    <row r="30" spans="2:28" ht="12.75" customHeight="1">
+    <row r="30" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="10" t="s">
         <v>157</v>
       </c>
@@ -3844,7 +3872,7 @@
       <c r="AA30" s="43"/>
       <c r="AB30" s="43"/>
     </row>
-    <row r="31" spans="2:28" ht="12.75" customHeight="1">
+    <row r="31" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="34" t="s">
         <v>106</v>
       </c>
@@ -3889,7 +3917,7 @@
       <c r="AA31" s="43"/>
       <c r="AB31" s="43"/>
     </row>
-    <row r="32" spans="2:28" ht="12.75" customHeight="1">
+    <row r="32" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="34" t="s">
         <v>160</v>
       </c>
@@ -3922,7 +3950,7 @@
       <c r="AA32" s="43"/>
       <c r="AB32" s="43"/>
     </row>
-    <row r="33" spans="2:28" ht="12.75" customHeight="1">
+    <row r="33" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="34" t="s">
         <v>162</v>
       </c>
@@ -3969,7 +3997,7 @@
       <c r="AA33" s="43"/>
       <c r="AB33" s="43"/>
     </row>
-    <row r="34" spans="2:28" ht="12.75" customHeight="1">
+    <row r="34" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="34" t="s">
         <v>14</v>
       </c>
@@ -4016,7 +4044,7 @@
       <c r="AA34" s="43"/>
       <c r="AB34" s="43"/>
     </row>
-    <row r="35" spans="2:28" ht="12.75" customHeight="1">
+    <row r="35" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="34" t="s">
         <v>22</v>
       </c>
@@ -4061,7 +4089,7 @@
       <c r="AA35" s="43"/>
       <c r="AB35" s="43"/>
     </row>
-    <row r="36" spans="2:28" ht="12.75" customHeight="1">
+    <row r="36" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="34" t="s">
         <v>169</v>
       </c>
@@ -4108,7 +4136,7 @@
       <c r="AA36" s="43"/>
       <c r="AB36" s="43"/>
     </row>
-    <row r="37" spans="2:28" ht="12.75" customHeight="1">
+    <row r="37" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
         <v>153</v>
       </c>
@@ -4155,7 +4183,7 @@
       <c r="AA37" s="43"/>
       <c r="AB37" s="43"/>
     </row>
-    <row r="38" spans="2:28" ht="12.75" customHeight="1">
+    <row r="38" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="34" t="s">
         <v>178</v>
       </c>
@@ -4202,7 +4230,7 @@
       <c r="AA38" s="43"/>
       <c r="AB38" s="43"/>
     </row>
-    <row r="39" spans="2:28" ht="12.75" customHeight="1">
+    <row r="39" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="10" t="s">
         <v>182</v>
       </c>
@@ -4239,7 +4267,7 @@
       <c r="AA39" s="43"/>
       <c r="AB39" s="43"/>
     </row>
-    <row r="40" spans="2:28" ht="12.75" customHeight="1">
+    <row r="40" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
@@ -4269,7 +4297,7 @@
       <c r="AA40" s="43"/>
       <c r="AB40" s="43"/>
     </row>
-    <row r="41" spans="2:28" ht="12.75" customHeight="1">
+    <row r="41" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="34" t="s">
         <v>14</v>
       </c>
@@ -4301,7 +4329,7 @@
       <c r="AA41" s="43"/>
       <c r="AB41" s="43"/>
     </row>
-    <row r="42" spans="2:28" ht="12.75" customHeight="1">
+    <row r="42" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="10" t="s">
         <v>22</v>
       </c>
@@ -4331,7 +4359,7 @@
       <c r="AA42" s="43"/>
       <c r="AB42" s="43"/>
     </row>
-    <row r="43" spans="2:28" ht="27.75" customHeight="1">
+    <row r="43" spans="2:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="10" t="s">
         <v>169</v>
       </c>
@@ -4364,7 +4392,7 @@
       <c r="AA43" s="43"/>
       <c r="AB43" s="43"/>
     </row>
-    <row r="44" spans="2:28" ht="12.75" customHeight="1">
+    <row r="44" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="10" t="s">
         <v>27</v>
       </c>
@@ -4405,7 +4433,7 @@
       <c r="AA44" s="43"/>
       <c r="AB44" s="43"/>
     </row>
-    <row r="45" spans="2:28" ht="12.75" customHeight="1">
+    <row r="45" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="10" t="s">
         <v>14</v>
       </c>
@@ -4444,7 +4472,7 @@
       <c r="AA45" s="43"/>
       <c r="AB45" s="43"/>
     </row>
-    <row r="46" spans="2:28" ht="12.75" customHeight="1">
+    <row r="46" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="10" t="s">
         <v>122</v>
       </c>
@@ -4483,7 +4511,7 @@
       <c r="AA46" s="43"/>
       <c r="AB46" s="43"/>
     </row>
-    <row r="47" spans="2:28" ht="12.75" customHeight="1">
+    <row r="47" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="10" t="s">
         <v>125</v>
       </c>
@@ -4522,7 +4550,7 @@
       <c r="AA47" s="43"/>
       <c r="AB47" s="43"/>
     </row>
-    <row r="48" spans="2:28" ht="12.75" customHeight="1">
+    <row r="48" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="10" t="s">
         <v>75</v>
       </c>
@@ -4553,7 +4581,7 @@
       <c r="AA48" s="43"/>
       <c r="AB48" s="43"/>
     </row>
-    <row r="49" spans="2:28" ht="12.75" customHeight="1">
+    <row r="49" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="10" t="s">
         <v>356</v>
       </c>
@@ -4598,7 +4626,7 @@
       <c r="AA49" s="43"/>
       <c r="AB49" s="43"/>
     </row>
-    <row r="50" spans="2:28" ht="12.75" customHeight="1">
+    <row r="50" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="10" t="s">
         <v>360</v>
       </c>
@@ -4633,7 +4661,7 @@
       <c r="AA50" s="43"/>
       <c r="AB50" s="43"/>
     </row>
-    <row r="51" spans="2:28" ht="12.75" customHeight="1">
+    <row r="51" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="10" t="s">
         <v>362</v>
       </c>
@@ -4668,16 +4696,34 @@
       <c r="AA51" s="43"/>
       <c r="AB51" s="43"/>
     </row>
-    <row r="52" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10"/>
+    <row r="52" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="J52" s="10">
+        <v>1000</v>
+      </c>
       <c r="K52" s="15"/>
       <c r="L52" s="15"/>
       <c r="M52" s="61"/>
@@ -4697,16 +4743,34 @@
       <c r="AA52" s="43"/>
       <c r="AB52" s="43"/>
     </row>
-    <row r="53" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10"/>
+    <row r="53" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="J53" s="10">
+        <v>1000</v>
+      </c>
       <c r="K53" s="15"/>
       <c r="L53" s="15"/>
       <c r="M53" s="61"/>
@@ -4726,16 +4790,35 @@
       <c r="AA53" s="43"/>
       <c r="AB53" s="43"/>
     </row>
-    <row r="54" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
+    <row r="54" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="J54" s="10">
+        <f>10^12</f>
+        <v>1000000000000</v>
+      </c>
       <c r="K54" s="15"/>
       <c r="L54" s="15"/>
       <c r="M54" s="61"/>
@@ -4755,15 +4838,31 @@
       <c r="AA54" s="43"/>
       <c r="AB54" s="43"/>
     </row>
-    <row r="55" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
+    <row r="55" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="J55" s="10"/>
       <c r="K55" s="15"/>
       <c r="L55" s="15"/>
@@ -4784,7 +4883,7 @@
       <c r="AA55" s="43"/>
       <c r="AB55" s="43"/>
     </row>
-    <row r="56" spans="2:28" ht="12.75" customHeight="1">
+    <row r="56" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -4813,7 +4912,7 @@
       <c r="AA56" s="43"/>
       <c r="AB56" s="43"/>
     </row>
-    <row r="57" spans="2:28" ht="12.75" customHeight="1">
+    <row r="57" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
@@ -4842,7 +4941,7 @@
       <c r="AA57" s="43"/>
       <c r="AB57" s="43"/>
     </row>
-    <row r="58" spans="2:28" ht="12.75" customHeight="1">
+    <row r="58" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
@@ -4871,7 +4970,7 @@
       <c r="AA58" s="43"/>
       <c r="AB58" s="43"/>
     </row>
-    <row r="59" spans="2:28" ht="12.75" customHeight="1">
+    <row r="59" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -4900,7 +4999,7 @@
       <c r="AA59" s="43"/>
       <c r="AB59" s="43"/>
     </row>
-    <row r="60" spans="2:28" ht="12.75" customHeight="1">
+    <row r="60" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
@@ -4929,7 +5028,7 @@
       <c r="AA60" s="43"/>
       <c r="AB60" s="43"/>
     </row>
-    <row r="61" spans="2:28" ht="12.75" customHeight="1">
+    <row r="61" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
@@ -4958,7 +5057,7 @@
       <c r="AA61" s="43"/>
       <c r="AB61" s="43"/>
     </row>
-    <row r="62" spans="2:28" ht="12.75" customHeight="1">
+    <row r="62" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="10"/>
@@ -4987,7 +5086,7 @@
       <c r="AA62" s="43"/>
       <c r="AB62" s="43"/>
     </row>
-    <row r="63" spans="2:28" ht="12.75" customHeight="1">
+    <row r="63" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -5016,7 +5115,7 @@
       <c r="AA63" s="43"/>
       <c r="AB63" s="43"/>
     </row>
-    <row r="64" spans="2:28" ht="12.75" customHeight="1">
+    <row r="64" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="38"/>
       <c r="C64" s="38"/>
       <c r="D64" s="38"/>
@@ -5043,7 +5142,7 @@
       <c r="AA64" s="43"/>
       <c r="AB64" s="43"/>
     </row>
-    <row r="65" spans="2:28" ht="12.75" customHeight="1">
+    <row r="65" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="38"/>
       <c r="C65" s="38"/>
       <c r="D65" s="38"/>
@@ -5070,7 +5169,7 @@
       <c r="AA65" s="43"/>
       <c r="AB65" s="43"/>
     </row>
-    <row r="66" spans="2:28" ht="12.75" customHeight="1">
+    <row r="66" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="38"/>
       <c r="C66" s="38"/>
       <c r="D66" s="38"/>
@@ -5097,7 +5196,7 @@
       <c r="AA66" s="43"/>
       <c r="AB66" s="43"/>
     </row>
-    <row r="67" spans="2:28" ht="12.75" customHeight="1">
+    <row r="67" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="38"/>
       <c r="C67" s="38"/>
       <c r="D67" s="38"/>
@@ -5124,7 +5223,7 @@
       <c r="AA67" s="43"/>
       <c r="AB67" s="43"/>
     </row>
-    <row r="68" spans="2:28" ht="12.75" customHeight="1">
+    <row r="68" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="38"/>
       <c r="C68" s="38"/>
       <c r="D68" s="38"/>
@@ -5151,7 +5250,7 @@
       <c r="AA68" s="43"/>
       <c r="AB68" s="43"/>
     </row>
-    <row r="69" spans="2:28" ht="12.75" customHeight="1">
+    <row r="69" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="38"/>
       <c r="C69" s="38"/>
       <c r="D69" s="38"/>
@@ -5178,7 +5277,7 @@
       <c r="AA69" s="43"/>
       <c r="AB69" s="43"/>
     </row>
-    <row r="70" spans="2:28" ht="12.75" customHeight="1">
+    <row r="70" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="38"/>
       <c r="C70" s="38"/>
       <c r="D70" s="38"/>
@@ -5205,7 +5304,7 @@
       <c r="AA70" s="43"/>
       <c r="AB70" s="43"/>
     </row>
-    <row r="71" spans="2:28" ht="12.75" customHeight="1">
+    <row r="71" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="38"/>
       <c r="C71" s="38"/>
       <c r="D71" s="38"/>
@@ -5232,7 +5331,7 @@
       <c r="AA71" s="43"/>
       <c r="AB71" s="43"/>
     </row>
-    <row r="72" spans="2:28" ht="12.75" customHeight="1">
+    <row r="72" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="38"/>
       <c r="C72" s="38"/>
       <c r="D72" s="38"/>
@@ -5259,7 +5358,7 @@
       <c r="AA72" s="43"/>
       <c r="AB72" s="43"/>
     </row>
-    <row r="73" spans="2:28" ht="12.75" customHeight="1">
+    <row r="73" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="38"/>
       <c r="C73" s="38"/>
       <c r="D73" s="38"/>
@@ -5286,7 +5385,7 @@
       <c r="AA73" s="43"/>
       <c r="AB73" s="43"/>
     </row>
-    <row r="74" spans="2:28" ht="12.75" customHeight="1">
+    <row r="74" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="38"/>
       <c r="C74" s="38"/>
       <c r="D74" s="38"/>
@@ -5313,7 +5412,7 @@
       <c r="AA74" s="43"/>
       <c r="AB74" s="43"/>
     </row>
-    <row r="75" spans="2:28" ht="12.75" customHeight="1">
+    <row r="75" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="35"/>
       <c r="C75" s="35"/>
       <c r="D75" s="35"/>
@@ -5340,7 +5439,7 @@
       <c r="AA75" s="43"/>
       <c r="AB75" s="43"/>
     </row>
-    <row r="76" spans="2:28" ht="12.75" customHeight="1">
+    <row r="76" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="35"/>
       <c r="C76" s="35"/>
       <c r="D76" s="35"/>
@@ -5367,7 +5466,7 @@
       <c r="AA76" s="43"/>
       <c r="AB76" s="43"/>
     </row>
-    <row r="77" spans="2:28" ht="12.75" customHeight="1">
+    <row r="77" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="35"/>
       <c r="C77" s="35"/>
       <c r="D77" s="35"/>
@@ -5394,7 +5493,7 @@
       <c r="AA77" s="43"/>
       <c r="AB77" s="43"/>
     </row>
-    <row r="78" spans="2:28" ht="12.75" customHeight="1">
+    <row r="78" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M78" s="61"/>
       <c r="N78" s="61"/>
       <c r="O78" s="61"/>
@@ -5412,7 +5511,7 @@
       <c r="AA78" s="43"/>
       <c r="AB78" s="43"/>
     </row>
-    <row r="79" spans="2:28" ht="12.75" customHeight="1">
+    <row r="79" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M79" s="61"/>
       <c r="N79" s="61"/>
       <c r="O79" s="61"/>
@@ -5430,7 +5529,7 @@
       <c r="AA79" s="43"/>
       <c r="AB79" s="43"/>
     </row>
-    <row r="80" spans="2:28" ht="12.75" customHeight="1">
+    <row r="80" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M80" s="61"/>
       <c r="N80" s="61"/>
       <c r="O80" s="61"/>
@@ -5448,7 +5547,7 @@
       <c r="AA80" s="43"/>
       <c r="AB80" s="43"/>
     </row>
-    <row r="81" spans="13:28" ht="12.75" customHeight="1">
+    <row r="81" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M81" s="61"/>
       <c r="N81" s="61"/>
       <c r="O81" s="61"/>
@@ -5466,7 +5565,7 @@
       <c r="AA81" s="43"/>
       <c r="AB81" s="43"/>
     </row>
-    <row r="82" spans="13:28" ht="12.75" customHeight="1">
+    <row r="82" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M82" s="61"/>
       <c r="N82" s="61"/>
       <c r="O82" s="61"/>
@@ -5484,7 +5583,7 @@
       <c r="AA82" s="43"/>
       <c r="AB82" s="43"/>
     </row>
-    <row r="83" spans="13:28" ht="12.75" customHeight="1">
+    <row r="83" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M83" s="61"/>
       <c r="N83" s="61"/>
       <c r="O83" s="61"/>
@@ -5502,7 +5601,7 @@
       <c r="AA83" s="43"/>
       <c r="AB83" s="43"/>
     </row>
-    <row r="84" spans="13:28" ht="12.75" customHeight="1">
+    <row r="84" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M84" s="61"/>
       <c r="N84" s="61"/>
       <c r="O84" s="61"/>
@@ -5520,7 +5619,7 @@
       <c r="AA84" s="43"/>
       <c r="AB84" s="43"/>
     </row>
-    <row r="85" spans="13:28" ht="12.75" customHeight="1">
+    <row r="85" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M85" s="61"/>
       <c r="N85" s="61"/>
       <c r="O85" s="61"/>
@@ -5538,7 +5637,7 @@
       <c r="AA85" s="43"/>
       <c r="AB85" s="43"/>
     </row>
-    <row r="86" spans="13:28" ht="12.75" customHeight="1">
+    <row r="86" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M86" s="61"/>
       <c r="N86" s="61"/>
       <c r="O86" s="61"/>
@@ -5556,7 +5655,7 @@
       <c r="AA86" s="43"/>
       <c r="AB86" s="43"/>
     </row>
-    <row r="87" spans="13:28" ht="12.75" customHeight="1">
+    <row r="87" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M87" s="61"/>
       <c r="N87" s="61"/>
       <c r="O87" s="61"/>
@@ -5634,19 +5733,19 @@
       <selection activeCell="F15" sqref="F15:O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="88.6640625" customWidth="1"/>
+    <col min="5" max="5" width="88.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" s="28" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:21" ht="12.75" customHeight="1">
+    <row r="3" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="62" t="s">
         <v>188</v>
       </c>
@@ -5670,7 +5769,7 @@
       <c r="T3" s="62"/>
       <c r="U3" s="62"/>
     </row>
-    <row r="4" spans="2:21">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -5692,7 +5791,7 @@
       <c r="T4" s="62"/>
       <c r="U4" s="62"/>
     </row>
-    <row r="5" spans="2:21">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B5" s="62"/>
       <c r="C5" s="62"/>
       <c r="D5" s="62"/>
@@ -5714,7 +5813,7 @@
       <c r="T5" s="62"/>
       <c r="U5" s="62"/>
     </row>
-    <row r="6" spans="2:21">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -5736,7 +5835,7 @@
       <c r="T6" s="62"/>
       <c r="U6" s="62"/>
     </row>
-    <row r="7" spans="2:21">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="62"/>
       <c r="C7" s="62"/>
       <c r="D7" s="62"/>
@@ -5758,7 +5857,7 @@
       <c r="T7" s="62"/>
       <c r="U7" s="62"/>
     </row>
-    <row r="8" spans="2:21">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
       <c r="D8" s="62"/>
@@ -5780,7 +5879,7 @@
       <c r="T8" s="62"/>
       <c r="U8" s="62"/>
     </row>
-    <row r="9" spans="2:21">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B9" s="62"/>
       <c r="C9" s="62"/>
       <c r="D9" s="62"/>
@@ -5802,7 +5901,7 @@
       <c r="T9" s="62"/>
       <c r="U9" s="62"/>
     </row>
-    <row r="10" spans="2:21">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" s="62"/>
       <c r="C10" s="62"/>
       <c r="D10" s="62"/>
@@ -5824,7 +5923,7 @@
       <c r="T10" s="62"/>
       <c r="U10" s="62"/>
     </row>
-    <row r="11" spans="2:21">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" s="62"/>
       <c r="C11" s="62"/>
       <c r="D11" s="62"/>
@@ -5846,7 +5945,7 @@
       <c r="T11" s="62"/>
       <c r="U11" s="62"/>
     </row>
-    <row r="12" spans="2:21">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
       <c r="D12" s="62"/>
@@ -5868,7 +5967,7 @@
       <c r="T12" s="62"/>
       <c r="U12" s="62"/>
     </row>
-    <row r="15" spans="2:21" ht="12.75" customHeight="1">
+    <row r="15" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>189</v>
       </c>
@@ -5885,7 +5984,7 @@
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
     </row>
-    <row r="16" spans="2:21">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="F16" s="61"/>
       <c r="G16" s="61"/>
       <c r="H16" s="61"/>
@@ -5897,7 +5996,7 @@
       <c r="N16" s="61"/>
       <c r="O16" s="61"/>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F17" s="61"/>
       <c r="G17" s="61"/>
       <c r="H17" s="61"/>
@@ -5909,7 +6008,7 @@
       <c r="N17" s="61"/>
       <c r="O17" s="61"/>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B18" s="28" t="s">
         <v>191</v>
       </c>
@@ -5933,7 +6032,7 @@
       <c r="N18" s="61"/>
       <c r="O18" s="61"/>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>193</v>
       </c>
@@ -5957,7 +6056,7 @@
       <c r="N19" s="61"/>
       <c r="O19" s="61"/>
     </row>
-    <row r="20" spans="2:15">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>196</v>
       </c>
@@ -5978,7 +6077,7 @@
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
     </row>
-    <row r="21" spans="2:15">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>199</v>
       </c>
@@ -5999,7 +6098,7 @@
       <c r="N21" s="61"/>
       <c r="O21" s="61"/>
     </row>
-    <row r="22" spans="2:15">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>61</v>
       </c>
@@ -6020,7 +6119,7 @@
       <c r="N22" s="61"/>
       <c r="O22" s="61"/>
     </row>
-    <row r="23" spans="2:15">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>203</v>
       </c>
@@ -6038,7 +6137,7 @@
       <c r="N23" s="61"/>
       <c r="O23" s="61"/>
     </row>
-    <row r="24" spans="2:15">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
       <c r="H24" s="61"/>
@@ -6050,7 +6149,7 @@
       <c r="N24" s="61"/>
       <c r="O24" s="61"/>
     </row>
-    <row r="25" spans="2:15">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
       <c r="H25" s="61"/>
@@ -6062,7 +6161,7 @@
       <c r="N25" s="61"/>
       <c r="O25" s="61"/>
     </row>
-    <row r="26" spans="2:15">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
       <c r="H26" s="61"/>
@@ -6074,7 +6173,7 @@
       <c r="N26" s="61"/>
       <c r="O26" s="61"/>
     </row>
-    <row r="27" spans="2:15">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F27" s="61"/>
       <c r="G27" s="61"/>
       <c r="H27" s="61"/>
@@ -6086,7 +6185,7 @@
       <c r="N27" s="61"/>
       <c r="O27" s="61"/>
     </row>
-    <row r="28" spans="2:15">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F28" s="61"/>
       <c r="G28" s="61"/>
       <c r="H28" s="61"/>
@@ -6098,7 +6197,7 @@
       <c r="N28" s="61"/>
       <c r="O28" s="61"/>
     </row>
-    <row r="29" spans="2:15">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F29" s="61"/>
       <c r="G29" s="61"/>
       <c r="H29" s="61"/>
@@ -6110,7 +6209,7 @@
       <c r="N29" s="61"/>
       <c r="O29" s="61"/>
     </row>
-    <row r="30" spans="2:15">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F30" s="61"/>
       <c r="G30" s="61"/>
       <c r="H30" s="61"/>
@@ -6122,7 +6221,7 @@
       <c r="N30" s="61"/>
       <c r="O30" s="61"/>
     </row>
-    <row r="31" spans="2:15">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F31" s="61"/>
       <c r="G31" s="61"/>
       <c r="H31" s="61"/>
@@ -6134,7 +6233,7 @@
       <c r="N31" s="61"/>
       <c r="O31" s="61"/>
     </row>
-    <row r="32" spans="2:15">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="F32" s="61"/>
       <c r="G32" s="61"/>
       <c r="H32" s="61"/>
@@ -6146,7 +6245,7 @@
       <c r="N32" s="61"/>
       <c r="O32" s="61"/>
     </row>
-    <row r="33" spans="6:15">
+    <row r="33" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F33" s="61"/>
       <c r="G33" s="61"/>
       <c r="H33" s="61"/>
@@ -6158,7 +6257,7 @@
       <c r="N33" s="61"/>
       <c r="O33" s="61"/>
     </row>
-    <row r="34" spans="6:15">
+    <row r="34" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F34" s="61"/>
       <c r="G34" s="61"/>
       <c r="H34" s="61"/>
@@ -6170,7 +6269,7 @@
       <c r="N34" s="61"/>
       <c r="O34" s="61"/>
     </row>
-    <row r="35" spans="6:15">
+    <row r="35" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F35" s="61"/>
       <c r="G35" s="61"/>
       <c r="H35" s="61"/>
@@ -6182,7 +6281,7 @@
       <c r="N35" s="61"/>
       <c r="O35" s="61"/>
     </row>
-    <row r="36" spans="6:15">
+    <row r="36" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F36" s="61"/>
       <c r="G36" s="61"/>
       <c r="H36" s="61"/>
@@ -6194,7 +6293,7 @@
       <c r="N36" s="61"/>
       <c r="O36" s="61"/>
     </row>
-    <row r="37" spans="6:15">
+    <row r="37" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F37" s="61"/>
       <c r="G37" s="61"/>
       <c r="H37" s="61"/>
@@ -6206,7 +6305,7 @@
       <c r="N37" s="61"/>
       <c r="O37" s="61"/>
     </row>
-    <row r="38" spans="6:15">
+    <row r="38" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F38" s="61"/>
       <c r="G38" s="61"/>
       <c r="H38" s="61"/>
@@ -6218,7 +6317,7 @@
       <c r="N38" s="61"/>
       <c r="O38" s="61"/>
     </row>
-    <row r="39" spans="6:15">
+    <row r="39" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F39" s="61"/>
       <c r="G39" s="61"/>
       <c r="H39" s="61"/>
@@ -6230,7 +6329,7 @@
       <c r="N39" s="61"/>
       <c r="O39" s="61"/>
     </row>
-    <row r="40" spans="6:15">
+    <row r="40" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F40" s="61"/>
       <c r="G40" s="61"/>
       <c r="H40" s="61"/>
@@ -6242,7 +6341,7 @@
       <c r="N40" s="61"/>
       <c r="O40" s="61"/>
     </row>
-    <row r="41" spans="6:15">
+    <row r="41" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F41" s="61"/>
       <c r="G41" s="61"/>
       <c r="H41" s="61"/>
@@ -6254,7 +6353,7 @@
       <c r="N41" s="61"/>
       <c r="O41" s="61"/>
     </row>
-    <row r="42" spans="6:15">
+    <row r="42" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F42" s="61"/>
       <c r="G42" s="61"/>
       <c r="H42" s="61"/>
@@ -6266,7 +6365,7 @@
       <c r="N42" s="61"/>
       <c r="O42" s="61"/>
     </row>
-    <row r="43" spans="6:15">
+    <row r="43" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F43" s="61"/>
       <c r="G43" s="61"/>
       <c r="H43" s="61"/>
@@ -6278,7 +6377,7 @@
       <c r="N43" s="61"/>
       <c r="O43" s="61"/>
     </row>
-    <row r="44" spans="6:15">
+    <row r="44" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F44" s="61"/>
       <c r="G44" s="61"/>
       <c r="H44" s="61"/>
@@ -6290,7 +6389,7 @@
       <c r="N44" s="61"/>
       <c r="O44" s="61"/>
     </row>
-    <row r="45" spans="6:15">
+    <row r="45" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F45" s="61"/>
       <c r="G45" s="61"/>
       <c r="H45" s="61"/>
@@ -6302,7 +6401,7 @@
       <c r="N45" s="61"/>
       <c r="O45" s="61"/>
     </row>
-    <row r="46" spans="6:15">
+    <row r="46" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F46" s="61"/>
       <c r="G46" s="61"/>
       <c r="H46" s="61"/>
@@ -6314,7 +6413,7 @@
       <c r="N46" s="61"/>
       <c r="O46" s="61"/>
     </row>
-    <row r="47" spans="6:15">
+    <row r="47" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F47" s="61"/>
       <c r="G47" s="61"/>
       <c r="H47" s="61"/>
@@ -6326,7 +6425,7 @@
       <c r="N47" s="61"/>
       <c r="O47" s="61"/>
     </row>
-    <row r="48" spans="6:15">
+    <row r="48" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F48" s="61"/>
       <c r="G48" s="61"/>
       <c r="H48" s="61"/>
@@ -6338,7 +6437,7 @@
       <c r="N48" s="61"/>
       <c r="O48" s="61"/>
     </row>
-    <row r="49" spans="6:15">
+    <row r="49" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F49" s="61"/>
       <c r="G49" s="61"/>
       <c r="H49" s="61"/>
@@ -6350,7 +6449,7 @@
       <c r="N49" s="61"/>
       <c r="O49" s="61"/>
     </row>
-    <row r="50" spans="6:15">
+    <row r="50" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F50" s="61"/>
       <c r="G50" s="61"/>
       <c r="H50" s="61"/>
@@ -6362,7 +6461,7 @@
       <c r="N50" s="61"/>
       <c r="O50" s="61"/>
     </row>
-    <row r="51" spans="6:15">
+    <row r="51" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F51" s="61"/>
       <c r="G51" s="61"/>
       <c r="H51" s="61"/>
@@ -6374,7 +6473,7 @@
       <c r="N51" s="61"/>
       <c r="O51" s="61"/>
     </row>
-    <row r="52" spans="6:15">
+    <row r="52" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F52" s="61"/>
       <c r="G52" s="61"/>
       <c r="H52" s="61"/>
@@ -6404,21 +6503,21 @@
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.5" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="33.1640625" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -6453,7 +6552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
         <v>205</v>
       </c>
@@ -6468,7 +6567,7 @@
       <c r="J2" s="40"/>
       <c r="K2" s="40"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="46">
         <v>1</v>
       </c>
@@ -6495,7 +6594,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="46">
         <v>2</v>
       </c>
@@ -6522,7 +6621,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="46">
         <v>3</v>
       </c>
@@ -6543,7 +6642,7 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="46">
         <v>4</v>
       </c>
@@ -6564,7 +6663,7 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="46">
         <v>5</v>
       </c>
@@ -6585,7 +6684,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C8" s="34" t="s">
         <v>73</v>
       </c>
@@ -6596,7 +6695,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C9" s="34" t="s">
         <v>78</v>
       </c>
@@ -6604,7 +6703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C10" s="10" t="s">
         <v>84</v>
       </c>
@@ -6612,7 +6711,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C11" s="10" t="s">
         <v>89</v>
       </c>
@@ -6620,7 +6719,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C12" s="10" t="s">
         <v>93</v>
       </c>
@@ -6628,7 +6727,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C13" s="10" t="s">
         <v>97</v>
       </c>
@@ -6636,7 +6735,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C14" s="10" t="s">
         <v>97</v>
       </c>
@@ -6644,7 +6743,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" s="10" t="s">
         <v>101</v>
       </c>
@@ -6652,7 +6751,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" s="10" t="s">
         <v>105</v>
       </c>
@@ -6660,7 +6759,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" s="10" t="s">
         <v>108</v>
       </c>
@@ -6668,7 +6767,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" s="10" t="s">
         <v>112</v>
       </c>
@@ -6676,7 +6775,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" s="10" t="s">
         <v>61</v>
       </c>
@@ -6684,7 +6783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="3:5">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" s="10" t="s">
         <v>121</v>
       </c>
@@ -6692,7 +6791,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="3:5">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" s="10" t="s">
         <v>124</v>
       </c>
@@ -6700,7 +6799,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="3:5">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C22" s="10" t="s">
         <v>127</v>
       </c>
@@ -6708,7 +6807,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="3:5">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C23" s="10" t="s">
         <v>131</v>
       </c>
@@ -6716,7 +6815,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="3:5">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C24" s="10" t="s">
         <v>134</v>
       </c>
@@ -6724,7 +6823,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="3:5">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C25" s="10" t="s">
         <v>139</v>
       </c>
@@ -6732,7 +6831,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="3:5">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C26" s="10" t="s">
         <v>143</v>
       </c>
@@ -6740,7 +6839,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="3:5">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C27" s="10" t="s">
         <v>149</v>
       </c>
@@ -6748,7 +6847,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="3:5">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C28" s="10" t="s">
         <v>152</v>
       </c>
@@ -6756,7 +6855,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="29" spans="3:5">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C29" s="10" t="s">
         <v>156</v>
       </c>
@@ -6764,7 +6863,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="3:5">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C30" s="10" t="s">
         <v>158</v>
       </c>
@@ -6772,7 +6871,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="3:5">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C31" s="10" t="s">
         <v>159</v>
       </c>
@@ -6780,7 +6879,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="3:5">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C32" s="10" t="s">
         <v>235</v>
       </c>
@@ -6788,7 +6887,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="3:5">
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C33" s="10" t="s">
         <v>166</v>
       </c>
@@ -6796,7 +6895,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="3:5">
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C34" s="10" t="s">
         <v>167</v>
       </c>
@@ -6804,7 +6903,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="35" spans="3:5">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C35" s="10" t="s">
         <v>168</v>
       </c>
@@ -6812,7 +6911,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="3:5">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C36" s="10" t="s">
         <v>173</v>
       </c>
@@ -6820,7 +6919,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="3:5">
+    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C37" s="10" t="s">
         <v>177</v>
       </c>
@@ -6828,7 +6927,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="3:5">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C38" s="10" t="s">
         <v>181</v>
       </c>
@@ -6836,7 +6935,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="3:5">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C39" s="10" t="s">
         <v>184</v>
       </c>
@@ -6844,557 +6943,557 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="3:5">
+    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E40" s="10" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="41" spans="3:5">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E41" s="10" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="3:5">
+    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E42" s="10" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="3:5">
+    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E43" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="3:5">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E44" s="10" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="3:5">
+    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E45" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="3:5">
+    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E46" s="10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="3:5">
+    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E47" s="10" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="48" spans="3:5">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E48" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="5:5">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E49" s="10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="5:5">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E50" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="5:5">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E51" s="10" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="5:5">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E52" s="10" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="53" spans="5:5">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E53" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="5:5">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E54" s="10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="5:5">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E55" s="10" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="56" spans="5:5">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E56" s="10" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="5:5">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E57" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="58" spans="5:5">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E58" s="10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="59" spans="5:5">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E59" s="10" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="60" spans="5:5">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E60" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="5:5">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E61" s="10" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="62" spans="5:5">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E62" s="10" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="63" spans="5:5">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E63" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="64" spans="5:5">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E64" s="10" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="65" spans="5:5">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E65" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="66" spans="5:5">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E66" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="5:5">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E67" s="10" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="5:5">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E68" s="10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="69" spans="5:5">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E69" s="10" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="70" spans="5:5">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E70" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="5:5">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E71" s="10" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="5:5">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E72" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="73" spans="5:5">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E73" s="10" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="5:5">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E74" s="10" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="75" spans="5:5">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E75" s="10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="76" spans="5:5">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E76" s="10" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="77" spans="5:5">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E77" s="10" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="78" spans="5:5">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E78" s="10" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="79" spans="5:5">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E79" s="10" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="80" spans="5:5">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E80" s="10" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="5:5">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E81" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="82" spans="5:5">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E82" s="10" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="83" spans="5:5">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E83" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="84" spans="5:5">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E84" s="10" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="5:5">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E85" s="10" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="5:5">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E86" s="10" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="87" spans="5:5">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E87" s="10" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="88" spans="5:5">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E88" s="10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="5:5">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E89" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="90" spans="5:5">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E90" s="10" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="91" spans="5:5">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E91" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="5:5">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E92" s="10" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="5:5">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E93" s="10" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="94" spans="5:5">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E94" s="10" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="5:5">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E95" s="10" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="5:5">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E96" s="10" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="97" spans="5:5">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E97" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="5:5">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E98" s="10" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="99" spans="5:5">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E99" s="10" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="100" spans="5:5">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E100" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="101" spans="5:5">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E101" s="10" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="102" spans="5:5">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E102" s="10" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="103" spans="5:5">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E103" s="10" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="104" spans="5:5">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E104" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="105" spans="5:5">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E105" s="10" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="106" spans="5:5">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E106" s="10" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="107" spans="5:5">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E107" s="10" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="108" spans="5:5">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E108" s="10" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="109" spans="5:5">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E109" s="10" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="110" spans="5:5">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E110" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="111" spans="5:5">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E111" s="10" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="112" spans="5:5">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E112" s="10" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="113" spans="5:5">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E113" s="10" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="114" spans="5:5">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E114" s="10" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="115" spans="5:5">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E115" s="10" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="116" spans="5:5">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E116" s="10" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="117" spans="5:5">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E117" s="10" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="118" spans="5:5">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E118" s="10" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="119" spans="5:5">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E119" s="10" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="120" spans="5:5">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E120" s="10" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="121" spans="5:5">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E121" s="10" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="5:5">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E122" s="10" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="123" spans="5:5">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E123" s="10" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="124" spans="5:5">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E124" s="10" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="125" spans="5:5">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E125" s="10" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="126" spans="5:5">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E126" s="10" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="127" spans="5:5">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E127" s="10" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="128" spans="5:5">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E128" s="10" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="129" spans="5:5">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E129" s="10" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="130" spans="5:5">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E130" s="10" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="131" spans="5:5">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E131" s="10" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="132" spans="5:5">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E132" s="10" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="133" spans="5:5">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E133" s="10" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="134" spans="5:5">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E134" s="10" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="135" spans="5:5">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E135" s="10" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="136" spans="5:5">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E136" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="5:5">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E137" s="10" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="138" spans="5:5">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E138" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="139" spans="5:5">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E139" s="10" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="140" spans="5:5">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E140" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="141" spans="5:5">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E141" s="10" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="142" spans="5:5">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E142" s="10" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="143" spans="5:5">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E143" s="10" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="144" spans="5:5">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E144" s="10" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="145" spans="5:5">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E145" s="10" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="146" spans="5:5">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E146" s="10" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="147" spans="5:5">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E147" s="10" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="148" spans="5:5">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E148" s="10" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="149" spans="5:5">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E149" s="10" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="150" spans="5:5">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E150" s="10" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
BEA API tool can now pull data from 3 of the BEA datasets: NIPA, NIPA_Details & FixedAsset.
</commit_message>
<xml_diff>
--- a/Generic_Macro/Control.xlsx
+++ b/Generic_Macro/Control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimmi\OneDrive\Documents\Documents\Scripts\VenV\Plebs_Macro\Generic_Macro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/TempVenv/Plebs_Macro/Generic_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB8111D-017F-404D-9ED8-BA0173E02F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2AE56F-AEFF-F94F-8EB6-B38385DC70C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter_Input" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="375">
   <si>
     <t>Index</t>
   </si>
@@ -1307,9 +1307,6 @@
     <t>odl</t>
   </si>
   <si>
-    <t>2010-01-01</t>
-  </si>
-  <si>
     <t>M2 money supply (U.S)</t>
   </si>
   <si>
@@ -1325,14 +1322,23 @@
     <t>Global M2 (top 50)</t>
   </si>
   <si>
-    <t>Monetary Aggregates, Bitcoin &amp; Equities.</t>
+    <t xml:space="preserve">Monetary Aggregates &amp; CPI. </t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>CPI YoY % change</t>
+  </si>
+  <si>
+    <t>1994-01-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1584,7 +1590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1741,6 +1747,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2127,25 +2136,25 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
     <col min="8" max="9" width="44" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
-    <col min="14" max="14" width="18.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="15.5" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" customWidth="1"/>
+    <col min="15" max="15" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2192,12 +2201,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>360</v>
+        <v>63</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>15</v>
@@ -2209,65 +2218,67 @@
         <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>365</v>
+        <v>65</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
       <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-    </row>
-    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="O2" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>54</v>
+        <v>373</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="N3" s="9"/>
+      <c r="O3" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>75</v>
+        <v>360</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>15</v>
@@ -2276,33 +2287,36 @@
         <v>16</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>76</v>
+        <v>365</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>77</v>
+        <v>361</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>30</v>
+        <v>367</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="7"/>
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
-      <c r="O4" s="10"/>
-    </row>
-    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="O4" s="8">
+        <f>10^12</f>
+        <v>1000000000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>370</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>15</v>
@@ -2311,47 +2325,69 @@
         <v>16</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>110</v>
+        <v>18</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="I5" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>367</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="9">
-        <v>2.5</v>
-      </c>
-      <c r="O5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="N5" s="9"/>
+      <c r="O5" s="8">
+        <f>10^12</f>
+        <v>1000000000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>367</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
-      <c r="O6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O6" s="63">
+        <f>10^12</f>
+        <v>1000000000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2366,12 +2402,12 @@
       <c r="L7" s="14"/>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="16">
       <c r="A8" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="C8" s="56" t="s">
         <v>32</v>
@@ -2386,7 +2422,7 @@
       <c r="K8" s="18"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="16">
       <c r="A9" s="16" t="s">
         <v>33</v>
       </c>
@@ -2404,7 +2440,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="16">
       <c r="A10" s="13"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -2418,7 +2454,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="16">
       <c r="A11" s="20" t="s">
         <v>35</v>
       </c>
@@ -2436,12 +2472,12 @@
       <c r="K11" s="18"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="16">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="59" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
@@ -2454,7 +2490,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="16">
       <c r="A13" s="21" t="s">
         <v>38</v>
       </c>
@@ -2472,7 +2508,7 @@
       <c r="K13" s="18"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="16">
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -2484,7 +2520,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="16">
       <c r="A15" s="21" t="s">
         <v>353</v>
       </c>
@@ -2502,7 +2538,7 @@
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="16">
       <c r="A16" s="51" t="s">
         <v>355</v>
       </c>
@@ -2512,13 +2548,13 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="13"/>
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="16">
       <c r="A17" s="51" t="s">
         <v>354</v>
       </c>
@@ -2534,7 +2570,7 @@
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
     </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="16">
       <c r="A18" s="13"/>
       <c r="B18" s="23"/>
       <c r="C18" s="18"/>
@@ -2548,7 +2584,7 @@
       <c r="K18" s="18"/>
       <c r="L18" s="19"/>
     </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="16">
       <c r="A19" s="13"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -2562,7 +2598,7 @@
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" s="24"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
@@ -2573,7 +2609,7 @@
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -2586,7 +2622,7 @@
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" s="24"/>
       <c r="B22" s="25"/>
       <c r="C22" s="26"/>
@@ -2597,7 +2633,7 @@
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
@@ -2608,7 +2644,7 @@
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" s="24"/>
       <c r="B24" s="25"/>
       <c r="C24" s="25"/>
@@ -2619,7 +2655,7 @@
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
     </row>
-    <row r="25" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="14">
       <c r="A25" s="24"/>
       <c r="B25" s="53"/>
       <c r="C25" s="54"/>
@@ -2633,7 +2669,7 @@
       <c r="K25" s="15"/>
       <c r="L25" s="24"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" s="24"/>
       <c r="B26" s="25"/>
       <c r="C26" s="25"/>
@@ -2646,35 +2682,35 @@
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="16">
       <c r="A27" s="15"/>
       <c r="E27" s="23"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" s="15"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" s="15"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" s="15"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" s="15"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" s="15"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="15"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="15"/>
       <c r="I34" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="15"/>
     </row>
   </sheetData>
@@ -2755,25 +2791,25 @@
   <dimension ref="A1:AB87"/>
   <sheetViews>
     <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B62" sqref="B60:I62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="46.7109375" customWidth="1"/>
-    <col min="9" max="9" width="35.28515625" customWidth="1"/>
-    <col min="10" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
+    <col min="8" max="8" width="46.6640625" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" customWidth="1"/>
+    <col min="10" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="25.5" customWidth="1"/>
     <col min="14" max="14" width="119" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="D1" s="27" t="s">
         <v>39</v>
       </c>
@@ -2794,7 +2830,7 @@
       <c r="R1" s="31"/>
       <c r="S1" s="31"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="29" t="s">
         <v>0</v>
       </c>
@@ -2836,7 +2872,7 @@
       <c r="R2" s="36"/>
       <c r="S2" s="37"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="B3" s="34" t="s">
         <v>14</v>
       </c>
@@ -2872,7 +2908,7 @@
       <c r="R3" s="35"/>
       <c r="S3" s="35"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="B4" s="34" t="s">
         <v>46</v>
       </c>
@@ -2908,7 +2944,7 @@
       <c r="R4" s="35"/>
       <c r="S4" s="35"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="B5" s="10" t="s">
         <v>51</v>
       </c>
@@ -2944,7 +2980,7 @@
       <c r="R5" s="35"/>
       <c r="S5" s="35"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="B6" s="34" t="s">
         <v>57</v>
       </c>
@@ -2980,7 +3016,7 @@
       <c r="R6" s="35"/>
       <c r="S6" s="35"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="B7" s="34" t="s">
         <v>63</v>
       </c>
@@ -3016,7 +3052,7 @@
       <c r="R7" s="35"/>
       <c r="S7" s="35"/>
     </row>
-    <row r="8" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="14">
       <c r="B8" s="39" t="s">
         <v>69</v>
       </c>
@@ -3047,7 +3083,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19">
       <c r="B9" s="34" t="s">
         <v>75</v>
       </c>
@@ -3078,7 +3114,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19">
       <c r="B10" s="10" t="s">
         <v>80</v>
       </c>
@@ -3112,7 +3148,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19">
       <c r="B11" s="10" t="s">
         <v>86</v>
       </c>
@@ -3142,7 +3178,7 @@
       </c>
       <c r="N11" s="35"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19">
       <c r="B12" s="10" t="s">
         <v>51</v>
       </c>
@@ -3174,7 +3210,7 @@
       </c>
       <c r="N12" s="35"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19">
       <c r="B13" s="10" t="s">
         <v>94</v>
       </c>
@@ -3206,7 +3242,7 @@
       </c>
       <c r="N13" s="35"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19">
       <c r="B14" s="10" t="s">
         <v>98</v>
       </c>
@@ -3235,7 +3271,7 @@
       </c>
       <c r="N14" s="35"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19">
       <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
@@ -3259,7 +3295,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19">
       <c r="B16" s="34" t="s">
         <v>51</v>
       </c>
@@ -3293,7 +3329,7 @@
       </c>
       <c r="N16" s="35"/>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:28">
       <c r="B17" s="34" t="s">
         <v>106</v>
       </c>
@@ -3328,7 +3364,7 @@
       </c>
       <c r="N17" s="35"/>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:28">
       <c r="B18" s="34" t="s">
         <v>109</v>
       </c>
@@ -3362,7 +3398,7 @@
       </c>
       <c r="N18" s="35"/>
     </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:28">
       <c r="B19" s="34" t="s">
         <v>113</v>
       </c>
@@ -3396,7 +3432,7 @@
       </c>
       <c r="N19" s="35"/>
     </row>
-    <row r="20" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:28" ht="12.75" customHeight="1">
       <c r="B20" s="34" t="s">
         <v>117</v>
       </c>
@@ -3442,7 +3478,7 @@
       <c r="AA20" s="43"/>
       <c r="AB20" s="43"/>
     </row>
-    <row r="21" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:28" ht="12.75" customHeight="1">
       <c r="B21" s="34" t="s">
         <v>122</v>
       </c>
@@ -3478,7 +3514,7 @@
       <c r="AA21" s="43"/>
       <c r="AB21" s="43"/>
     </row>
-    <row r="22" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:28" ht="12.75" customHeight="1">
       <c r="B22" s="10" t="s">
         <v>125</v>
       </c>
@@ -3514,7 +3550,7 @@
       <c r="AA22" s="43"/>
       <c r="AB22" s="43"/>
     </row>
-    <row r="23" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:28" ht="12.75" customHeight="1">
       <c r="B23" s="34" t="s">
         <v>128</v>
       </c>
@@ -3560,7 +3596,7 @@
       <c r="AA23" s="43"/>
       <c r="AB23" s="43"/>
     </row>
-    <row r="24" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:28" ht="12.75" customHeight="1">
       <c r="B24" s="10" t="s">
         <v>132</v>
       </c>
@@ -3596,7 +3632,7 @@
       <c r="AA24" s="43"/>
       <c r="AB24" s="43"/>
     </row>
-    <row r="25" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:28" ht="12.75" customHeight="1">
       <c r="B25" s="34" t="s">
         <v>135</v>
       </c>
@@ -3643,7 +3679,7 @@
       <c r="AA25" s="43"/>
       <c r="AB25" s="43"/>
     </row>
-    <row r="26" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:28" ht="12.75" customHeight="1">
       <c r="B26" s="34" t="s">
         <v>140</v>
       </c>
@@ -3690,7 +3726,7 @@
       <c r="AA26" s="43"/>
       <c r="AB26" s="43"/>
     </row>
-    <row r="27" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:28" ht="12.75" customHeight="1">
       <c r="B27" s="17" t="s">
         <v>144</v>
       </c>
@@ -3735,7 +3771,7 @@
       <c r="AA27" s="43"/>
       <c r="AB27" s="43"/>
     </row>
-    <row r="28" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:28" ht="12.75" customHeight="1">
       <c r="B28" s="10" t="s">
         <v>135</v>
       </c>
@@ -3782,7 +3818,7 @@
       <c r="AA28" s="43"/>
       <c r="AB28" s="43"/>
     </row>
-    <row r="29" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:28" ht="12.75" customHeight="1">
       <c r="B29" s="10" t="s">
         <v>153</v>
       </c>
@@ -3825,7 +3861,7 @@
       <c r="AA29" s="43"/>
       <c r="AB29" s="43"/>
     </row>
-    <row r="30" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:28" ht="12.75" customHeight="1">
       <c r="B30" s="10" t="s">
         <v>157</v>
       </c>
@@ -3872,7 +3908,7 @@
       <c r="AA30" s="43"/>
       <c r="AB30" s="43"/>
     </row>
-    <row r="31" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:28" ht="12.75" customHeight="1">
       <c r="B31" s="34" t="s">
         <v>106</v>
       </c>
@@ -3917,7 +3953,7 @@
       <c r="AA31" s="43"/>
       <c r="AB31" s="43"/>
     </row>
-    <row r="32" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:28" ht="12.75" customHeight="1">
       <c r="B32" s="34" t="s">
         <v>160</v>
       </c>
@@ -3950,7 +3986,7 @@
       <c r="AA32" s="43"/>
       <c r="AB32" s="43"/>
     </row>
-    <row r="33" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:28" ht="12.75" customHeight="1">
       <c r="B33" s="34" t="s">
         <v>162</v>
       </c>
@@ -3997,7 +4033,7 @@
       <c r="AA33" s="43"/>
       <c r="AB33" s="43"/>
     </row>
-    <row r="34" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:28" ht="12.75" customHeight="1">
       <c r="B34" s="34" t="s">
         <v>14</v>
       </c>
@@ -4044,7 +4080,7 @@
       <c r="AA34" s="43"/>
       <c r="AB34" s="43"/>
     </row>
-    <row r="35" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:28" ht="12.75" customHeight="1">
       <c r="B35" s="34" t="s">
         <v>22</v>
       </c>
@@ -4089,7 +4125,7 @@
       <c r="AA35" s="43"/>
       <c r="AB35" s="43"/>
     </row>
-    <row r="36" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:28" ht="12.75" customHeight="1">
       <c r="B36" s="34" t="s">
         <v>169</v>
       </c>
@@ -4136,7 +4172,7 @@
       <c r="AA36" s="43"/>
       <c r="AB36" s="43"/>
     </row>
-    <row r="37" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:28" ht="12.75" customHeight="1">
       <c r="B37" s="10" t="s">
         <v>153</v>
       </c>
@@ -4183,7 +4219,7 @@
       <c r="AA37" s="43"/>
       <c r="AB37" s="43"/>
     </row>
-    <row r="38" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:28" ht="12.75" customHeight="1">
       <c r="B38" s="34" t="s">
         <v>178</v>
       </c>
@@ -4230,7 +4266,7 @@
       <c r="AA38" s="43"/>
       <c r="AB38" s="43"/>
     </row>
-    <row r="39" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:28" ht="12.75" customHeight="1">
       <c r="B39" s="10" t="s">
         <v>182</v>
       </c>
@@ -4267,7 +4303,7 @@
       <c r="AA39" s="43"/>
       <c r="AB39" s="43"/>
     </row>
-    <row r="40" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:28" ht="12.75" customHeight="1">
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
       <c r="D40" s="34"/>
@@ -4297,7 +4333,7 @@
       <c r="AA40" s="43"/>
       <c r="AB40" s="43"/>
     </row>
-    <row r="41" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:28" ht="12.75" customHeight="1">
       <c r="B41" s="34" t="s">
         <v>14</v>
       </c>
@@ -4329,7 +4365,7 @@
       <c r="AA41" s="43"/>
       <c r="AB41" s="43"/>
     </row>
-    <row r="42" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:28" ht="12.75" customHeight="1">
       <c r="B42" s="10" t="s">
         <v>22</v>
       </c>
@@ -4359,7 +4395,7 @@
       <c r="AA42" s="43"/>
       <c r="AB42" s="43"/>
     </row>
-    <row r="43" spans="2:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:28" ht="27.75" customHeight="1">
       <c r="B43" s="10" t="s">
         <v>169</v>
       </c>
@@ -4392,7 +4428,7 @@
       <c r="AA43" s="43"/>
       <c r="AB43" s="43"/>
     </row>
-    <row r="44" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:28" ht="12.75" customHeight="1">
       <c r="B44" s="10" t="s">
         <v>27</v>
       </c>
@@ -4433,7 +4469,7 @@
       <c r="AA44" s="43"/>
       <c r="AB44" s="43"/>
     </row>
-    <row r="45" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:28" ht="12.75" customHeight="1">
       <c r="B45" s="10" t="s">
         <v>14</v>
       </c>
@@ -4472,7 +4508,7 @@
       <c r="AA45" s="43"/>
       <c r="AB45" s="43"/>
     </row>
-    <row r="46" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:28" ht="12.75" customHeight="1">
       <c r="B46" s="10" t="s">
         <v>122</v>
       </c>
@@ -4511,7 +4547,7 @@
       <c r="AA46" s="43"/>
       <c r="AB46" s="43"/>
     </row>
-    <row r="47" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:28" ht="12.75" customHeight="1">
       <c r="B47" s="10" t="s">
         <v>125</v>
       </c>
@@ -4550,7 +4586,7 @@
       <c r="AA47" s="43"/>
       <c r="AB47" s="43"/>
     </row>
-    <row r="48" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:28" ht="12.75" customHeight="1">
       <c r="B48" s="10" t="s">
         <v>75</v>
       </c>
@@ -4581,7 +4617,7 @@
       <c r="AA48" s="43"/>
       <c r="AB48" s="43"/>
     </row>
-    <row r="49" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:28" ht="12.75" customHeight="1">
       <c r="B49" s="10" t="s">
         <v>356</v>
       </c>
@@ -4626,7 +4662,7 @@
       <c r="AA49" s="43"/>
       <c r="AB49" s="43"/>
     </row>
-    <row r="50" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:28" ht="12.75" customHeight="1">
       <c r="B50" s="10" t="s">
         <v>360</v>
       </c>
@@ -4661,7 +4697,7 @@
       <c r="AA50" s="43"/>
       <c r="AB50" s="43"/>
     </row>
-    <row r="51" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:28" ht="12.75" customHeight="1">
       <c r="B51" s="10" t="s">
         <v>362</v>
       </c>
@@ -4696,7 +4732,7 @@
       <c r="AA51" s="43"/>
       <c r="AB51" s="43"/>
     </row>
-    <row r="52" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:28" ht="12.75" customHeight="1">
       <c r="B52" s="10" t="s">
         <v>63</v>
       </c>
@@ -4716,10 +4752,10 @@
         <v>19</v>
       </c>
       <c r="H52" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="I52" s="10" t="s">
         <v>367</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>368</v>
       </c>
       <c r="J52" s="10">
         <v>1000</v>
@@ -4743,7 +4779,7 @@
       <c r="AA52" s="43"/>
       <c r="AB52" s="43"/>
     </row>
-    <row r="53" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:28" ht="12.75" customHeight="1">
       <c r="B53" s="10" t="s">
         <v>360</v>
       </c>
@@ -4766,7 +4802,7 @@
         <v>361</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J53" s="10">
         <v>1000</v>
@@ -4790,7 +4826,7 @@
       <c r="AA53" s="43"/>
       <c r="AB53" s="43"/>
     </row>
-    <row r="54" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:28" ht="12.75" customHeight="1">
       <c r="B54" s="10" t="s">
         <v>14</v>
       </c>
@@ -4813,7 +4849,7 @@
         <v>20</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J54" s="10">
         <f>10^12</f>
@@ -4838,7 +4874,7 @@
       <c r="AA54" s="43"/>
       <c r="AB54" s="43"/>
     </row>
-    <row r="55" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:28" ht="12.75" customHeight="1">
       <c r="B55" s="10" t="s">
         <v>75</v>
       </c>
@@ -4883,15 +4919,31 @@
       <c r="AA55" s="43"/>
       <c r="AB55" s="43"/>
     </row>
-    <row r="56" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
+    <row r="56" spans="2:28" ht="12.75" customHeight="1">
+      <c r="B56" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>367</v>
+      </c>
       <c r="J56" s="10"/>
       <c r="K56" s="15"/>
       <c r="L56" s="15"/>
@@ -4912,14 +4964,28 @@
       <c r="AA56" s="43"/>
       <c r="AB56" s="43"/>
     </row>
-    <row r="57" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
+    <row r="57" spans="2:28" ht="12.75" customHeight="1">
+      <c r="B57" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="15"/>
@@ -4941,15 +5007,31 @@
       <c r="AA57" s="43"/>
       <c r="AB57" s="43"/>
     </row>
-    <row r="58" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
+    <row r="58" spans="2:28" ht="12.75" customHeight="1">
+      <c r="B58" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I58" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="J58" s="10"/>
       <c r="K58" s="15"/>
       <c r="L58" s="15"/>
@@ -4970,14 +5052,28 @@
       <c r="AA58" s="43"/>
       <c r="AB58" s="43"/>
     </row>
-    <row r="59" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10"/>
+    <row r="59" spans="2:28" ht="12.75" customHeight="1">
+      <c r="B59" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>370</v>
+      </c>
       <c r="I59" s="10"/>
       <c r="J59" s="10"/>
       <c r="K59" s="15"/>
@@ -4999,15 +5095,31 @@
       <c r="AA59" s="43"/>
       <c r="AB59" s="43"/>
     </row>
-    <row r="60" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="10"/>
+    <row r="60" spans="2:28" ht="12.75" customHeight="1">
+      <c r="B60" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="I60" s="10" t="s">
+        <v>367</v>
+      </c>
       <c r="J60" s="10"/>
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
@@ -5028,15 +5140,31 @@
       <c r="AA60" s="43"/>
       <c r="AB60" s="43"/>
     </row>
-    <row r="61" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
+    <row r="61" spans="2:28" ht="12.75" customHeight="1">
+      <c r="B61" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I61" s="10" t="s">
+        <v>367</v>
+      </c>
       <c r="J61" s="10"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
@@ -5057,15 +5185,31 @@
       <c r="AA61" s="43"/>
       <c r="AB61" s="43"/>
     </row>
-    <row r="62" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
+    <row r="62" spans="2:28" ht="12.75" customHeight="1">
+      <c r="B62" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="I62" s="10" t="s">
+        <v>367</v>
+      </c>
       <c r="J62" s="10"/>
       <c r="K62" s="15"/>
       <c r="L62" s="15"/>
@@ -5086,7 +5230,7 @@
       <c r="AA62" s="43"/>
       <c r="AB62" s="43"/>
     </row>
-    <row r="63" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:28" ht="12.75" customHeight="1">
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
@@ -5115,7 +5259,7 @@
       <c r="AA63" s="43"/>
       <c r="AB63" s="43"/>
     </row>
-    <row r="64" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:28" ht="12.75" customHeight="1">
       <c r="B64" s="38"/>
       <c r="C64" s="38"/>
       <c r="D64" s="38"/>
@@ -5142,7 +5286,7 @@
       <c r="AA64" s="43"/>
       <c r="AB64" s="43"/>
     </row>
-    <row r="65" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:28" ht="12.75" customHeight="1">
       <c r="B65" s="38"/>
       <c r="C65" s="38"/>
       <c r="D65" s="38"/>
@@ -5169,7 +5313,7 @@
       <c r="AA65" s="43"/>
       <c r="AB65" s="43"/>
     </row>
-    <row r="66" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:28" ht="12.75" customHeight="1">
       <c r="B66" s="38"/>
       <c r="C66" s="38"/>
       <c r="D66" s="38"/>
@@ -5196,7 +5340,7 @@
       <c r="AA66" s="43"/>
       <c r="AB66" s="43"/>
     </row>
-    <row r="67" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:28" ht="12.75" customHeight="1">
       <c r="B67" s="38"/>
       <c r="C67" s="38"/>
       <c r="D67" s="38"/>
@@ -5223,7 +5367,7 @@
       <c r="AA67" s="43"/>
       <c r="AB67" s="43"/>
     </row>
-    <row r="68" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:28" ht="12.75" customHeight="1">
       <c r="B68" s="38"/>
       <c r="C68" s="38"/>
       <c r="D68" s="38"/>
@@ -5250,7 +5394,7 @@
       <c r="AA68" s="43"/>
       <c r="AB68" s="43"/>
     </row>
-    <row r="69" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:28" ht="12.75" customHeight="1">
       <c r="B69" s="38"/>
       <c r="C69" s="38"/>
       <c r="D69" s="38"/>
@@ -5277,7 +5421,7 @@
       <c r="AA69" s="43"/>
       <c r="AB69" s="43"/>
     </row>
-    <row r="70" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:28" ht="12.75" customHeight="1">
       <c r="B70" s="38"/>
       <c r="C70" s="38"/>
       <c r="D70" s="38"/>
@@ -5304,7 +5448,7 @@
       <c r="AA70" s="43"/>
       <c r="AB70" s="43"/>
     </row>
-    <row r="71" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:28" ht="12.75" customHeight="1">
       <c r="B71" s="38"/>
       <c r="C71" s="38"/>
       <c r="D71" s="38"/>
@@ -5331,7 +5475,7 @@
       <c r="AA71" s="43"/>
       <c r="AB71" s="43"/>
     </row>
-    <row r="72" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:28" ht="12.75" customHeight="1">
       <c r="B72" s="38"/>
       <c r="C72" s="38"/>
       <c r="D72" s="38"/>
@@ -5358,7 +5502,7 @@
       <c r="AA72" s="43"/>
       <c r="AB72" s="43"/>
     </row>
-    <row r="73" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:28" ht="12.75" customHeight="1">
       <c r="B73" s="38"/>
       <c r="C73" s="38"/>
       <c r="D73" s="38"/>
@@ -5385,7 +5529,7 @@
       <c r="AA73" s="43"/>
       <c r="AB73" s="43"/>
     </row>
-    <row r="74" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:28" ht="12.75" customHeight="1">
       <c r="B74" s="38"/>
       <c r="C74" s="38"/>
       <c r="D74" s="38"/>
@@ -5412,7 +5556,7 @@
       <c r="AA74" s="43"/>
       <c r="AB74" s="43"/>
     </row>
-    <row r="75" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:28" ht="12.75" customHeight="1">
       <c r="B75" s="35"/>
       <c r="C75" s="35"/>
       <c r="D75" s="35"/>
@@ -5439,7 +5583,7 @@
       <c r="AA75" s="43"/>
       <c r="AB75" s="43"/>
     </row>
-    <row r="76" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:28" ht="12.75" customHeight="1">
       <c r="B76" s="35"/>
       <c r="C76" s="35"/>
       <c r="D76" s="35"/>
@@ -5466,7 +5610,7 @@
       <c r="AA76" s="43"/>
       <c r="AB76" s="43"/>
     </row>
-    <row r="77" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:28" ht="12.75" customHeight="1">
       <c r="B77" s="35"/>
       <c r="C77" s="35"/>
       <c r="D77" s="35"/>
@@ -5493,7 +5637,7 @@
       <c r="AA77" s="43"/>
       <c r="AB77" s="43"/>
     </row>
-    <row r="78" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:28" ht="12.75" customHeight="1">
       <c r="M78" s="61"/>
       <c r="N78" s="61"/>
       <c r="O78" s="61"/>
@@ -5511,7 +5655,7 @@
       <c r="AA78" s="43"/>
       <c r="AB78" s="43"/>
     </row>
-    <row r="79" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:28" ht="12.75" customHeight="1">
       <c r="M79" s="61"/>
       <c r="N79" s="61"/>
       <c r="O79" s="61"/>
@@ -5529,7 +5673,7 @@
       <c r="AA79" s="43"/>
       <c r="AB79" s="43"/>
     </row>
-    <row r="80" spans="2:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:28" ht="12.75" customHeight="1">
       <c r="M80" s="61"/>
       <c r="N80" s="61"/>
       <c r="O80" s="61"/>
@@ -5547,7 +5691,7 @@
       <c r="AA80" s="43"/>
       <c r="AB80" s="43"/>
     </row>
-    <row r="81" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="13:28" ht="12.75" customHeight="1">
       <c r="M81" s="61"/>
       <c r="N81" s="61"/>
       <c r="O81" s="61"/>
@@ -5565,7 +5709,7 @@
       <c r="AA81" s="43"/>
       <c r="AB81" s="43"/>
     </row>
-    <row r="82" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="13:28" ht="12.75" customHeight="1">
       <c r="M82" s="61"/>
       <c r="N82" s="61"/>
       <c r="O82" s="61"/>
@@ -5583,7 +5727,7 @@
       <c r="AA82" s="43"/>
       <c r="AB82" s="43"/>
     </row>
-    <row r="83" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="13:28" ht="12.75" customHeight="1">
       <c r="M83" s="61"/>
       <c r="N83" s="61"/>
       <c r="O83" s="61"/>
@@ -5601,7 +5745,7 @@
       <c r="AA83" s="43"/>
       <c r="AB83" s="43"/>
     </row>
-    <row r="84" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="13:28" ht="12.75" customHeight="1">
       <c r="M84" s="61"/>
       <c r="N84" s="61"/>
       <c r="O84" s="61"/>
@@ -5619,7 +5763,7 @@
       <c r="AA84" s="43"/>
       <c r="AB84" s="43"/>
     </row>
-    <row r="85" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="13:28" ht="12.75" customHeight="1">
       <c r="M85" s="61"/>
       <c r="N85" s="61"/>
       <c r="O85" s="61"/>
@@ -5637,7 +5781,7 @@
       <c r="AA85" s="43"/>
       <c r="AB85" s="43"/>
     </row>
-    <row r="86" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="13:28" ht="12.75" customHeight="1">
       <c r="M86" s="61"/>
       <c r="N86" s="61"/>
       <c r="O86" s="61"/>
@@ -5655,7 +5799,7 @@
       <c r="AA86" s="43"/>
       <c r="AB86" s="43"/>
     </row>
-    <row r="87" spans="13:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="13:28" ht="12.75" customHeight="1">
       <c r="M87" s="61"/>
       <c r="N87" s="61"/>
       <c r="O87" s="61"/>
@@ -5682,7 +5826,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>DropDownValues!$G$2:$G$4</xm:f>
@@ -5733,19 +5877,19 @@
       <selection activeCell="F15" sqref="F15:O52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="88.7109375" customWidth="1"/>
+    <col min="5" max="5" width="88.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:21">
       <c r="B2" s="28" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" ht="12.75" customHeight="1">
       <c r="B3" s="62" t="s">
         <v>188</v>
       </c>
@@ -5769,7 +5913,7 @@
       <c r="T3" s="62"/>
       <c r="U3" s="62"/>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21">
       <c r="B4" s="62"/>
       <c r="C4" s="62"/>
       <c r="D4" s="62"/>
@@ -5791,7 +5935,7 @@
       <c r="T4" s="62"/>
       <c r="U4" s="62"/>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:21">
       <c r="B5" s="62"/>
       <c r="C5" s="62"/>
       <c r="D5" s="62"/>
@@ -5813,7 +5957,7 @@
       <c r="T5" s="62"/>
       <c r="U5" s="62"/>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:21">
       <c r="B6" s="62"/>
       <c r="C6" s="62"/>
       <c r="D6" s="62"/>
@@ -5835,7 +5979,7 @@
       <c r="T6" s="62"/>
       <c r="U6" s="62"/>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:21">
       <c r="B7" s="62"/>
       <c r="C7" s="62"/>
       <c r="D7" s="62"/>
@@ -5857,7 +6001,7 @@
       <c r="T7" s="62"/>
       <c r="U7" s="62"/>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:21">
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
       <c r="D8" s="62"/>
@@ -5879,7 +6023,7 @@
       <c r="T8" s="62"/>
       <c r="U8" s="62"/>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:21">
       <c r="B9" s="62"/>
       <c r="C9" s="62"/>
       <c r="D9" s="62"/>
@@ -5901,7 +6045,7 @@
       <c r="T9" s="62"/>
       <c r="U9" s="62"/>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:21">
       <c r="B10" s="62"/>
       <c r="C10" s="62"/>
       <c r="D10" s="62"/>
@@ -5923,7 +6067,7 @@
       <c r="T10" s="62"/>
       <c r="U10" s="62"/>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:21">
       <c r="B11" s="62"/>
       <c r="C11" s="62"/>
       <c r="D11" s="62"/>
@@ -5945,7 +6089,7 @@
       <c r="T11" s="62"/>
       <c r="U11" s="62"/>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:21">
       <c r="B12" s="62"/>
       <c r="C12" s="62"/>
       <c r="D12" s="62"/>
@@ -5967,7 +6111,7 @@
       <c r="T12" s="62"/>
       <c r="U12" s="62"/>
     </row>
-    <row r="15" spans="2:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:21" ht="12.75" customHeight="1">
       <c r="B15" t="s">
         <v>189</v>
       </c>
@@ -5984,7 +6128,7 @@
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21">
       <c r="F16" s="61"/>
       <c r="G16" s="61"/>
       <c r="H16" s="61"/>
@@ -5996,7 +6140,7 @@
       <c r="N16" s="61"/>
       <c r="O16" s="61"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15">
       <c r="F17" s="61"/>
       <c r="G17" s="61"/>
       <c r="H17" s="61"/>
@@ -6008,7 +6152,7 @@
       <c r="N17" s="61"/>
       <c r="O17" s="61"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15">
       <c r="B18" s="28" t="s">
         <v>191</v>
       </c>
@@ -6032,7 +6176,7 @@
       <c r="N18" s="61"/>
       <c r="O18" s="61"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15">
       <c r="B19" t="s">
         <v>193</v>
       </c>
@@ -6056,7 +6200,7 @@
       <c r="N19" s="61"/>
       <c r="O19" s="61"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15">
       <c r="C20" t="s">
         <v>196</v>
       </c>
@@ -6077,7 +6221,7 @@
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15">
       <c r="B21" t="s">
         <v>199</v>
       </c>
@@ -6098,7 +6242,7 @@
       <c r="N21" s="61"/>
       <c r="O21" s="61"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15">
       <c r="C22" t="s">
         <v>61</v>
       </c>
@@ -6119,7 +6263,7 @@
       <c r="N22" s="61"/>
       <c r="O22" s="61"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15">
       <c r="B23" t="s">
         <v>203</v>
       </c>
@@ -6137,7 +6281,7 @@
       <c r="N23" s="61"/>
       <c r="O23" s="61"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15">
       <c r="F24" s="61"/>
       <c r="G24" s="61"/>
       <c r="H24" s="61"/>
@@ -6149,7 +6293,7 @@
       <c r="N24" s="61"/>
       <c r="O24" s="61"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15">
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
       <c r="H25" s="61"/>
@@ -6161,7 +6305,7 @@
       <c r="N25" s="61"/>
       <c r="O25" s="61"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15">
       <c r="F26" s="61"/>
       <c r="G26" s="61"/>
       <c r="H26" s="61"/>
@@ -6173,7 +6317,7 @@
       <c r="N26" s="61"/>
       <c r="O26" s="61"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15">
       <c r="F27" s="61"/>
       <c r="G27" s="61"/>
       <c r="H27" s="61"/>
@@ -6185,7 +6329,7 @@
       <c r="N27" s="61"/>
       <c r="O27" s="61"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15">
       <c r="F28" s="61"/>
       <c r="G28" s="61"/>
       <c r="H28" s="61"/>
@@ -6197,7 +6341,7 @@
       <c r="N28" s="61"/>
       <c r="O28" s="61"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15">
       <c r="F29" s="61"/>
       <c r="G29" s="61"/>
       <c r="H29" s="61"/>
@@ -6209,7 +6353,7 @@
       <c r="N29" s="61"/>
       <c r="O29" s="61"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15">
       <c r="F30" s="61"/>
       <c r="G30" s="61"/>
       <c r="H30" s="61"/>
@@ -6221,7 +6365,7 @@
       <c r="N30" s="61"/>
       <c r="O30" s="61"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15">
       <c r="F31" s="61"/>
       <c r="G31" s="61"/>
       <c r="H31" s="61"/>
@@ -6233,7 +6377,7 @@
       <c r="N31" s="61"/>
       <c r="O31" s="61"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15">
       <c r="F32" s="61"/>
       <c r="G32" s="61"/>
       <c r="H32" s="61"/>
@@ -6245,7 +6389,7 @@
       <c r="N32" s="61"/>
       <c r="O32" s="61"/>
     </row>
-    <row r="33" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:15">
       <c r="F33" s="61"/>
       <c r="G33" s="61"/>
       <c r="H33" s="61"/>
@@ -6257,7 +6401,7 @@
       <c r="N33" s="61"/>
       <c r="O33" s="61"/>
     </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:15">
       <c r="F34" s="61"/>
       <c r="G34" s="61"/>
       <c r="H34" s="61"/>
@@ -6269,7 +6413,7 @@
       <c r="N34" s="61"/>
       <c r="O34" s="61"/>
     </row>
-    <row r="35" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:15">
       <c r="F35" s="61"/>
       <c r="G35" s="61"/>
       <c r="H35" s="61"/>
@@ -6281,7 +6425,7 @@
       <c r="N35" s="61"/>
       <c r="O35" s="61"/>
     </row>
-    <row r="36" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:15">
       <c r="F36" s="61"/>
       <c r="G36" s="61"/>
       <c r="H36" s="61"/>
@@ -6293,7 +6437,7 @@
       <c r="N36" s="61"/>
       <c r="O36" s="61"/>
     </row>
-    <row r="37" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:15">
       <c r="F37" s="61"/>
       <c r="G37" s="61"/>
       <c r="H37" s="61"/>
@@ -6305,7 +6449,7 @@
       <c r="N37" s="61"/>
       <c r="O37" s="61"/>
     </row>
-    <row r="38" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:15">
       <c r="F38" s="61"/>
       <c r="G38" s="61"/>
       <c r="H38" s="61"/>
@@ -6317,7 +6461,7 @@
       <c r="N38" s="61"/>
       <c r="O38" s="61"/>
     </row>
-    <row r="39" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:15">
       <c r="F39" s="61"/>
       <c r="G39" s="61"/>
       <c r="H39" s="61"/>
@@ -6329,7 +6473,7 @@
       <c r="N39" s="61"/>
       <c r="O39" s="61"/>
     </row>
-    <row r="40" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:15">
       <c r="F40" s="61"/>
       <c r="G40" s="61"/>
       <c r="H40" s="61"/>
@@ -6341,7 +6485,7 @@
       <c r="N40" s="61"/>
       <c r="O40" s="61"/>
     </row>
-    <row r="41" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:15">
       <c r="F41" s="61"/>
       <c r="G41" s="61"/>
       <c r="H41" s="61"/>
@@ -6353,7 +6497,7 @@
       <c r="N41" s="61"/>
       <c r="O41" s="61"/>
     </row>
-    <row r="42" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:15">
       <c r="F42" s="61"/>
       <c r="G42" s="61"/>
       <c r="H42" s="61"/>
@@ -6365,7 +6509,7 @@
       <c r="N42" s="61"/>
       <c r="O42" s="61"/>
     </row>
-    <row r="43" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:15">
       <c r="F43" s="61"/>
       <c r="G43" s="61"/>
       <c r="H43" s="61"/>
@@ -6377,7 +6521,7 @@
       <c r="N43" s="61"/>
       <c r="O43" s="61"/>
     </row>
-    <row r="44" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:15">
       <c r="F44" s="61"/>
       <c r="G44" s="61"/>
       <c r="H44" s="61"/>
@@ -6389,7 +6533,7 @@
       <c r="N44" s="61"/>
       <c r="O44" s="61"/>
     </row>
-    <row r="45" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:15">
       <c r="F45" s="61"/>
       <c r="G45" s="61"/>
       <c r="H45" s="61"/>
@@ -6401,7 +6545,7 @@
       <c r="N45" s="61"/>
       <c r="O45" s="61"/>
     </row>
-    <row r="46" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:15">
       <c r="F46" s="61"/>
       <c r="G46" s="61"/>
       <c r="H46" s="61"/>
@@ -6413,7 +6557,7 @@
       <c r="N46" s="61"/>
       <c r="O46" s="61"/>
     </row>
-    <row r="47" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:15">
       <c r="F47" s="61"/>
       <c r="G47" s="61"/>
       <c r="H47" s="61"/>
@@ -6425,7 +6569,7 @@
       <c r="N47" s="61"/>
       <c r="O47" s="61"/>
     </row>
-    <row r="48" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="6:15">
       <c r="F48" s="61"/>
       <c r="G48" s="61"/>
       <c r="H48" s="61"/>
@@ -6437,7 +6581,7 @@
       <c r="N48" s="61"/>
       <c r="O48" s="61"/>
     </row>
-    <row r="49" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:15">
       <c r="F49" s="61"/>
       <c r="G49" s="61"/>
       <c r="H49" s="61"/>
@@ -6449,7 +6593,7 @@
       <c r="N49" s="61"/>
       <c r="O49" s="61"/>
     </row>
-    <row r="50" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:15">
       <c r="F50" s="61"/>
       <c r="G50" s="61"/>
       <c r="H50" s="61"/>
@@ -6461,7 +6605,7 @@
       <c r="N50" s="61"/>
       <c r="O50" s="61"/>
     </row>
-    <row r="51" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:15">
       <c r="F51" s="61"/>
       <c r="G51" s="61"/>
       <c r="H51" s="61"/>
@@ -6473,7 +6617,7 @@
       <c r="N51" s="61"/>
       <c r="O51" s="61"/>
     </row>
-    <row r="52" spans="6:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:15">
       <c r="F52" s="61"/>
       <c r="G52" s="61"/>
       <c r="H52" s="61"/>
@@ -6503,21 +6647,21 @@
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="33.1640625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -6552,7 +6696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="46" t="s">
         <v>205</v>
       </c>
@@ -6567,7 +6711,7 @@
       <c r="J2" s="40"/>
       <c r="K2" s="40"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="46">
         <v>1</v>
       </c>
@@ -6594,7 +6738,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="46">
         <v>2</v>
       </c>
@@ -6621,7 +6765,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="46">
         <v>3</v>
       </c>
@@ -6642,7 +6786,7 @@
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="46">
         <v>4</v>
       </c>
@@ -6663,7 +6807,7 @@
       <c r="J6" s="34"/>
       <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="46">
         <v>5</v>
       </c>
@@ -6684,7 +6828,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="34"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="C8" s="34" t="s">
         <v>73</v>
       </c>
@@ -6695,7 +6839,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="C9" s="34" t="s">
         <v>78</v>
       </c>
@@ -6703,7 +6847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="C10" s="10" t="s">
         <v>84</v>
       </c>
@@ -6711,7 +6855,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="C11" s="10" t="s">
         <v>89</v>
       </c>
@@ -6719,7 +6863,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="C12" s="10" t="s">
         <v>93</v>
       </c>
@@ -6727,7 +6871,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="C13" s="10" t="s">
         <v>97</v>
       </c>
@@ -6735,7 +6879,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="C14" s="10" t="s">
         <v>97</v>
       </c>
@@ -6743,7 +6887,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="C15" s="10" t="s">
         <v>101</v>
       </c>
@@ -6751,7 +6895,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="C16" s="10" t="s">
         <v>105</v>
       </c>
@@ -6759,7 +6903,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5">
       <c r="C17" s="10" t="s">
         <v>108</v>
       </c>
@@ -6767,7 +6911,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5">
       <c r="C18" s="10" t="s">
         <v>112</v>
       </c>
@@ -6775,7 +6919,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:5">
       <c r="C19" s="10" t="s">
         <v>61</v>
       </c>
@@ -6783,7 +6927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:5">
       <c r="C20" s="10" t="s">
         <v>121</v>
       </c>
@@ -6791,7 +6935,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:5">
       <c r="C21" s="10" t="s">
         <v>124</v>
       </c>
@@ -6799,7 +6943,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:5">
       <c r="C22" s="10" t="s">
         <v>127</v>
       </c>
@@ -6807,7 +6951,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:5">
       <c r="C23" s="10" t="s">
         <v>131</v>
       </c>
@@ -6815,7 +6959,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:5">
       <c r="C24" s="10" t="s">
         <v>134</v>
       </c>
@@ -6823,7 +6967,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:5">
       <c r="C25" s="10" t="s">
         <v>139</v>
       </c>
@@ -6831,7 +6975,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:5">
       <c r="C26" s="10" t="s">
         <v>143</v>
       </c>
@@ -6839,7 +6983,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:5">
       <c r="C27" s="10" t="s">
         <v>149</v>
       </c>
@@ -6847,7 +6991,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:5">
       <c r="C28" s="10" t="s">
         <v>152</v>
       </c>
@@ -6855,7 +6999,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:5">
       <c r="C29" s="10" t="s">
         <v>156</v>
       </c>
@@ -6863,7 +7007,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:5">
       <c r="C30" s="10" t="s">
         <v>158</v>
       </c>
@@ -6871,7 +7015,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:5">
       <c r="C31" s="10" t="s">
         <v>159</v>
       </c>
@@ -6879,7 +7023,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:5">
       <c r="C32" s="10" t="s">
         <v>235</v>
       </c>
@@ -6887,7 +7031,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:5">
       <c r="C33" s="10" t="s">
         <v>166</v>
       </c>
@@ -6895,7 +7039,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:5">
       <c r="C34" s="10" t="s">
         <v>167</v>
       </c>
@@ -6903,7 +7047,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:5">
       <c r="C35" s="10" t="s">
         <v>168</v>
       </c>
@@ -6911,7 +7055,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:5">
       <c r="C36" s="10" t="s">
         <v>173</v>
       </c>
@@ -6919,7 +7063,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:5">
       <c r="C37" s="10" t="s">
         <v>177</v>
       </c>
@@ -6927,7 +7071,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:5">
       <c r="C38" s="10" t="s">
         <v>181</v>
       </c>
@@ -6935,7 +7079,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:5">
       <c r="C39" s="10" t="s">
         <v>184</v>
       </c>
@@ -6943,557 +7087,557 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:5">
       <c r="E40" s="10" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:5">
       <c r="E41" s="10" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:5">
       <c r="E42" s="10" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:5">
       <c r="E43" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:5">
       <c r="E44" s="10" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:5">
       <c r="E45" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:5">
       <c r="E46" s="10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:5">
       <c r="E47" s="10" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:5">
       <c r="E48" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5">
       <c r="E49" s="10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:5">
       <c r="E50" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:5">
       <c r="E51" s="10" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:5">
       <c r="E52" s="10" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:5">
       <c r="E53" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:5">
       <c r="E54" s="10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:5">
       <c r="E55" s="10" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:5">
       <c r="E56" s="10" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:5">
       <c r="E57" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:5">
       <c r="E58" s="10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:5">
       <c r="E59" s="10" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:5">
       <c r="E60" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:5">
       <c r="E61" s="10" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:5">
       <c r="E62" s="10" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:5">
       <c r="E63" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:5">
       <c r="E64" s="10" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:5">
       <c r="E65" s="10" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:5">
       <c r="E66" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:5">
       <c r="E67" s="10" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:5">
       <c r="E68" s="10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:5">
       <c r="E69" s="10" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:5">
       <c r="E70" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:5">
       <c r="E71" s="10" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:5">
       <c r="E72" s="10" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:5">
       <c r="E73" s="10" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:5">
       <c r="E74" s="10" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:5">
       <c r="E75" s="10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="5:5">
       <c r="E76" s="10" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="5:5">
       <c r="E77" s="10" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="5:5">
       <c r="E78" s="10" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="5:5">
       <c r="E79" s="10" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:5">
       <c r="E80" s="10" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="5:5">
       <c r="E81" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="5:5">
       <c r="E82" s="10" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="5:5">
       <c r="E83" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="5:5">
       <c r="E84" s="10" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="5:5">
       <c r="E85" s="10" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="5:5">
       <c r="E86" s="10" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="5:5">
       <c r="E87" s="10" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="5:5">
       <c r="E88" s="10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="5:5">
       <c r="E89" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="5:5">
       <c r="E90" s="10" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="5:5">
       <c r="E91" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="5:5">
       <c r="E92" s="10" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="5:5">
       <c r="E93" s="10" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="5:5">
       <c r="E94" s="10" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="5:5">
       <c r="E95" s="10" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="5:5">
       <c r="E96" s="10" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:5">
       <c r="E97" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:5">
       <c r="E98" s="10" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:5">
       <c r="E99" s="10" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:5">
       <c r="E100" s="10" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:5">
       <c r="E101" s="10" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:5">
       <c r="E102" s="10" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:5">
       <c r="E103" s="10" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:5">
       <c r="E104" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:5">
       <c r="E105" s="10" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:5">
       <c r="E106" s="10" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:5">
       <c r="E107" s="10" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:5">
       <c r="E108" s="10" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:5">
       <c r="E109" s="10" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="5:5">
       <c r="E110" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="5:5">
       <c r="E111" s="10" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="5:5">
       <c r="E112" s="10" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:5">
       <c r="E113" s="10" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:5">
       <c r="E114" s="10" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:5">
       <c r="E115" s="10" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:5">
       <c r="E116" s="10" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:5">
       <c r="E117" s="10" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="5:5">
       <c r="E118" s="10" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="5:5">
       <c r="E119" s="10" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="5:5">
       <c r="E120" s="10" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="5:5">
       <c r="E121" s="10" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="5:5">
       <c r="E122" s="10" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="5:5">
       <c r="E123" s="10" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="5:5">
       <c r="E124" s="10" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="5:5">
       <c r="E125" s="10" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="5:5">
       <c r="E126" s="10" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="5:5">
       <c r="E127" s="10" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="5:5">
       <c r="E128" s="10" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="5:5">
       <c r="E129" s="10" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="5:5">
       <c r="E130" s="10" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="5:5">
       <c r="E131" s="10" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="5:5">
       <c r="E132" s="10" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="5:5">
       <c r="E133" s="10" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="5:5">
       <c r="E134" s="10" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="5:5">
       <c r="E135" s="10" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="5:5">
       <c r="E136" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="5:5">
       <c r="E137" s="10" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="5:5">
       <c r="E138" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="5:5">
       <c r="E139" s="10" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="5:5">
       <c r="E140" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="5:5">
       <c r="E141" s="10" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="5:5">
       <c r="E142" s="10" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="5:5">
       <c r="E143" s="10" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="5:5">
       <c r="E144" s="10" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="5:5">
       <c r="E145" s="10" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="5:5">
       <c r="E146" s="10" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="5:5">
       <c r="E147" s="10" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="5:5">
       <c r="E148" s="10" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="5:5">
       <c r="E149" s="10" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="5:5">
       <c r="E150" s="10" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Some upgrades here. Nearly finished adding data fitting routnes as an option for the generic plotting tool. Added second derivitives support with respect to time for same tool.
</commit_message>
<xml_diff>
--- a/Generic_Macro/Control.xlsx
+++ b/Generic_Macro/Control.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/TempVenv/Plebs_Macro/Generic_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2AE56F-AEFF-F94F-8EB6-B38385DC70C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E20BE-6529-4C4E-8CA4-E0BFD6DC7803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="389">
   <si>
     <t>Index</t>
   </si>
@@ -1322,16 +1322,58 @@
     <t>Global M2 (top 50)</t>
   </si>
   <si>
-    <t xml:space="preserve">Monetary Aggregates &amp; CPI. </t>
-  </si>
-  <si>
-    <t>CPI</t>
-  </si>
-  <si>
-    <t>CPI YoY % change</t>
-  </si>
-  <si>
-    <t>1994-01-01</t>
+    <t>YoY of Yoy, i.e YoY^2</t>
+  </si>
+  <si>
+    <t>YoY^2 % change</t>
+  </si>
+  <si>
+    <t>YoY % Change</t>
+  </si>
+  <si>
+    <t>btcyoy</t>
+  </si>
+  <si>
+    <t>btcyoy2</t>
+  </si>
+  <si>
+    <t>BTC (USD)</t>
+  </si>
+  <si>
+    <t>BTC_USD YoY % change</t>
+  </si>
+  <si>
+    <t>BTC_USD YoY % change 2nd derivative</t>
+  </si>
+  <si>
+    <t>Add_MA</t>
+  </si>
+  <si>
+    <t>1959-01-01</t>
+  </si>
+  <si>
+    <t>cpi</t>
+  </si>
+  <si>
+    <t>cpi1</t>
+  </si>
+  <si>
+    <t>cpi2</t>
+  </si>
+  <si>
+    <t>US CPI - YoY % change</t>
+  </si>
+  <si>
+    <t>US CPI - YoY % change 2nd derivative</t>
+  </si>
+  <si>
+    <t>index (a.u)</t>
+  </si>
+  <si>
+    <t>US CPI, first and second 12 month derivatives.</t>
+  </si>
+  <si>
+    <t>75</t>
   </si>
 </sst>
 </file>
@@ -1727,6 +1769,9 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1747,9 +1792,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2133,10 +2175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -2152,9 +2194,10 @@
     <col min="13" max="13" width="15.5" customWidth="1"/>
     <col min="14" max="14" width="18.83203125" customWidth="1"/>
     <col min="15" max="15" width="18.5" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18">
+    <row r="1" spans="1:16" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2192,58 +2235,62 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18">
+    <row r="2" spans="1:16" ht="18">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>16</v>
+        <v>145</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>65</v>
+        <v>381</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>366</v>
+        <v>133</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>367</v>
+        <v>386</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="18">
+      <c r="N2" s="8"/>
+      <c r="O2" s="9">
+        <v>2</v>
+      </c>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:16" ht="18">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>15</v>
@@ -2252,142 +2299,109 @@
         <v>16</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="J3" s="5" t="s">
+        <v>388</v>
+      </c>
       <c r="K3" s="5"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="18">
+      <c r="N3" s="8"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="8"/>
+    </row>
+    <row r="4" spans="1:16" ht="18">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>360</v>
+        <v>125</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>16</v>
+        <v>371</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>365</v>
+        <v>383</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>361</v>
+        <v>385</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="J4" s="5"/>
+        <v>372</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>388</v>
+      </c>
       <c r="K4" s="5"/>
       <c r="L4" s="7"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="8">
-        <f>10^12</f>
-        <v>1000000000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="18">
+      <c r="N4" s="8"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" spans="1:16" ht="18">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>367</v>
-      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="8">
-        <f>10^12</f>
-        <v>1000000000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="18">
+      <c r="N5" s="8"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="1:16" ht="18">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>367</v>
-      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="63">
-        <f>10^12</f>
-        <v>1000000000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="16">
+      <c r="N6" s="8"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="56"/>
+    </row>
+    <row r="7" spans="1:16" ht="16">
       <c r="A7" s="12"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -2402,17 +2416,17 @@
       <c r="L7" s="14"/>
       <c r="O7" s="15"/>
     </row>
-    <row r="8" spans="1:15" ht="16">
+    <row r="8" spans="1:16" ht="16">
       <c r="A8" s="16" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>374</v>
-      </c>
-      <c r="C8" s="56" t="s">
+        <v>380</v>
+      </c>
+      <c r="C8" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="56"/>
+      <c r="D8" s="57"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
@@ -2422,16 +2436,16 @@
       <c r="K8" s="18"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:15" ht="16">
+    <row r="9" spans="1:16" ht="16">
       <c r="A9" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="17"/>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
       <c r="H9" s="18"/>
@@ -2440,7 +2454,7 @@
       <c r="K9" s="18"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:15" ht="16">
+    <row r="10" spans="1:16" ht="16">
       <c r="A10" s="13"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -2454,15 +2468,15 @@
       <c r="K10" s="18"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:15" ht="16">
+    <row r="11" spans="1:16" ht="16">
       <c r="A11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
@@ -2472,17 +2486,17 @@
       <c r="K11" s="18"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:15" ht="16">
+    <row r="12" spans="1:16" ht="16">
       <c r="A12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="59" t="s">
-        <v>371</v>
-      </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
+      <c r="B12" s="60" t="s">
+        <v>387</v>
+      </c>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
@@ -2490,7 +2504,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="1:15" ht="16">
+    <row r="13" spans="1:16" ht="16">
       <c r="A13" s="21" t="s">
         <v>38</v>
       </c>
@@ -2508,7 +2522,7 @@
       <c r="K13" s="18"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="1:15" ht="16">
+    <row r="14" spans="1:16" ht="16">
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -2520,7 +2534,7 @@
       <c r="K14" s="18"/>
       <c r="L14" s="19"/>
     </row>
-    <row r="15" spans="1:15" ht="16">
+    <row r="15" spans="1:16" ht="16">
       <c r="A15" s="21" t="s">
         <v>353</v>
       </c>
@@ -2538,7 +2552,7 @@
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="1:15" ht="16">
+    <row r="16" spans="1:16" ht="16">
       <c r="A16" s="51" t="s">
         <v>355</v>
       </c>
@@ -2734,7 +2748,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>DropDownValues!$D$2:$D$8</xm:f>
@@ -2742,7 +2756,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D25 D2:D6</xm:sqref>
+          <xm:sqref>D25</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -2780,6 +2794,12 @@
           </x14:formula2>
           <xm:sqref>L2:L6</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{64C6ABE8-DCB4-414D-B37D-679EAFCE6B33}">
+          <x14:formula1>
+            <xm:f>DropDownValues!$D$2:$D$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D6</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2790,8 +2810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB87"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B60:I62"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="B24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -4409,13 +4429,13 @@
       <c r="J43" s="10"/>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
-      <c r="M43" s="60" t="s">
+      <c r="M43" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="N43" s="60"/>
-      <c r="O43" s="60"/>
-      <c r="P43" s="60"/>
-      <c r="Q43" s="60"/>
+      <c r="N43" s="61"/>
+      <c r="O43" s="61"/>
+      <c r="P43" s="61"/>
+      <c r="Q43" s="61"/>
       <c r="R43" s="43"/>
       <c r="S43" s="43"/>
       <c r="T43" s="43"/>
@@ -4450,13 +4470,13 @@
       <c r="J44" s="10"/>
       <c r="K44" s="15"/>
       <c r="L44" s="15"/>
-      <c r="M44" s="61" t="s">
+      <c r="M44" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="N44" s="61"/>
-      <c r="O44" s="61"/>
-      <c r="P44" s="61"/>
-      <c r="Q44" s="61"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="62"/>
       <c r="R44" s="43"/>
       <c r="S44" s="43"/>
       <c r="T44" s="43"/>
@@ -4491,11 +4511,11 @@
       <c r="J45" s="10"/>
       <c r="K45" s="15"/>
       <c r="L45" s="15"/>
-      <c r="M45" s="61"/>
-      <c r="N45" s="61"/>
-      <c r="O45" s="61"/>
-      <c r="P45" s="61"/>
-      <c r="Q45" s="61"/>
+      <c r="M45" s="62"/>
+      <c r="N45" s="62"/>
+      <c r="O45" s="62"/>
+      <c r="P45" s="62"/>
+      <c r="Q45" s="62"/>
       <c r="R45" s="43"/>
       <c r="S45" s="43"/>
       <c r="T45" s="43"/>
@@ -4530,11 +4550,11 @@
       <c r="J46" s="10"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
-      <c r="M46" s="61"/>
-      <c r="N46" s="61"/>
-      <c r="O46" s="61"/>
-      <c r="P46" s="61"/>
-      <c r="Q46" s="61"/>
+      <c r="M46" s="62"/>
+      <c r="N46" s="62"/>
+      <c r="O46" s="62"/>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="62"/>
       <c r="R46" s="43"/>
       <c r="S46" s="43"/>
       <c r="T46" s="43"/>
@@ -4569,11 +4589,11 @@
       <c r="J47" s="10"/>
       <c r="K47" s="15"/>
       <c r="L47" s="15"/>
-      <c r="M47" s="61"/>
-      <c r="N47" s="61"/>
-      <c r="O47" s="61"/>
-      <c r="P47" s="61"/>
-      <c r="Q47" s="61"/>
+      <c r="M47" s="62"/>
+      <c r="N47" s="62"/>
+      <c r="O47" s="62"/>
+      <c r="P47" s="62"/>
+      <c r="Q47" s="62"/>
       <c r="R47" s="43"/>
       <c r="S47" s="43"/>
       <c r="T47" s="43"/>
@@ -4600,11 +4620,11 @@
       <c r="J48" s="10"/>
       <c r="K48" s="15"/>
       <c r="L48" s="15"/>
-      <c r="M48" s="61"/>
-      <c r="N48" s="61"/>
-      <c r="O48" s="61"/>
-      <c r="P48" s="61"/>
-      <c r="Q48" s="61"/>
+      <c r="M48" s="62"/>
+      <c r="N48" s="62"/>
+      <c r="O48" s="62"/>
+      <c r="P48" s="62"/>
+      <c r="Q48" s="62"/>
       <c r="R48" s="43"/>
       <c r="S48" s="43"/>
       <c r="T48" s="43"/>
@@ -4645,11 +4665,11 @@
       <c r="J49" s="10"/>
       <c r="K49" s="15"/>
       <c r="L49" s="15"/>
-      <c r="M49" s="61"/>
-      <c r="N49" s="61"/>
-      <c r="O49" s="61"/>
-      <c r="P49" s="61"/>
-      <c r="Q49" s="61"/>
+      <c r="M49" s="62"/>
+      <c r="N49" s="62"/>
+      <c r="O49" s="62"/>
+      <c r="P49" s="62"/>
+      <c r="Q49" s="62"/>
       <c r="R49" s="43"/>
       <c r="S49" s="43"/>
       <c r="T49" s="43"/>
@@ -4680,11 +4700,11 @@
       <c r="J50" s="10"/>
       <c r="K50" s="15"/>
       <c r="L50" s="15"/>
-      <c r="M50" s="61"/>
-      <c r="N50" s="61"/>
-      <c r="O50" s="61"/>
-      <c r="P50" s="61"/>
-      <c r="Q50" s="61"/>
+      <c r="M50" s="62"/>
+      <c r="N50" s="62"/>
+      <c r="O50" s="62"/>
+      <c r="P50" s="62"/>
+      <c r="Q50" s="62"/>
       <c r="R50" s="43"/>
       <c r="S50" s="43"/>
       <c r="T50" s="43"/>
@@ -4715,11 +4735,11 @@
       <c r="J51" s="10"/>
       <c r="K51" s="15"/>
       <c r="L51" s="15"/>
-      <c r="M51" s="61"/>
-      <c r="N51" s="61"/>
-      <c r="O51" s="61"/>
-      <c r="P51" s="61"/>
-      <c r="Q51" s="61"/>
+      <c r="M51" s="62"/>
+      <c r="N51" s="62"/>
+      <c r="O51" s="62"/>
+      <c r="P51" s="62"/>
+      <c r="Q51" s="62"/>
       <c r="R51" s="43"/>
       <c r="S51" s="43"/>
       <c r="T51" s="43"/>
@@ -4762,11 +4782,11 @@
       </c>
       <c r="K52" s="15"/>
       <c r="L52" s="15"/>
-      <c r="M52" s="61"/>
-      <c r="N52" s="61"/>
-      <c r="O52" s="61"/>
-      <c r="P52" s="61"/>
-      <c r="Q52" s="61"/>
+      <c r="M52" s="62"/>
+      <c r="N52" s="62"/>
+      <c r="O52" s="62"/>
+      <c r="P52" s="62"/>
+      <c r="Q52" s="62"/>
       <c r="R52" s="43"/>
       <c r="S52" s="43"/>
       <c r="T52" s="43"/>
@@ -4809,11 +4829,11 @@
       </c>
       <c r="K53" s="15"/>
       <c r="L53" s="15"/>
-      <c r="M53" s="61"/>
-      <c r="N53" s="61"/>
-      <c r="O53" s="61"/>
-      <c r="P53" s="61"/>
-      <c r="Q53" s="61"/>
+      <c r="M53" s="62"/>
+      <c r="N53" s="62"/>
+      <c r="O53" s="62"/>
+      <c r="P53" s="62"/>
+      <c r="Q53" s="62"/>
       <c r="R53" s="43"/>
       <c r="S53" s="43"/>
       <c r="T53" s="43"/>
@@ -4857,11 +4877,11 @@
       </c>
       <c r="K54" s="15"/>
       <c r="L54" s="15"/>
-      <c r="M54" s="61"/>
-      <c r="N54" s="61"/>
-      <c r="O54" s="61"/>
-      <c r="P54" s="61"/>
-      <c r="Q54" s="61"/>
+      <c r="M54" s="62"/>
+      <c r="N54" s="62"/>
+      <c r="O54" s="62"/>
+      <c r="P54" s="62"/>
+      <c r="Q54" s="62"/>
       <c r="R54" s="43"/>
       <c r="S54" s="43"/>
       <c r="T54" s="43"/>
@@ -4902,11 +4922,11 @@
       <c r="J55" s="10"/>
       <c r="K55" s="15"/>
       <c r="L55" s="15"/>
-      <c r="M55" s="61"/>
-      <c r="N55" s="61"/>
-      <c r="O55" s="61"/>
-      <c r="P55" s="61"/>
-      <c r="Q55" s="61"/>
+      <c r="M55" s="62"/>
+      <c r="N55" s="62"/>
+      <c r="O55" s="62"/>
+      <c r="P55" s="62"/>
+      <c r="Q55" s="62"/>
       <c r="R55" s="43"/>
       <c r="S55" s="43"/>
       <c r="T55" s="43"/>
@@ -4947,11 +4967,11 @@
       <c r="J56" s="10"/>
       <c r="K56" s="15"/>
       <c r="L56" s="15"/>
-      <c r="M56" s="61"/>
-      <c r="N56" s="61"/>
-      <c r="O56" s="61"/>
-      <c r="P56" s="61"/>
-      <c r="Q56" s="61"/>
+      <c r="M56" s="62"/>
+      <c r="N56" s="62"/>
+      <c r="O56" s="62"/>
+      <c r="P56" s="62"/>
+      <c r="Q56" s="62"/>
       <c r="R56" s="43"/>
       <c r="S56" s="43"/>
       <c r="T56" s="43"/>
@@ -4990,11 +5010,11 @@
       <c r="J57" s="10"/>
       <c r="K57" s="15"/>
       <c r="L57" s="15"/>
-      <c r="M57" s="61"/>
-      <c r="N57" s="61"/>
-      <c r="O57" s="61"/>
-      <c r="P57" s="61"/>
-      <c r="Q57" s="61"/>
+      <c r="M57" s="62"/>
+      <c r="N57" s="62"/>
+      <c r="O57" s="62"/>
+      <c r="P57" s="62"/>
+      <c r="Q57" s="62"/>
       <c r="R57" s="43"/>
       <c r="S57" s="43"/>
       <c r="T57" s="43"/>
@@ -5035,11 +5055,11 @@
       <c r="J58" s="10"/>
       <c r="K58" s="15"/>
       <c r="L58" s="15"/>
-      <c r="M58" s="61"/>
-      <c r="N58" s="61"/>
-      <c r="O58" s="61"/>
-      <c r="P58" s="61"/>
-      <c r="Q58" s="61"/>
+      <c r="M58" s="62"/>
+      <c r="N58" s="62"/>
+      <c r="O58" s="62"/>
+      <c r="P58" s="62"/>
+      <c r="Q58" s="62"/>
       <c r="R58" s="43"/>
       <c r="S58" s="43"/>
       <c r="T58" s="43"/>
@@ -5078,11 +5098,11 @@
       <c r="J59" s="10"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
-      <c r="M59" s="61"/>
-      <c r="N59" s="61"/>
-      <c r="O59" s="61"/>
-      <c r="P59" s="61"/>
-      <c r="Q59" s="61"/>
+      <c r="M59" s="62"/>
+      <c r="N59" s="62"/>
+      <c r="O59" s="62"/>
+      <c r="P59" s="62"/>
+      <c r="Q59" s="62"/>
       <c r="R59" s="43"/>
       <c r="S59" s="43"/>
       <c r="T59" s="43"/>
@@ -5123,11 +5143,11 @@
       <c r="J60" s="10"/>
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
-      <c r="M60" s="61"/>
-      <c r="N60" s="61"/>
-      <c r="O60" s="61"/>
-      <c r="P60" s="61"/>
-      <c r="Q60" s="61"/>
+      <c r="M60" s="62"/>
+      <c r="N60" s="62"/>
+      <c r="O60" s="62"/>
+      <c r="P60" s="62"/>
+      <c r="Q60" s="62"/>
       <c r="R60" s="43"/>
       <c r="S60" s="43"/>
       <c r="T60" s="43"/>
@@ -5168,11 +5188,11 @@
       <c r="J61" s="10"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
-      <c r="M61" s="61"/>
-      <c r="N61" s="61"/>
-      <c r="O61" s="61"/>
-      <c r="P61" s="61"/>
-      <c r="Q61" s="61"/>
+      <c r="M61" s="62"/>
+      <c r="N61" s="62"/>
+      <c r="O61" s="62"/>
+      <c r="P61" s="62"/>
+      <c r="Q61" s="62"/>
       <c r="R61" s="43"/>
       <c r="S61" s="43"/>
       <c r="T61" s="43"/>
@@ -5213,11 +5233,11 @@
       <c r="J62" s="10"/>
       <c r="K62" s="15"/>
       <c r="L62" s="15"/>
-      <c r="M62" s="61"/>
-      <c r="N62" s="61"/>
-      <c r="O62" s="61"/>
-      <c r="P62" s="61"/>
-      <c r="Q62" s="61"/>
+      <c r="M62" s="62"/>
+      <c r="N62" s="62"/>
+      <c r="O62" s="62"/>
+      <c r="P62" s="62"/>
+      <c r="Q62" s="62"/>
       <c r="R62" s="43"/>
       <c r="S62" s="43"/>
       <c r="T62" s="43"/>
@@ -5231,22 +5251,38 @@
       <c r="AB62" s="43"/>
     </row>
     <row r="63" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B63" s="10"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
+      <c r="B63" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="J63" s="10"/>
       <c r="K63" s="15"/>
       <c r="L63" s="15"/>
-      <c r="M63" s="61"/>
-      <c r="N63" s="61"/>
-      <c r="O63" s="61"/>
-      <c r="P63" s="61"/>
-      <c r="Q63" s="61"/>
+      <c r="M63" s="62"/>
+      <c r="N63" s="62"/>
+      <c r="O63" s="62"/>
+      <c r="P63" s="62"/>
+      <c r="Q63" s="62"/>
       <c r="R63" s="43"/>
       <c r="S63" s="43"/>
       <c r="T63" s="43"/>
@@ -5260,20 +5296,36 @@
       <c r="AB63" s="43"/>
     </row>
     <row r="64" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B64" s="38"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="38"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
+      <c r="B64" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F64" s="38" t="s">
+        <v>374</v>
+      </c>
+      <c r="G64" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" s="38" t="s">
+        <v>377</v>
+      </c>
+      <c r="I64" s="38" t="s">
+        <v>373</v>
+      </c>
       <c r="J64" s="38"/>
-      <c r="M64" s="61"/>
-      <c r="N64" s="61"/>
-      <c r="O64" s="61"/>
-      <c r="P64" s="61"/>
-      <c r="Q64" s="61"/>
+      <c r="M64" s="62"/>
+      <c r="N64" s="62"/>
+      <c r="O64" s="62"/>
+      <c r="P64" s="62"/>
+      <c r="Q64" s="62"/>
       <c r="R64" s="43"/>
       <c r="S64" s="43"/>
       <c r="T64" s="43"/>
@@ -5287,20 +5339,36 @@
       <c r="AB64" s="43"/>
     </row>
     <row r="65" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B65" s="38"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
-      <c r="F65" s="38"/>
-      <c r="G65" s="38"/>
-      <c r="H65" s="38"/>
-      <c r="I65" s="38"/>
+      <c r="B65" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" s="38" t="s">
+        <v>371</v>
+      </c>
+      <c r="E65" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="F65" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="G65" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="I65" s="38" t="s">
+        <v>372</v>
+      </c>
       <c r="J65" s="38"/>
-      <c r="M65" s="61"/>
-      <c r="N65" s="61"/>
-      <c r="O65" s="61"/>
-      <c r="P65" s="61"/>
-      <c r="Q65" s="61"/>
+      <c r="M65" s="62"/>
+      <c r="N65" s="62"/>
+      <c r="O65" s="62"/>
+      <c r="P65" s="62"/>
+      <c r="Q65" s="62"/>
       <c r="R65" s="43"/>
       <c r="S65" s="43"/>
       <c r="T65" s="43"/>
@@ -5323,11 +5391,11 @@
       <c r="H66" s="38"/>
       <c r="I66" s="38"/>
       <c r="J66" s="38"/>
-      <c r="M66" s="61"/>
-      <c r="N66" s="61"/>
-      <c r="O66" s="61"/>
-      <c r="P66" s="61"/>
-      <c r="Q66" s="61"/>
+      <c r="M66" s="62"/>
+      <c r="N66" s="62"/>
+      <c r="O66" s="62"/>
+      <c r="P66" s="62"/>
+      <c r="Q66" s="62"/>
       <c r="R66" s="43"/>
       <c r="S66" s="43"/>
       <c r="T66" s="43"/>
@@ -5350,11 +5418,11 @@
       <c r="H67" s="38"/>
       <c r="I67" s="38"/>
       <c r="J67" s="38"/>
-      <c r="M67" s="61"/>
-      <c r="N67" s="61"/>
-      <c r="O67" s="61"/>
-      <c r="P67" s="61"/>
-      <c r="Q67" s="61"/>
+      <c r="M67" s="62"/>
+      <c r="N67" s="62"/>
+      <c r="O67" s="62"/>
+      <c r="P67" s="62"/>
+      <c r="Q67" s="62"/>
       <c r="R67" s="43"/>
       <c r="S67" s="43"/>
       <c r="T67" s="43"/>
@@ -5377,11 +5445,11 @@
       <c r="H68" s="38"/>
       <c r="I68" s="38"/>
       <c r="J68" s="38"/>
-      <c r="M68" s="61"/>
-      <c r="N68" s="61"/>
-      <c r="O68" s="61"/>
-      <c r="P68" s="61"/>
-      <c r="Q68" s="61"/>
+      <c r="M68" s="62"/>
+      <c r="N68" s="62"/>
+      <c r="O68" s="62"/>
+      <c r="P68" s="62"/>
+      <c r="Q68" s="62"/>
       <c r="R68" s="43"/>
       <c r="S68" s="43"/>
       <c r="T68" s="43"/>
@@ -5404,11 +5472,11 @@
       <c r="H69" s="38"/>
       <c r="I69" s="38"/>
       <c r="J69" s="38"/>
-      <c r="M69" s="61"/>
-      <c r="N69" s="61"/>
-      <c r="O69" s="61"/>
-      <c r="P69" s="61"/>
-      <c r="Q69" s="61"/>
+      <c r="M69" s="62"/>
+      <c r="N69" s="62"/>
+      <c r="O69" s="62"/>
+      <c r="P69" s="62"/>
+      <c r="Q69" s="62"/>
       <c r="R69" s="43"/>
       <c r="S69" s="43"/>
       <c r="T69" s="43"/>
@@ -5431,11 +5499,11 @@
       <c r="H70" s="38"/>
       <c r="I70" s="38"/>
       <c r="J70" s="38"/>
-      <c r="M70" s="61"/>
-      <c r="N70" s="61"/>
-      <c r="O70" s="61"/>
-      <c r="P70" s="61"/>
-      <c r="Q70" s="61"/>
+      <c r="M70" s="62"/>
+      <c r="N70" s="62"/>
+      <c r="O70" s="62"/>
+      <c r="P70" s="62"/>
+      <c r="Q70" s="62"/>
       <c r="R70" s="43"/>
       <c r="S70" s="43"/>
       <c r="T70" s="43"/>
@@ -5458,11 +5526,11 @@
       <c r="H71" s="38"/>
       <c r="I71" s="38"/>
       <c r="J71" s="38"/>
-      <c r="M71" s="61"/>
-      <c r="N71" s="61"/>
-      <c r="O71" s="61"/>
-      <c r="P71" s="61"/>
-      <c r="Q71" s="61"/>
+      <c r="M71" s="62"/>
+      <c r="N71" s="62"/>
+      <c r="O71" s="62"/>
+      <c r="P71" s="62"/>
+      <c r="Q71" s="62"/>
       <c r="R71" s="43"/>
       <c r="S71" s="43"/>
       <c r="T71" s="43"/>
@@ -5485,11 +5553,11 @@
       <c r="H72" s="38"/>
       <c r="I72" s="38"/>
       <c r="J72" s="38"/>
-      <c r="M72" s="61"/>
-      <c r="N72" s="61"/>
-      <c r="O72" s="61"/>
-      <c r="P72" s="61"/>
-      <c r="Q72" s="61"/>
+      <c r="M72" s="62"/>
+      <c r="N72" s="62"/>
+      <c r="O72" s="62"/>
+      <c r="P72" s="62"/>
+      <c r="Q72" s="62"/>
       <c r="R72" s="43"/>
       <c r="S72" s="43"/>
       <c r="T72" s="43"/>
@@ -5512,11 +5580,11 @@
       <c r="H73" s="38"/>
       <c r="I73" s="38"/>
       <c r="J73" s="38"/>
-      <c r="M73" s="61"/>
-      <c r="N73" s="61"/>
-      <c r="O73" s="61"/>
-      <c r="P73" s="61"/>
-      <c r="Q73" s="61"/>
+      <c r="M73" s="62"/>
+      <c r="N73" s="62"/>
+      <c r="O73" s="62"/>
+      <c r="P73" s="62"/>
+      <c r="Q73" s="62"/>
       <c r="R73" s="43"/>
       <c r="S73" s="43"/>
       <c r="T73" s="43"/>
@@ -5539,11 +5607,11 @@
       <c r="H74" s="38"/>
       <c r="I74" s="38"/>
       <c r="J74" s="38"/>
-      <c r="M74" s="61"/>
-      <c r="N74" s="61"/>
-      <c r="O74" s="61"/>
-      <c r="P74" s="61"/>
-      <c r="Q74" s="61"/>
+      <c r="M74" s="62"/>
+      <c r="N74" s="62"/>
+      <c r="O74" s="62"/>
+      <c r="P74" s="62"/>
+      <c r="Q74" s="62"/>
       <c r="R74" s="43"/>
       <c r="S74" s="43"/>
       <c r="T74" s="43"/>
@@ -5566,11 +5634,11 @@
       <c r="H75" s="35"/>
       <c r="I75" s="35"/>
       <c r="J75" s="35"/>
-      <c r="M75" s="61"/>
-      <c r="N75" s="61"/>
-      <c r="O75" s="61"/>
-      <c r="P75" s="61"/>
-      <c r="Q75" s="61"/>
+      <c r="M75" s="62"/>
+      <c r="N75" s="62"/>
+      <c r="O75" s="62"/>
+      <c r="P75" s="62"/>
+      <c r="Q75" s="62"/>
       <c r="R75" s="43"/>
       <c r="S75" s="43"/>
       <c r="T75" s="43"/>
@@ -5593,11 +5661,11 @@
       <c r="H76" s="35"/>
       <c r="I76" s="35"/>
       <c r="J76" s="35"/>
-      <c r="M76" s="61"/>
-      <c r="N76" s="61"/>
-      <c r="O76" s="61"/>
-      <c r="P76" s="61"/>
-      <c r="Q76" s="61"/>
+      <c r="M76" s="62"/>
+      <c r="N76" s="62"/>
+      <c r="O76" s="62"/>
+      <c r="P76" s="62"/>
+      <c r="Q76" s="62"/>
       <c r="R76" s="43"/>
       <c r="S76" s="43"/>
       <c r="T76" s="43"/>
@@ -5620,11 +5688,11 @@
       <c r="H77" s="35"/>
       <c r="I77" s="35"/>
       <c r="J77" s="35"/>
-      <c r="M77" s="61"/>
-      <c r="N77" s="61"/>
-      <c r="O77" s="61"/>
-      <c r="P77" s="61"/>
-      <c r="Q77" s="61"/>
+      <c r="M77" s="62"/>
+      <c r="N77" s="62"/>
+      <c r="O77" s="62"/>
+      <c r="P77" s="62"/>
+      <c r="Q77" s="62"/>
       <c r="R77" s="43"/>
       <c r="S77" s="43"/>
       <c r="T77" s="43"/>
@@ -5638,11 +5706,11 @@
       <c r="AB77" s="43"/>
     </row>
     <row r="78" spans="2:28" ht="12.75" customHeight="1">
-      <c r="M78" s="61"/>
-      <c r="N78" s="61"/>
-      <c r="O78" s="61"/>
-      <c r="P78" s="61"/>
-      <c r="Q78" s="61"/>
+      <c r="M78" s="62"/>
+      <c r="N78" s="62"/>
+      <c r="O78" s="62"/>
+      <c r="P78" s="62"/>
+      <c r="Q78" s="62"/>
       <c r="R78" s="43"/>
       <c r="S78" s="43"/>
       <c r="T78" s="43"/>
@@ -5656,11 +5724,11 @@
       <c r="AB78" s="43"/>
     </row>
     <row r="79" spans="2:28" ht="12.75" customHeight="1">
-      <c r="M79" s="61"/>
-      <c r="N79" s="61"/>
-      <c r="O79" s="61"/>
-      <c r="P79" s="61"/>
-      <c r="Q79" s="61"/>
+      <c r="M79" s="62"/>
+      <c r="N79" s="62"/>
+      <c r="O79" s="62"/>
+      <c r="P79" s="62"/>
+      <c r="Q79" s="62"/>
       <c r="R79" s="43"/>
       <c r="S79" s="43"/>
       <c r="T79" s="43"/>
@@ -5674,11 +5742,11 @@
       <c r="AB79" s="43"/>
     </row>
     <row r="80" spans="2:28" ht="12.75" customHeight="1">
-      <c r="M80" s="61"/>
-      <c r="N80" s="61"/>
-      <c r="O80" s="61"/>
-      <c r="P80" s="61"/>
-      <c r="Q80" s="61"/>
+      <c r="M80" s="62"/>
+      <c r="N80" s="62"/>
+      <c r="O80" s="62"/>
+      <c r="P80" s="62"/>
+      <c r="Q80" s="62"/>
       <c r="R80" s="43"/>
       <c r="S80" s="43"/>
       <c r="T80" s="43"/>
@@ -5692,11 +5760,11 @@
       <c r="AB80" s="43"/>
     </row>
     <row r="81" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M81" s="61"/>
-      <c r="N81" s="61"/>
-      <c r="O81" s="61"/>
-      <c r="P81" s="61"/>
-      <c r="Q81" s="61"/>
+      <c r="M81" s="62"/>
+      <c r="N81" s="62"/>
+      <c r="O81" s="62"/>
+      <c r="P81" s="62"/>
+      <c r="Q81" s="62"/>
       <c r="R81" s="43"/>
       <c r="S81" s="43"/>
       <c r="T81" s="43"/>
@@ -5710,11 +5778,11 @@
       <c r="AB81" s="43"/>
     </row>
     <row r="82" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M82" s="61"/>
-      <c r="N82" s="61"/>
-      <c r="O82" s="61"/>
-      <c r="P82" s="61"/>
-      <c r="Q82" s="61"/>
+      <c r="M82" s="62"/>
+      <c r="N82" s="62"/>
+      <c r="O82" s="62"/>
+      <c r="P82" s="62"/>
+      <c r="Q82" s="62"/>
       <c r="R82" s="43"/>
       <c r="S82" s="43"/>
       <c r="T82" s="43"/>
@@ -5728,11 +5796,11 @@
       <c r="AB82" s="43"/>
     </row>
     <row r="83" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M83" s="61"/>
-      <c r="N83" s="61"/>
-      <c r="O83" s="61"/>
-      <c r="P83" s="61"/>
-      <c r="Q83" s="61"/>
+      <c r="M83" s="62"/>
+      <c r="N83" s="62"/>
+      <c r="O83" s="62"/>
+      <c r="P83" s="62"/>
+      <c r="Q83" s="62"/>
       <c r="R83" s="43"/>
       <c r="S83" s="43"/>
       <c r="T83" s="43"/>
@@ -5746,11 +5814,11 @@
       <c r="AB83" s="43"/>
     </row>
     <row r="84" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M84" s="61"/>
-      <c r="N84" s="61"/>
-      <c r="O84" s="61"/>
-      <c r="P84" s="61"/>
-      <c r="Q84" s="61"/>
+      <c r="M84" s="62"/>
+      <c r="N84" s="62"/>
+      <c r="O84" s="62"/>
+      <c r="P84" s="62"/>
+      <c r="Q84" s="62"/>
       <c r="R84" s="43"/>
       <c r="S84" s="43"/>
       <c r="T84" s="43"/>
@@ -5764,11 +5832,11 @@
       <c r="AB84" s="43"/>
     </row>
     <row r="85" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M85" s="61"/>
-      <c r="N85" s="61"/>
-      <c r="O85" s="61"/>
-      <c r="P85" s="61"/>
-      <c r="Q85" s="61"/>
+      <c r="M85" s="62"/>
+      <c r="N85" s="62"/>
+      <c r="O85" s="62"/>
+      <c r="P85" s="62"/>
+      <c r="Q85" s="62"/>
       <c r="R85" s="43"/>
       <c r="S85" s="43"/>
       <c r="T85" s="43"/>
@@ -5782,11 +5850,11 @@
       <c r="AB85" s="43"/>
     </row>
     <row r="86" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M86" s="61"/>
-      <c r="N86" s="61"/>
-      <c r="O86" s="61"/>
-      <c r="P86" s="61"/>
-      <c r="Q86" s="61"/>
+      <c r="M86" s="62"/>
+      <c r="N86" s="62"/>
+      <c r="O86" s="62"/>
+      <c r="P86" s="62"/>
+      <c r="Q86" s="62"/>
       <c r="R86" s="43"/>
       <c r="S86" s="43"/>
       <c r="T86" s="43"/>
@@ -5800,11 +5868,11 @@
       <c r="AB86" s="43"/>
     </row>
     <row r="87" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M87" s="61"/>
-      <c r="N87" s="61"/>
-      <c r="O87" s="61"/>
-      <c r="P87" s="61"/>
-      <c r="Q87" s="61"/>
+      <c r="M87" s="62"/>
+      <c r="N87" s="62"/>
+      <c r="O87" s="62"/>
+      <c r="P87" s="62"/>
+      <c r="Q87" s="62"/>
       <c r="R87" s="43"/>
       <c r="S87" s="43"/>
       <c r="T87" s="43"/>
@@ -5890,267 +5958,267 @@
       </c>
     </row>
     <row r="3" spans="2:21" ht="12.75" customHeight="1">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="63" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="63"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="63"/>
+      <c r="T3" s="63"/>
+      <c r="U3" s="63"/>
     </row>
     <row r="4" spans="2:21">
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="62"/>
-      <c r="U4" s="62"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
+      <c r="T4" s="63"/>
+      <c r="U4" s="63"/>
     </row>
     <row r="5" spans="2:21">
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="62"/>
-      <c r="K5" s="62"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="62"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="62"/>
-      <c r="U5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
     </row>
     <row r="6" spans="2:21">
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
     </row>
     <row r="7" spans="2:21">
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="62"/>
-      <c r="T7" s="62"/>
-      <c r="U7" s="62"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
     </row>
     <row r="8" spans="2:21">
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62"/>
-      <c r="T8" s="62"/>
-      <c r="U8" s="62"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
     </row>
     <row r="9" spans="2:21">
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="62"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="62"/>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="63"/>
+      <c r="T9" s="63"/>
+      <c r="U9" s="63"/>
     </row>
     <row r="10" spans="2:21">
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="62"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
-      <c r="T10" s="62"/>
-      <c r="U10" s="62"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="63"/>
+      <c r="T10" s="63"/>
+      <c r="U10" s="63"/>
     </row>
     <row r="11" spans="2:21">
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="62"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="62"/>
-      <c r="O11" s="62"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="62"/>
-      <c r="T11" s="62"/>
-      <c r="U11" s="62"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
+      <c r="U11" s="63"/>
     </row>
     <row r="12" spans="2:21">
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62"/>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="62"/>
-      <c r="S12" s="62"/>
-      <c r="T12" s="62"/>
-      <c r="U12" s="62"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
+      <c r="U12" s="63"/>
     </row>
     <row r="15" spans="2:21" ht="12.75" customHeight="1">
       <c r="B15" t="s">
         <v>189</v>
       </c>
-      <c r="F15" s="61" t="s">
+      <c r="F15" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="61"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="62"/>
     </row>
     <row r="16" spans="2:21">
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="62"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="62"/>
+      <c r="N17" s="62"/>
+      <c r="O17" s="62"/>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" s="28" t="s">
@@ -6165,16 +6233,16 @@
       <c r="E18" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="61"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="62"/>
+      <c r="N18" s="62"/>
+      <c r="O18" s="62"/>
     </row>
     <row r="19" spans="2:15">
       <c r="B19" t="s">
@@ -6189,16 +6257,16 @@
       <c r="E19" t="s">
         <v>195</v>
       </c>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="62"/>
     </row>
     <row r="20" spans="2:15">
       <c r="C20" t="s">
@@ -6210,16 +6278,16 @@
       <c r="E20" t="s">
         <v>198</v>
       </c>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="61"/>
-      <c r="N20" s="61"/>
-      <c r="O20" s="61"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+      <c r="N20" s="62"/>
+      <c r="O20" s="62"/>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
@@ -6231,16 +6299,16 @@
       <c r="D21" t="s">
         <v>200</v>
       </c>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
-      <c r="N21" s="61"/>
-      <c r="O21" s="61"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="62"/>
+      <c r="N21" s="62"/>
+      <c r="O21" s="62"/>
     </row>
     <row r="22" spans="2:15">
       <c r="C22" t="s">
@@ -6252,16 +6320,16 @@
       <c r="E22" t="s">
         <v>202</v>
       </c>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="62"/>
+      <c r="M22" s="62"/>
+      <c r="N22" s="62"/>
+      <c r="O22" s="62"/>
     </row>
     <row r="23" spans="2:15">
       <c r="B23" t="s">
@@ -6270,364 +6338,364 @@
       <c r="D23" t="s">
         <v>204</v>
       </c>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="62"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="62"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="62"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="62"/>
+      <c r="O26" s="62"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="62"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="61"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="61"/>
-      <c r="N29" s="61"/>
-      <c r="O29" s="61"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="62"/>
+      <c r="N29" s="62"/>
+      <c r="O29" s="62"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="61"/>
-      <c r="N30" s="61"/>
-      <c r="O30" s="61"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="62"/>
+      <c r="N30" s="62"/>
+      <c r="O30" s="62"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="61"/>
-      <c r="N31" s="61"/>
-      <c r="O31" s="61"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="62"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="62"/>
+      <c r="N31" s="62"/>
+      <c r="O31" s="62"/>
     </row>
     <row r="32" spans="2:15">
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
-      <c r="N32" s="61"/>
-      <c r="O32" s="61"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="62"/>
     </row>
     <row r="33" spans="6:15">
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="61"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="62"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="62"/>
     </row>
     <row r="34" spans="6:15">
-      <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="61"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="61"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="62"/>
+      <c r="N34" s="62"/>
+      <c r="O34" s="62"/>
     </row>
     <row r="35" spans="6:15">
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="61"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="61"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="61"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="62"/>
+      <c r="K35" s="62"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="62"/>
+      <c r="N35" s="62"/>
+      <c r="O35" s="62"/>
     </row>
     <row r="36" spans="6:15">
-      <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="61"/>
-      <c r="J36" s="61"/>
-      <c r="K36" s="61"/>
-      <c r="L36" s="61"/>
-      <c r="M36" s="61"/>
-      <c r="N36" s="61"/>
-      <c r="O36" s="61"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="62"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="62"/>
+      <c r="N36" s="62"/>
+      <c r="O36" s="62"/>
     </row>
     <row r="37" spans="6:15">
-      <c r="F37" s="61"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="61"/>
-      <c r="I37" s="61"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="61"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="61"/>
-      <c r="N37" s="61"/>
-      <c r="O37" s="61"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="62"/>
+      <c r="M37" s="62"/>
+      <c r="N37" s="62"/>
+      <c r="O37" s="62"/>
     </row>
     <row r="38" spans="6:15">
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="61"/>
-      <c r="I38" s="61"/>
-      <c r="J38" s="61"/>
-      <c r="K38" s="61"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="61"/>
-      <c r="O38" s="61"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="62"/>
+      <c r="N38" s="62"/>
+      <c r="O38" s="62"/>
     </row>
     <row r="39" spans="6:15">
-      <c r="F39" s="61"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="61"/>
-      <c r="I39" s="61"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="61"/>
-      <c r="O39" s="61"/>
+      <c r="F39" s="62"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="62"/>
+      <c r="N39" s="62"/>
+      <c r="O39" s="62"/>
     </row>
     <row r="40" spans="6:15">
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="61"/>
-      <c r="J40" s="61"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="61"/>
-      <c r="O40" s="61"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="62"/>
     </row>
     <row r="41" spans="6:15">
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="61"/>
-      <c r="K41" s="61"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="61"/>
-      <c r="N41" s="61"/>
-      <c r="O41" s="61"/>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="62"/>
+      <c r="L41" s="62"/>
+      <c r="M41" s="62"/>
+      <c r="N41" s="62"/>
+      <c r="O41" s="62"/>
     </row>
     <row r="42" spans="6:15">
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="61"/>
-      <c r="J42" s="61"/>
-      <c r="K42" s="61"/>
-      <c r="L42" s="61"/>
-      <c r="M42" s="61"/>
-      <c r="N42" s="61"/>
-      <c r="O42" s="61"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="62"/>
+      <c r="N42" s="62"/>
+      <c r="O42" s="62"/>
     </row>
     <row r="43" spans="6:15">
-      <c r="F43" s="61"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="61"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="61"/>
-      <c r="L43" s="61"/>
-      <c r="M43" s="61"/>
-      <c r="N43" s="61"/>
-      <c r="O43" s="61"/>
+      <c r="F43" s="62"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="62"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
+      <c r="M43" s="62"/>
+      <c r="N43" s="62"/>
+      <c r="O43" s="62"/>
     </row>
     <row r="44" spans="6:15">
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="61"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="61"/>
-      <c r="N44" s="61"/>
-      <c r="O44" s="61"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="62"/>
+      <c r="N44" s="62"/>
+      <c r="O44" s="62"/>
     </row>
     <row r="45" spans="6:15">
-      <c r="F45" s="61"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="61"/>
-      <c r="N45" s="61"/>
-      <c r="O45" s="61"/>
+      <c r="F45" s="62"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="62"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="62"/>
+      <c r="N45" s="62"/>
+      <c r="O45" s="62"/>
     </row>
     <row r="46" spans="6:15">
-      <c r="F46" s="61"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="61"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="L46" s="61"/>
-      <c r="M46" s="61"/>
-      <c r="N46" s="61"/>
-      <c r="O46" s="61"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="62"/>
+      <c r="J46" s="62"/>
+      <c r="K46" s="62"/>
+      <c r="L46" s="62"/>
+      <c r="M46" s="62"/>
+      <c r="N46" s="62"/>
+      <c r="O46" s="62"/>
     </row>
     <row r="47" spans="6:15">
-      <c r="F47" s="61"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="61"/>
-      <c r="I47" s="61"/>
-      <c r="J47" s="61"/>
-      <c r="K47" s="61"/>
-      <c r="L47" s="61"/>
-      <c r="M47" s="61"/>
-      <c r="N47" s="61"/>
-      <c r="O47" s="61"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="62"/>
+      <c r="L47" s="62"/>
+      <c r="M47" s="62"/>
+      <c r="N47" s="62"/>
+      <c r="O47" s="62"/>
     </row>
     <row r="48" spans="6:15">
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="61"/>
-      <c r="I48" s="61"/>
-      <c r="J48" s="61"/>
-      <c r="K48" s="61"/>
-      <c r="L48" s="61"/>
-      <c r="M48" s="61"/>
-      <c r="N48" s="61"/>
-      <c r="O48" s="61"/>
+      <c r="F48" s="62"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="62"/>
+      <c r="J48" s="62"/>
+      <c r="K48" s="62"/>
+      <c r="L48" s="62"/>
+      <c r="M48" s="62"/>
+      <c r="N48" s="62"/>
+      <c r="O48" s="62"/>
     </row>
     <row r="49" spans="6:15">
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="61"/>
-      <c r="I49" s="61"/>
-      <c r="J49" s="61"/>
-      <c r="K49" s="61"/>
-      <c r="L49" s="61"/>
-      <c r="M49" s="61"/>
-      <c r="N49" s="61"/>
-      <c r="O49" s="61"/>
+      <c r="F49" s="62"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="62"/>
+      <c r="K49" s="62"/>
+      <c r="L49" s="62"/>
+      <c r="M49" s="62"/>
+      <c r="N49" s="62"/>
+      <c r="O49" s="62"/>
     </row>
     <row r="50" spans="6:15">
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="61"/>
-      <c r="I50" s="61"/>
-      <c r="J50" s="61"/>
-      <c r="K50" s="61"/>
-      <c r="L50" s="61"/>
-      <c r="M50" s="61"/>
-      <c r="N50" s="61"/>
-      <c r="O50" s="61"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="62"/>
+      <c r="K50" s="62"/>
+      <c r="L50" s="62"/>
+      <c r="M50" s="62"/>
+      <c r="N50" s="62"/>
+      <c r="O50" s="62"/>
     </row>
     <row r="51" spans="6:15">
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="61"/>
-      <c r="I51" s="61"/>
-      <c r="J51" s="61"/>
-      <c r="K51" s="61"/>
-      <c r="L51" s="61"/>
-      <c r="M51" s="61"/>
-      <c r="N51" s="61"/>
-      <c r="O51" s="61"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="62"/>
+      <c r="I51" s="62"/>
+      <c r="J51" s="62"/>
+      <c r="K51" s="62"/>
+      <c r="L51" s="62"/>
+      <c r="M51" s="62"/>
+      <c r="N51" s="62"/>
+      <c r="O51" s="62"/>
     </row>
     <row r="52" spans="6:15">
-      <c r="F52" s="61"/>
-      <c r="G52" s="61"/>
-      <c r="H52" s="61"/>
-      <c r="I52" s="61"/>
-      <c r="J52" s="61"/>
-      <c r="K52" s="61"/>
-      <c r="L52" s="61"/>
-      <c r="M52" s="61"/>
-      <c r="N52" s="61"/>
-      <c r="O52" s="61"/>
+      <c r="F52" s="62"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="62"/>
+      <c r="I52" s="62"/>
+      <c r="J52" s="62"/>
+      <c r="K52" s="62"/>
+      <c r="L52" s="62"/>
+      <c r="M52" s="62"/>
+      <c r="N52" s="62"/>
+      <c r="O52" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6644,7 +6712,7 @@
   <dimension ref="A1:K150"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -6843,6 +6911,9 @@
       <c r="C9" s="34" t="s">
         <v>78</v>
       </c>
+      <c r="D9" s="10" t="s">
+        <v>371</v>
+      </c>
       <c r="E9" s="10" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Solid updates to global M2 script and PriceImporter utility functions etc.
</commit_message>
<xml_diff>
--- a/Generic_Macro/Control.xlsx
+++ b/Generic_Macro/Control.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesbishop/Documents/Python/TempVenv/Plebs_Macro/Generic_Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8964FD6B-891B-FB46-A244-F062EA5921FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B425F8B-17D8-1D42-87ED-D6E6F6BBAAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="405">
   <si>
     <t>Index</t>
   </si>
@@ -1373,34 +1373,55 @@
     <t>Real disposable personal income</t>
   </si>
   <si>
-    <t>Real personal income USA</t>
-  </si>
-  <si>
     <t>Trillions of chained 2017 US $</t>
   </si>
   <si>
     <t>CNLIVRR, ECONOMICS</t>
   </si>
   <si>
-    <t>CNLiq</t>
-  </si>
-  <si>
     <t>CNLIVRR_cum</t>
   </si>
   <si>
     <t>BTCUSD, INDEX</t>
   </si>
   <si>
-    <t xml:space="preserve">YoY % change </t>
-  </si>
-  <si>
-    <t>CNY Liq Injections (cumulative since 2019, YoY % change)</t>
-  </si>
-  <si>
-    <t>BTC (USD) YoY % change</t>
-  </si>
-  <si>
-    <t>2020-01-01</t>
+    <t>China stimmie via RRP</t>
+  </si>
+  <si>
+    <t>China stimmie via RRP (cumulative)</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>M2 money supply U.S</t>
+  </si>
+  <si>
+    <t>QCNPAMUSDA</t>
+  </si>
+  <si>
+    <t>Credit to private, non-financial sector, China</t>
+  </si>
+  <si>
+    <t>cncred</t>
+  </si>
+  <si>
+    <t>China M2 proxies?</t>
+  </si>
+  <si>
+    <t>CNM2, ECONOMICS</t>
+  </si>
+  <si>
+    <t>M2 money supply China</t>
+  </si>
+  <si>
+    <t>Yuan</t>
+  </si>
+  <si>
+    <t>1997-01-01</t>
+  </si>
+  <si>
+    <t>Trilliions of Chinese Yuan</t>
   </si>
 </sst>
 </file>
@@ -1671,7 +1692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1818,6 +1839,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2225,8 +2250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -2300,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>15</v>
@@ -2312,16 +2337,16 @@
         <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -2341,7 +2366,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>15</v>
@@ -2350,19 +2375,19 @@
         <v>145</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>367</v>
+        <v>398</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>394</v>
+        <v>366</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -2370,7 +2395,9 @@
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="8"/>
-      <c r="P3" s="7"/>
+      <c r="P3" s="7">
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" spans="1:16" ht="18">
       <c r="A4" s="3">
@@ -2452,12 +2479,12 @@
         <v>31</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>397</v>
-      </c>
-      <c r="C8" s="60" t="s">
+        <v>403</v>
+      </c>
+      <c r="C8" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -2472,11 +2499,11 @@
         <v>33</v>
       </c>
       <c r="B9" s="16"/>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -2503,11 +2530,11 @@
       <c r="A11" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -2521,13 +2548,13 @@
       <c r="A12" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="63" t="s">
-        <v>388</v>
-      </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
+      <c r="B12" s="65" t="s">
+        <v>399</v>
+      </c>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -2649,6 +2676,7 @@
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="F20" s="23"/>
+      <c r="G20" s="60"/>
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
       <c r="K20" s="23"/>
@@ -2660,7 +2688,7 @@
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
-      <c r="G21" s="14"/>
+      <c r="G21" s="61"/>
       <c r="H21" s="14"/>
       <c r="I21" s="22"/>
       <c r="J21" s="23"/>
@@ -2845,8 +2873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB87"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -4474,13 +4502,13 @@
       <c r="J43" s="9"/>
       <c r="K43" s="14"/>
       <c r="L43" s="14"/>
-      <c r="M43" s="64" t="s">
+      <c r="M43" s="66" t="s">
         <v>185</v>
       </c>
-      <c r="N43" s="64"/>
-      <c r="O43" s="64"/>
-      <c r="P43" s="64"/>
-      <c r="Q43" s="64"/>
+      <c r="N43" s="66"/>
+      <c r="O43" s="66"/>
+      <c r="P43" s="66"/>
+      <c r="Q43" s="66"/>
       <c r="R43" s="41"/>
       <c r="S43" s="41"/>
       <c r="T43" s="41"/>
@@ -4515,13 +4543,13 @@
       <c r="J44" s="9"/>
       <c r="K44" s="14"/>
       <c r="L44" s="14"/>
-      <c r="M44" s="65" t="s">
+      <c r="M44" s="67" t="s">
         <v>186</v>
       </c>
-      <c r="N44" s="65"/>
-      <c r="O44" s="65"/>
-      <c r="P44" s="65"/>
-      <c r="Q44" s="65"/>
+      <c r="N44" s="67"/>
+      <c r="O44" s="67"/>
+      <c r="P44" s="67"/>
+      <c r="Q44" s="67"/>
       <c r="R44" s="41"/>
       <c r="S44" s="41"/>
       <c r="T44" s="41"/>
@@ -4556,11 +4584,11 @@
       <c r="J45" s="9"/>
       <c r="K45" s="14"/>
       <c r="L45" s="14"/>
-      <c r="M45" s="65"/>
-      <c r="N45" s="65"/>
-      <c r="O45" s="65"/>
-      <c r="P45" s="65"/>
-      <c r="Q45" s="65"/>
+      <c r="M45" s="67"/>
+      <c r="N45" s="67"/>
+      <c r="O45" s="67"/>
+      <c r="P45" s="67"/>
+      <c r="Q45" s="67"/>
       <c r="R45" s="41"/>
       <c r="S45" s="41"/>
       <c r="T45" s="41"/>
@@ -4595,11 +4623,11 @@
       <c r="J46" s="9"/>
       <c r="K46" s="14"/>
       <c r="L46" s="14"/>
-      <c r="M46" s="65"/>
-      <c r="N46" s="65"/>
-      <c r="O46" s="65"/>
-      <c r="P46" s="65"/>
-      <c r="Q46" s="65"/>
+      <c r="M46" s="67"/>
+      <c r="N46" s="67"/>
+      <c r="O46" s="67"/>
+      <c r="P46" s="67"/>
+      <c r="Q46" s="67"/>
       <c r="R46" s="41"/>
       <c r="S46" s="41"/>
       <c r="T46" s="41"/>
@@ -4634,11 +4662,11 @@
       <c r="J47" s="9"/>
       <c r="K47" s="14"/>
       <c r="L47" s="14"/>
-      <c r="M47" s="65"/>
-      <c r="N47" s="65"/>
-      <c r="O47" s="65"/>
-      <c r="P47" s="65"/>
-      <c r="Q47" s="65"/>
+      <c r="M47" s="67"/>
+      <c r="N47" s="67"/>
+      <c r="O47" s="67"/>
+      <c r="P47" s="67"/>
+      <c r="Q47" s="67"/>
       <c r="R47" s="41"/>
       <c r="S47" s="41"/>
       <c r="T47" s="41"/>
@@ -4665,11 +4693,11 @@
       <c r="J48" s="9"/>
       <c r="K48" s="14"/>
       <c r="L48" s="14"/>
-      <c r="M48" s="65"/>
-      <c r="N48" s="65"/>
-      <c r="O48" s="65"/>
-      <c r="P48" s="65"/>
-      <c r="Q48" s="65"/>
+      <c r="M48" s="67"/>
+      <c r="N48" s="67"/>
+      <c r="O48" s="67"/>
+      <c r="P48" s="67"/>
+      <c r="Q48" s="67"/>
       <c r="R48" s="41"/>
       <c r="S48" s="41"/>
       <c r="T48" s="41"/>
@@ -4710,11 +4738,11 @@
       <c r="J49" s="9"/>
       <c r="K49" s="14"/>
       <c r="L49" s="14"/>
-      <c r="M49" s="65"/>
-      <c r="N49" s="65"/>
-      <c r="O49" s="65"/>
-      <c r="P49" s="65"/>
-      <c r="Q49" s="65"/>
+      <c r="M49" s="67"/>
+      <c r="N49" s="67"/>
+      <c r="O49" s="67"/>
+      <c r="P49" s="67"/>
+      <c r="Q49" s="67"/>
       <c r="R49" s="41"/>
       <c r="S49" s="41"/>
       <c r="T49" s="41"/>
@@ -4745,11 +4773,11 @@
       <c r="J50" s="9"/>
       <c r="K50" s="14"/>
       <c r="L50" s="14"/>
-      <c r="M50" s="65"/>
-      <c r="N50" s="65"/>
-      <c r="O50" s="65"/>
-      <c r="P50" s="65"/>
-      <c r="Q50" s="65"/>
+      <c r="M50" s="67"/>
+      <c r="N50" s="67"/>
+      <c r="O50" s="67"/>
+      <c r="P50" s="67"/>
+      <c r="Q50" s="67"/>
       <c r="R50" s="41"/>
       <c r="S50" s="41"/>
       <c r="T50" s="41"/>
@@ -4780,11 +4808,11 @@
       <c r="J51" s="9"/>
       <c r="K51" s="14"/>
       <c r="L51" s="14"/>
-      <c r="M51" s="65"/>
-      <c r="N51" s="65"/>
-      <c r="O51" s="65"/>
-      <c r="P51" s="65"/>
-      <c r="Q51" s="65"/>
+      <c r="M51" s="67"/>
+      <c r="N51" s="67"/>
+      <c r="O51" s="67"/>
+      <c r="P51" s="67"/>
+      <c r="Q51" s="67"/>
       <c r="R51" s="41"/>
       <c r="S51" s="41"/>
       <c r="T51" s="41"/>
@@ -4827,11 +4855,11 @@
       </c>
       <c r="K52" s="14"/>
       <c r="L52" s="14"/>
-      <c r="M52" s="65"/>
-      <c r="N52" s="65"/>
-      <c r="O52" s="65"/>
-      <c r="P52" s="65"/>
-      <c r="Q52" s="65"/>
+      <c r="M52" s="67"/>
+      <c r="N52" s="67"/>
+      <c r="O52" s="67"/>
+      <c r="P52" s="67"/>
+      <c r="Q52" s="67"/>
       <c r="R52" s="41"/>
       <c r="S52" s="41"/>
       <c r="T52" s="41"/>
@@ -4874,11 +4902,11 @@
       </c>
       <c r="K53" s="14"/>
       <c r="L53" s="14"/>
-      <c r="M53" s="65"/>
-      <c r="N53" s="65"/>
-      <c r="O53" s="65"/>
-      <c r="P53" s="65"/>
-      <c r="Q53" s="65"/>
+      <c r="M53" s="67"/>
+      <c r="N53" s="67"/>
+      <c r="O53" s="67"/>
+      <c r="P53" s="67"/>
+      <c r="Q53" s="67"/>
       <c r="R53" s="41"/>
       <c r="S53" s="41"/>
       <c r="T53" s="41"/>
@@ -4922,11 +4950,11 @@
       </c>
       <c r="K54" s="14"/>
       <c r="L54" s="14"/>
-      <c r="M54" s="65"/>
-      <c r="N54" s="65"/>
-      <c r="O54" s="65"/>
-      <c r="P54" s="65"/>
-      <c r="Q54" s="65"/>
+      <c r="M54" s="67"/>
+      <c r="N54" s="67"/>
+      <c r="O54" s="67"/>
+      <c r="P54" s="67"/>
+      <c r="Q54" s="67"/>
       <c r="R54" s="41"/>
       <c r="S54" s="41"/>
       <c r="T54" s="41"/>
@@ -4967,11 +4995,11 @@
       <c r="J55" s="9"/>
       <c r="K55" s="14"/>
       <c r="L55" s="14"/>
-      <c r="M55" s="65"/>
-      <c r="N55" s="65"/>
-      <c r="O55" s="65"/>
-      <c r="P55" s="65"/>
-      <c r="Q55" s="65"/>
+      <c r="M55" s="67"/>
+      <c r="N55" s="67"/>
+      <c r="O55" s="67"/>
+      <c r="P55" s="67"/>
+      <c r="Q55" s="67"/>
       <c r="R55" s="41"/>
       <c r="S55" s="41"/>
       <c r="T55" s="41"/>
@@ -5012,11 +5040,11 @@
       <c r="J56" s="9"/>
       <c r="K56" s="14"/>
       <c r="L56" s="14"/>
-      <c r="M56" s="65"/>
-      <c r="N56" s="65"/>
-      <c r="O56" s="65"/>
-      <c r="P56" s="65"/>
-      <c r="Q56" s="65"/>
+      <c r="M56" s="67"/>
+      <c r="N56" s="67"/>
+      <c r="O56" s="67"/>
+      <c r="P56" s="67"/>
+      <c r="Q56" s="67"/>
       <c r="R56" s="41"/>
       <c r="S56" s="41"/>
       <c r="T56" s="41"/>
@@ -5055,11 +5083,11 @@
       <c r="J57" s="9"/>
       <c r="K57" s="14"/>
       <c r="L57" s="14"/>
-      <c r="M57" s="65"/>
-      <c r="N57" s="65"/>
-      <c r="O57" s="65"/>
-      <c r="P57" s="65"/>
-      <c r="Q57" s="65"/>
+      <c r="M57" s="67"/>
+      <c r="N57" s="67"/>
+      <c r="O57" s="67"/>
+      <c r="P57" s="67"/>
+      <c r="Q57" s="67"/>
       <c r="R57" s="41"/>
       <c r="S57" s="41"/>
       <c r="T57" s="41"/>
@@ -5100,11 +5128,11 @@
       <c r="J58" s="9"/>
       <c r="K58" s="14"/>
       <c r="L58" s="14"/>
-      <c r="M58" s="65"/>
-      <c r="N58" s="65"/>
-      <c r="O58" s="65"/>
-      <c r="P58" s="65"/>
-      <c r="Q58" s="65"/>
+      <c r="M58" s="67"/>
+      <c r="N58" s="67"/>
+      <c r="O58" s="67"/>
+      <c r="P58" s="67"/>
+      <c r="Q58" s="67"/>
       <c r="R58" s="41"/>
       <c r="S58" s="41"/>
       <c r="T58" s="41"/>
@@ -5143,11 +5171,11 @@
       <c r="J59" s="9"/>
       <c r="K59" s="14"/>
       <c r="L59" s="14"/>
-      <c r="M59" s="65"/>
-      <c r="N59" s="65"/>
-      <c r="O59" s="65"/>
-      <c r="P59" s="65"/>
-      <c r="Q59" s="65"/>
+      <c r="M59" s="67"/>
+      <c r="N59" s="67"/>
+      <c r="O59" s="67"/>
+      <c r="P59" s="67"/>
+      <c r="Q59" s="67"/>
       <c r="R59" s="41"/>
       <c r="S59" s="41"/>
       <c r="T59" s="41"/>
@@ -5188,11 +5216,11 @@
       <c r="J60" s="9"/>
       <c r="K60" s="14"/>
       <c r="L60" s="14"/>
-      <c r="M60" s="65"/>
-      <c r="N60" s="65"/>
-      <c r="O60" s="65"/>
-      <c r="P60" s="65"/>
-      <c r="Q60" s="65"/>
+      <c r="M60" s="67"/>
+      <c r="N60" s="67"/>
+      <c r="O60" s="67"/>
+      <c r="P60" s="67"/>
+      <c r="Q60" s="67"/>
       <c r="R60" s="41"/>
       <c r="S60" s="41"/>
       <c r="T60" s="41"/>
@@ -5233,11 +5261,11 @@
       <c r="J61" s="9"/>
       <c r="K61" s="14"/>
       <c r="L61" s="14"/>
-      <c r="M61" s="65"/>
-      <c r="N61" s="65"/>
-      <c r="O61" s="65"/>
-      <c r="P61" s="65"/>
-      <c r="Q61" s="65"/>
+      <c r="M61" s="67"/>
+      <c r="N61" s="67"/>
+      <c r="O61" s="67"/>
+      <c r="P61" s="67"/>
+      <c r="Q61" s="67"/>
       <c r="R61" s="41"/>
       <c r="S61" s="41"/>
       <c r="T61" s="41"/>
@@ -5278,11 +5306,11 @@
       <c r="J62" s="9"/>
       <c r="K62" s="14"/>
       <c r="L62" s="14"/>
-      <c r="M62" s="65"/>
-      <c r="N62" s="65"/>
-      <c r="O62" s="65"/>
-      <c r="P62" s="65"/>
-      <c r="Q62" s="65"/>
+      <c r="M62" s="67"/>
+      <c r="N62" s="67"/>
+      <c r="O62" s="67"/>
+      <c r="P62" s="67"/>
+      <c r="Q62" s="67"/>
       <c r="R62" s="41"/>
       <c r="S62" s="41"/>
       <c r="T62" s="41"/>
@@ -5323,11 +5351,11 @@
       <c r="J63" s="9"/>
       <c r="K63" s="14"/>
       <c r="L63" s="14"/>
-      <c r="M63" s="65"/>
-      <c r="N63" s="65"/>
-      <c r="O63" s="65"/>
-      <c r="P63" s="65"/>
-      <c r="Q63" s="65"/>
+      <c r="M63" s="67"/>
+      <c r="N63" s="67"/>
+      <c r="O63" s="67"/>
+      <c r="P63" s="67"/>
+      <c r="Q63" s="67"/>
       <c r="R63" s="41"/>
       <c r="S63" s="41"/>
       <c r="T63" s="41"/>
@@ -5366,11 +5394,11 @@
         <v>372</v>
       </c>
       <c r="J64" s="36"/>
-      <c r="M64" s="65"/>
-      <c r="N64" s="65"/>
-      <c r="O64" s="65"/>
-      <c r="P64" s="65"/>
-      <c r="Q64" s="65"/>
+      <c r="M64" s="67"/>
+      <c r="N64" s="67"/>
+      <c r="O64" s="67"/>
+      <c r="P64" s="67"/>
+      <c r="Q64" s="67"/>
       <c r="R64" s="41"/>
       <c r="S64" s="41"/>
       <c r="T64" s="41"/>
@@ -5409,11 +5437,11 @@
         <v>371</v>
       </c>
       <c r="J65" s="36"/>
-      <c r="M65" s="65"/>
-      <c r="N65" s="65"/>
-      <c r="O65" s="65"/>
-      <c r="P65" s="65"/>
-      <c r="Q65" s="65"/>
+      <c r="M65" s="67"/>
+      <c r="N65" s="67"/>
+      <c r="O65" s="67"/>
+      <c r="P65" s="67"/>
+      <c r="Q65" s="67"/>
       <c r="R65" s="41"/>
       <c r="S65" s="41"/>
       <c r="T65" s="41"/>
@@ -5449,14 +5477,14 @@
         <v>387</v>
       </c>
       <c r="I66" s="36" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J66" s="36"/>
-      <c r="M66" s="65"/>
-      <c r="N66" s="65"/>
-      <c r="O66" s="65"/>
-      <c r="P66" s="65"/>
-      <c r="Q66" s="65"/>
+      <c r="M66" s="67"/>
+      <c r="N66" s="67"/>
+      <c r="O66" s="67"/>
+      <c r="P66" s="67"/>
+      <c r="Q66" s="67"/>
       <c r="R66" s="41"/>
       <c r="S66" s="41"/>
       <c r="T66" s="41"/>
@@ -5471,7 +5499,7 @@
     </row>
     <row r="67" spans="2:28" ht="12.75" customHeight="1">
       <c r="B67" s="36" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C67" s="36" t="s">
         <v>73</v>
@@ -5480,14 +5508,16 @@
       <c r="E67" s="36"/>
       <c r="F67" s="36"/>
       <c r="G67" s="36"/>
-      <c r="H67" s="36"/>
+      <c r="H67" s="36" t="s">
+        <v>392</v>
+      </c>
       <c r="I67" s="36"/>
       <c r="J67" s="36"/>
-      <c r="M67" s="65"/>
-      <c r="N67" s="65"/>
-      <c r="O67" s="65"/>
-      <c r="P67" s="65"/>
-      <c r="Q67" s="65"/>
+      <c r="M67" s="67"/>
+      <c r="N67" s="67"/>
+      <c r="O67" s="67"/>
+      <c r="P67" s="67"/>
+      <c r="Q67" s="67"/>
       <c r="R67" s="41"/>
       <c r="S67" s="41"/>
       <c r="T67" s="41"/>
@@ -5501,20 +5531,26 @@
       <c r="AB67" s="41"/>
     </row>
     <row r="68" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
+      <c r="B68" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="C68" s="36" t="s">
+        <v>15</v>
+      </c>
       <c r="D68" s="36"/>
       <c r="E68" s="36"/>
       <c r="F68" s="36"/>
       <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
+      <c r="H68" s="36" t="s">
+        <v>393</v>
+      </c>
       <c r="I68" s="36"/>
       <c r="J68" s="36"/>
-      <c r="M68" s="65"/>
-      <c r="N68" s="65"/>
-      <c r="O68" s="65"/>
-      <c r="P68" s="65"/>
-      <c r="Q68" s="65"/>
+      <c r="M68" s="67"/>
+      <c r="N68" s="67"/>
+      <c r="O68" s="67"/>
+      <c r="P68" s="67"/>
+      <c r="Q68" s="67"/>
       <c r="R68" s="41"/>
       <c r="S68" s="41"/>
       <c r="T68" s="41"/>
@@ -5528,8 +5564,12 @@
       <c r="AB68" s="41"/>
     </row>
     <row r="69" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
+      <c r="B69" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C69" s="36" t="s">
+        <v>73</v>
+      </c>
       <c r="D69" s="36"/>
       <c r="E69" s="36"/>
       <c r="F69" s="36"/>
@@ -5537,11 +5577,11 @@
       <c r="H69" s="36"/>
       <c r="I69" s="36"/>
       <c r="J69" s="36"/>
-      <c r="M69" s="65"/>
-      <c r="N69" s="65"/>
-      <c r="O69" s="65"/>
-      <c r="P69" s="65"/>
-      <c r="Q69" s="65"/>
+      <c r="M69" s="67"/>
+      <c r="N69" s="67"/>
+      <c r="O69" s="67"/>
+      <c r="P69" s="67"/>
+      <c r="Q69" s="67"/>
       <c r="R69" s="41"/>
       <c r="S69" s="41"/>
       <c r="T69" s="41"/>
@@ -5555,20 +5595,36 @@
       <c r="AB69" s="41"/>
     </row>
     <row r="70" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="36"/>
-      <c r="H70" s="36"/>
-      <c r="I70" s="36"/>
+      <c r="B70" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C70" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="36" t="s">
+        <v>394</v>
+      </c>
+      <c r="G70" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" s="36" t="s">
+        <v>395</v>
+      </c>
+      <c r="I70" s="36" t="s">
+        <v>366</v>
+      </c>
       <c r="J70" s="36"/>
-      <c r="M70" s="65"/>
-      <c r="N70" s="65"/>
-      <c r="O70" s="65"/>
-      <c r="P70" s="65"/>
-      <c r="Q70" s="65"/>
+      <c r="M70" s="67"/>
+      <c r="N70" s="67"/>
+      <c r="O70" s="67"/>
+      <c r="P70" s="67"/>
+      <c r="Q70" s="67"/>
       <c r="R70" s="41"/>
       <c r="S70" s="41"/>
       <c r="T70" s="41"/>
@@ -5582,20 +5638,36 @@
       <c r="AB70" s="41"/>
     </row>
     <row r="71" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="36"/>
-      <c r="I71" s="36"/>
+      <c r="B71" s="36" t="s">
+        <v>359</v>
+      </c>
+      <c r="C71" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="E71" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="F71" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="G71" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="I71" s="36" t="s">
+        <v>366</v>
+      </c>
       <c r="J71" s="36"/>
-      <c r="M71" s="65"/>
-      <c r="N71" s="65"/>
-      <c r="O71" s="65"/>
-      <c r="P71" s="65"/>
-      <c r="Q71" s="65"/>
+      <c r="M71" s="67"/>
+      <c r="N71" s="67"/>
+      <c r="O71" s="67"/>
+      <c r="P71" s="67"/>
+      <c r="Q71" s="67"/>
       <c r="R71" s="41"/>
       <c r="S71" s="41"/>
       <c r="T71" s="41"/>
@@ -5609,7 +5681,9 @@
       <c r="AB71" s="41"/>
     </row>
     <row r="72" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B72" s="36"/>
+      <c r="B72" s="36" t="s">
+        <v>396</v>
+      </c>
       <c r="C72" s="36"/>
       <c r="D72" s="36"/>
       <c r="E72" s="36"/>
@@ -5618,11 +5692,11 @@
       <c r="H72" s="36"/>
       <c r="I72" s="36"/>
       <c r="J72" s="36"/>
-      <c r="M72" s="65"/>
-      <c r="N72" s="65"/>
-      <c r="O72" s="65"/>
-      <c r="P72" s="65"/>
-      <c r="Q72" s="65"/>
+      <c r="M72" s="67"/>
+      <c r="N72" s="67"/>
+      <c r="O72" s="67"/>
+      <c r="P72" s="67"/>
+      <c r="Q72" s="67"/>
       <c r="R72" s="41"/>
       <c r="S72" s="41"/>
       <c r="T72" s="41"/>
@@ -5636,20 +5710,36 @@
       <c r="AB72" s="41"/>
     </row>
     <row r="73" spans="2:28" ht="12.75" customHeight="1">
-      <c r="B73" s="36"/>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="36"/>
-      <c r="G73" s="36"/>
-      <c r="H73" s="36"/>
-      <c r="I73" s="36"/>
+      <c r="B73" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="C73" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D73" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="E73" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" s="36" t="s">
+        <v>394</v>
+      </c>
+      <c r="G73" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H73" s="36" t="s">
+        <v>401</v>
+      </c>
+      <c r="I73" s="36" t="s">
+        <v>402</v>
+      </c>
       <c r="J73" s="36"/>
-      <c r="M73" s="65"/>
-      <c r="N73" s="65"/>
-      <c r="O73" s="65"/>
-      <c r="P73" s="65"/>
-      <c r="Q73" s="65"/>
+      <c r="M73" s="67"/>
+      <c r="N73" s="67"/>
+      <c r="O73" s="67"/>
+      <c r="P73" s="67"/>
+      <c r="Q73" s="67"/>
       <c r="R73" s="41"/>
       <c r="S73" s="41"/>
       <c r="T73" s="41"/>
@@ -5672,11 +5762,11 @@
       <c r="H74" s="36"/>
       <c r="I74" s="36"/>
       <c r="J74" s="36"/>
-      <c r="M74" s="65"/>
-      <c r="N74" s="65"/>
-      <c r="O74" s="65"/>
-      <c r="P74" s="65"/>
-      <c r="Q74" s="65"/>
+      <c r="M74" s="67"/>
+      <c r="N74" s="67"/>
+      <c r="O74" s="67"/>
+      <c r="P74" s="67"/>
+      <c r="Q74" s="67"/>
       <c r="R74" s="41"/>
       <c r="S74" s="41"/>
       <c r="T74" s="41"/>
@@ -5699,11 +5789,11 @@
       <c r="H75" s="33"/>
       <c r="I75" s="33"/>
       <c r="J75" s="33"/>
-      <c r="M75" s="65"/>
-      <c r="N75" s="65"/>
-      <c r="O75" s="65"/>
-      <c r="P75" s="65"/>
-      <c r="Q75" s="65"/>
+      <c r="M75" s="67"/>
+      <c r="N75" s="67"/>
+      <c r="O75" s="67"/>
+      <c r="P75" s="67"/>
+      <c r="Q75" s="67"/>
       <c r="R75" s="41"/>
       <c r="S75" s="41"/>
       <c r="T75" s="41"/>
@@ -5726,11 +5816,11 @@
       <c r="H76" s="33"/>
       <c r="I76" s="33"/>
       <c r="J76" s="33"/>
-      <c r="M76" s="65"/>
-      <c r="N76" s="65"/>
-      <c r="O76" s="65"/>
-      <c r="P76" s="65"/>
-      <c r="Q76" s="65"/>
+      <c r="M76" s="67"/>
+      <c r="N76" s="67"/>
+      <c r="O76" s="67"/>
+      <c r="P76" s="67"/>
+      <c r="Q76" s="67"/>
       <c r="R76" s="41"/>
       <c r="S76" s="41"/>
       <c r="T76" s="41"/>
@@ -5753,11 +5843,11 @@
       <c r="H77" s="33"/>
       <c r="I77" s="33"/>
       <c r="J77" s="33"/>
-      <c r="M77" s="65"/>
-      <c r="N77" s="65"/>
-      <c r="O77" s="65"/>
-      <c r="P77" s="65"/>
-      <c r="Q77" s="65"/>
+      <c r="M77" s="67"/>
+      <c r="N77" s="67"/>
+      <c r="O77" s="67"/>
+      <c r="P77" s="67"/>
+      <c r="Q77" s="67"/>
       <c r="R77" s="41"/>
       <c r="S77" s="41"/>
       <c r="T77" s="41"/>
@@ -5771,11 +5861,11 @@
       <c r="AB77" s="41"/>
     </row>
     <row r="78" spans="2:28" ht="12.75" customHeight="1">
-      <c r="M78" s="65"/>
-      <c r="N78" s="65"/>
-      <c r="O78" s="65"/>
-      <c r="P78" s="65"/>
-      <c r="Q78" s="65"/>
+      <c r="M78" s="67"/>
+      <c r="N78" s="67"/>
+      <c r="O78" s="67"/>
+      <c r="P78" s="67"/>
+      <c r="Q78" s="67"/>
       <c r="R78" s="41"/>
       <c r="S78" s="41"/>
       <c r="T78" s="41"/>
@@ -5789,11 +5879,11 @@
       <c r="AB78" s="41"/>
     </row>
     <row r="79" spans="2:28" ht="12.75" customHeight="1">
-      <c r="M79" s="65"/>
-      <c r="N79" s="65"/>
-      <c r="O79" s="65"/>
-      <c r="P79" s="65"/>
-      <c r="Q79" s="65"/>
+      <c r="M79" s="67"/>
+      <c r="N79" s="67"/>
+      <c r="O79" s="67"/>
+      <c r="P79" s="67"/>
+      <c r="Q79" s="67"/>
       <c r="R79" s="41"/>
       <c r="S79" s="41"/>
       <c r="T79" s="41"/>
@@ -5807,11 +5897,11 @@
       <c r="AB79" s="41"/>
     </row>
     <row r="80" spans="2:28" ht="12.75" customHeight="1">
-      <c r="M80" s="65"/>
-      <c r="N80" s="65"/>
-      <c r="O80" s="65"/>
-      <c r="P80" s="65"/>
-      <c r="Q80" s="65"/>
+      <c r="M80" s="67"/>
+      <c r="N80" s="67"/>
+      <c r="O80" s="67"/>
+      <c r="P80" s="67"/>
+      <c r="Q80" s="67"/>
       <c r="R80" s="41"/>
       <c r="S80" s="41"/>
       <c r="T80" s="41"/>
@@ -5825,11 +5915,11 @@
       <c r="AB80" s="41"/>
     </row>
     <row r="81" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M81" s="65"/>
-      <c r="N81" s="65"/>
-      <c r="O81" s="65"/>
-      <c r="P81" s="65"/>
-      <c r="Q81" s="65"/>
+      <c r="M81" s="67"/>
+      <c r="N81" s="67"/>
+      <c r="O81" s="67"/>
+      <c r="P81" s="67"/>
+      <c r="Q81" s="67"/>
       <c r="R81" s="41"/>
       <c r="S81" s="41"/>
       <c r="T81" s="41"/>
@@ -5843,11 +5933,11 @@
       <c r="AB81" s="41"/>
     </row>
     <row r="82" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M82" s="65"/>
-      <c r="N82" s="65"/>
-      <c r="O82" s="65"/>
-      <c r="P82" s="65"/>
-      <c r="Q82" s="65"/>
+      <c r="M82" s="67"/>
+      <c r="N82" s="67"/>
+      <c r="O82" s="67"/>
+      <c r="P82" s="67"/>
+      <c r="Q82" s="67"/>
       <c r="R82" s="41"/>
       <c r="S82" s="41"/>
       <c r="T82" s="41"/>
@@ -5861,11 +5951,11 @@
       <c r="AB82" s="41"/>
     </row>
     <row r="83" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M83" s="65"/>
-      <c r="N83" s="65"/>
-      <c r="O83" s="65"/>
-      <c r="P83" s="65"/>
-      <c r="Q83" s="65"/>
+      <c r="M83" s="67"/>
+      <c r="N83" s="67"/>
+      <c r="O83" s="67"/>
+      <c r="P83" s="67"/>
+      <c r="Q83" s="67"/>
       <c r="R83" s="41"/>
       <c r="S83" s="41"/>
       <c r="T83" s="41"/>
@@ -5879,11 +5969,11 @@
       <c r="AB83" s="41"/>
     </row>
     <row r="84" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M84" s="65"/>
-      <c r="N84" s="65"/>
-      <c r="O84" s="65"/>
-      <c r="P84" s="65"/>
-      <c r="Q84" s="65"/>
+      <c r="M84" s="67"/>
+      <c r="N84" s="67"/>
+      <c r="O84" s="67"/>
+      <c r="P84" s="67"/>
+      <c r="Q84" s="67"/>
       <c r="R84" s="41"/>
       <c r="S84" s="41"/>
       <c r="T84" s="41"/>
@@ -5897,11 +5987,11 @@
       <c r="AB84" s="41"/>
     </row>
     <row r="85" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M85" s="65"/>
-      <c r="N85" s="65"/>
-      <c r="O85" s="65"/>
-      <c r="P85" s="65"/>
-      <c r="Q85" s="65"/>
+      <c r="M85" s="67"/>
+      <c r="N85" s="67"/>
+      <c r="O85" s="67"/>
+      <c r="P85" s="67"/>
+      <c r="Q85" s="67"/>
       <c r="R85" s="41"/>
       <c r="S85" s="41"/>
       <c r="T85" s="41"/>
@@ -5915,11 +6005,11 @@
       <c r="AB85" s="41"/>
     </row>
     <row r="86" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M86" s="65"/>
-      <c r="N86" s="65"/>
-      <c r="O86" s="65"/>
-      <c r="P86" s="65"/>
-      <c r="Q86" s="65"/>
+      <c r="M86" s="67"/>
+      <c r="N86" s="67"/>
+      <c r="O86" s="67"/>
+      <c r="P86" s="67"/>
+      <c r="Q86" s="67"/>
       <c r="R86" s="41"/>
       <c r="S86" s="41"/>
       <c r="T86" s="41"/>
@@ -5933,11 +6023,11 @@
       <c r="AB86" s="41"/>
     </row>
     <row r="87" spans="13:28" ht="12.75" customHeight="1">
-      <c r="M87" s="65"/>
-      <c r="N87" s="65"/>
-      <c r="O87" s="65"/>
-      <c r="P87" s="65"/>
-      <c r="Q87" s="65"/>
+      <c r="M87" s="67"/>
+      <c r="N87" s="67"/>
+      <c r="O87" s="67"/>
+      <c r="P87" s="67"/>
+      <c r="Q87" s="67"/>
       <c r="R87" s="41"/>
       <c r="S87" s="41"/>
       <c r="T87" s="41"/>
@@ -6023,267 +6113,267 @@
       </c>
     </row>
     <row r="3" spans="2:21" ht="12.75" customHeight="1">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="68" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
     </row>
     <row r="4" spans="2:21">
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="68"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
     </row>
     <row r="5" spans="2:21">
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="68"/>
+      <c r="S5" s="68"/>
+      <c r="T5" s="68"/>
+      <c r="U5" s="68"/>
     </row>
     <row r="6" spans="2:21">
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="66"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
     </row>
     <row r="7" spans="2:21">
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="66"/>
-      <c r="T7" s="66"/>
-      <c r="U7" s="66"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="68"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="68"/>
     </row>
     <row r="8" spans="2:21">
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
-      <c r="S8" s="66"/>
-      <c r="T8" s="66"/>
-      <c r="U8" s="66"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+      <c r="R8" s="68"/>
+      <c r="S8" s="68"/>
+      <c r="T8" s="68"/>
+      <c r="U8" s="68"/>
     </row>
     <row r="9" spans="2:21">
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="66"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="66"/>
-      <c r="R9" s="66"/>
-      <c r="S9" s="66"/>
-      <c r="T9" s="66"/>
-      <c r="U9" s="66"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
+      <c r="R9" s="68"/>
+      <c r="S9" s="68"/>
+      <c r="T9" s="68"/>
+      <c r="U9" s="68"/>
     </row>
     <row r="10" spans="2:21">
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="66"/>
-      <c r="U10" s="66"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="68"/>
+      <c r="S10" s="68"/>
+      <c r="T10" s="68"/>
+      <c r="U10" s="68"/>
     </row>
     <row r="11" spans="2:21">
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="66"/>
-      <c r="S11" s="66"/>
-      <c r="T11" s="66"/>
-      <c r="U11" s="66"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="68"/>
+      <c r="R11" s="68"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="68"/>
+      <c r="U11" s="68"/>
     </row>
     <row r="12" spans="2:21">
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="66"/>
-      <c r="M12" s="66"/>
-      <c r="N12" s="66"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="66"/>
-      <c r="S12" s="66"/>
-      <c r="T12" s="66"/>
-      <c r="U12" s="66"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="68"/>
+      <c r="Q12" s="68"/>
+      <c r="R12" s="68"/>
+      <c r="S12" s="68"/>
+      <c r="T12" s="68"/>
+      <c r="U12" s="68"/>
     </row>
     <row r="15" spans="2:21" ht="12.75" customHeight="1">
       <c r="B15" t="s">
         <v>189</v>
       </c>
-      <c r="F15" s="65" t="s">
+      <c r="F15" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="K15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
     </row>
     <row r="16" spans="2:21">
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="65"/>
-      <c r="L16" s="65"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="65"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="65"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="67"/>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" s="26" t="s">
@@ -6298,16 +6388,16 @@
       <c r="E18" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="65"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="65"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
     </row>
     <row r="19" spans="2:15">
       <c r="B19" t="s">
@@ -6322,16 +6412,16 @@
       <c r="E19" t="s">
         <v>195</v>
       </c>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="65"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="65"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
     </row>
     <row r="20" spans="2:15">
       <c r="C20" t="s">
@@ -6343,16 +6433,16 @@
       <c r="E20" t="s">
         <v>198</v>
       </c>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="65"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
@@ -6364,16 +6454,16 @@
       <c r="D21" t="s">
         <v>200</v>
       </c>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="65"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
     </row>
     <row r="22" spans="2:15">
       <c r="C22" t="s">
@@ -6385,16 +6475,16 @@
       <c r="E22" t="s">
         <v>202</v>
       </c>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="65"/>
-      <c r="N22" s="65"/>
-      <c r="O22" s="65"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
     </row>
     <row r="23" spans="2:15">
       <c r="B23" t="s">
@@ -6403,364 +6493,364 @@
       <c r="D23" t="s">
         <v>204</v>
       </c>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="65"/>
-      <c r="N23" s="65"/>
-      <c r="O23" s="65"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="65"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="67"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="65"/>
-      <c r="K25" s="65"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="65"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="65"/>
-      <c r="K26" s="65"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="65"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="67"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="65"/>
-      <c r="K27" s="65"/>
-      <c r="L27" s="65"/>
-      <c r="M27" s="65"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="65"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="67"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="65"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
+      <c r="O28" s="67"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="65"/>
-      <c r="N29" s="65"/>
-      <c r="O29" s="65"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="67"/>
+      <c r="N29" s="67"/>
+      <c r="O29" s="67"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="F30" s="65"/>
-      <c r="G30" s="65"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="65"/>
-      <c r="N30" s="65"/>
-      <c r="O30" s="65"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="67"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="65"/>
-      <c r="M31" s="65"/>
-      <c r="N31" s="65"/>
-      <c r="O31" s="65"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
     </row>
     <row r="32" spans="2:15">
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="65"/>
-      <c r="M32" s="65"/>
-      <c r="N32" s="65"/>
-      <c r="O32" s="65"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="67"/>
+      <c r="J32" s="67"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="67"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="67"/>
     </row>
     <row r="33" spans="6:15">
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="65"/>
-      <c r="K33" s="65"/>
-      <c r="L33" s="65"/>
-      <c r="M33" s="65"/>
-      <c r="N33" s="65"/>
-      <c r="O33" s="65"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="67"/>
+      <c r="O33" s="67"/>
     </row>
     <row r="34" spans="6:15">
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
-      <c r="L34" s="65"/>
-      <c r="M34" s="65"/>
-      <c r="N34" s="65"/>
-      <c r="O34" s="65"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="67"/>
     </row>
     <row r="35" spans="6:15">
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="65"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="65"/>
-      <c r="L35" s="65"/>
-      <c r="M35" s="65"/>
-      <c r="N35" s="65"/>
-      <c r="O35" s="65"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="67"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="67"/>
+      <c r="N35" s="67"/>
+      <c r="O35" s="67"/>
     </row>
     <row r="36" spans="6:15">
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="65"/>
-      <c r="M36" s="65"/>
-      <c r="N36" s="65"/>
-      <c r="O36" s="65"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="67"/>
+      <c r="N36" s="67"/>
+      <c r="O36" s="67"/>
     </row>
     <row r="37" spans="6:15">
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
-      <c r="H37" s="65"/>
-      <c r="I37" s="65"/>
-      <c r="J37" s="65"/>
-      <c r="K37" s="65"/>
-      <c r="L37" s="65"/>
-      <c r="M37" s="65"/>
-      <c r="N37" s="65"/>
-      <c r="O37" s="65"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="67"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="67"/>
+      <c r="N37" s="67"/>
+      <c r="O37" s="67"/>
     </row>
     <row r="38" spans="6:15">
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="65"/>
-      <c r="J38" s="65"/>
-      <c r="K38" s="65"/>
-      <c r="L38" s="65"/>
-      <c r="M38" s="65"/>
-      <c r="N38" s="65"/>
-      <c r="O38" s="65"/>
+      <c r="F38" s="67"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="67"/>
+      <c r="I38" s="67"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="67"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="67"/>
+      <c r="N38" s="67"/>
+      <c r="O38" s="67"/>
     </row>
     <row r="39" spans="6:15">
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="65"/>
-      <c r="K39" s="65"/>
-      <c r="L39" s="65"/>
-      <c r="M39" s="65"/>
-      <c r="N39" s="65"/>
-      <c r="O39" s="65"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="67"/>
+      <c r="O39" s="67"/>
     </row>
     <row r="40" spans="6:15">
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="65"/>
-      <c r="I40" s="65"/>
-      <c r="J40" s="65"/>
-      <c r="K40" s="65"/>
-      <c r="L40" s="65"/>
-      <c r="M40" s="65"/>
-      <c r="N40" s="65"/>
-      <c r="O40" s="65"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="67"/>
+      <c r="K40" s="67"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="67"/>
+      <c r="N40" s="67"/>
+      <c r="O40" s="67"/>
     </row>
     <row r="41" spans="6:15">
-      <c r="F41" s="65"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="65"/>
-      <c r="I41" s="65"/>
-      <c r="J41" s="65"/>
-      <c r="K41" s="65"/>
-      <c r="L41" s="65"/>
-      <c r="M41" s="65"/>
-      <c r="N41" s="65"/>
-      <c r="O41" s="65"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="67"/>
+      <c r="J41" s="67"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="67"/>
+      <c r="M41" s="67"/>
+      <c r="N41" s="67"/>
+      <c r="O41" s="67"/>
     </row>
     <row r="42" spans="6:15">
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="65"/>
-      <c r="L42" s="65"/>
-      <c r="M42" s="65"/>
-      <c r="N42" s="65"/>
-      <c r="O42" s="65"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="67"/>
+      <c r="O42" s="67"/>
     </row>
     <row r="43" spans="6:15">
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="65"/>
-      <c r="I43" s="65"/>
-      <c r="J43" s="65"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="65"/>
-      <c r="M43" s="65"/>
-      <c r="N43" s="65"/>
-      <c r="O43" s="65"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="67"/>
+      <c r="N43" s="67"/>
+      <c r="O43" s="67"/>
     </row>
     <row r="44" spans="6:15">
-      <c r="F44" s="65"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="65"/>
-      <c r="I44" s="65"/>
-      <c r="J44" s="65"/>
-      <c r="K44" s="65"/>
-      <c r="L44" s="65"/>
-      <c r="M44" s="65"/>
-      <c r="N44" s="65"/>
-      <c r="O44" s="65"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="67"/>
+      <c r="M44" s="67"/>
+      <c r="N44" s="67"/>
+      <c r="O44" s="67"/>
     </row>
     <row r="45" spans="6:15">
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="65"/>
-      <c r="I45" s="65"/>
-      <c r="J45" s="65"/>
-      <c r="K45" s="65"/>
-      <c r="L45" s="65"/>
-      <c r="M45" s="65"/>
-      <c r="N45" s="65"/>
-      <c r="O45" s="65"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="67"/>
+      <c r="H45" s="67"/>
+      <c r="I45" s="67"/>
+      <c r="J45" s="67"/>
+      <c r="K45" s="67"/>
+      <c r="L45" s="67"/>
+      <c r="M45" s="67"/>
+      <c r="N45" s="67"/>
+      <c r="O45" s="67"/>
     </row>
     <row r="46" spans="6:15">
-      <c r="F46" s="65"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="65"/>
-      <c r="I46" s="65"/>
-      <c r="J46" s="65"/>
-      <c r="K46" s="65"/>
-      <c r="L46" s="65"/>
-      <c r="M46" s="65"/>
-      <c r="N46" s="65"/>
-      <c r="O46" s="65"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="67"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
+      <c r="L46" s="67"/>
+      <c r="M46" s="67"/>
+      <c r="N46" s="67"/>
+      <c r="O46" s="67"/>
     </row>
     <row r="47" spans="6:15">
-      <c r="F47" s="65"/>
-      <c r="G47" s="65"/>
-      <c r="H47" s="65"/>
-      <c r="I47" s="65"/>
-      <c r="J47" s="65"/>
-      <c r="K47" s="65"/>
-      <c r="L47" s="65"/>
-      <c r="M47" s="65"/>
-      <c r="N47" s="65"/>
-      <c r="O47" s="65"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="67"/>
+      <c r="J47" s="67"/>
+      <c r="K47" s="67"/>
+      <c r="L47" s="67"/>
+      <c r="M47" s="67"/>
+      <c r="N47" s="67"/>
+      <c r="O47" s="67"/>
     </row>
     <row r="48" spans="6:15">
-      <c r="F48" s="65"/>
-      <c r="G48" s="65"/>
-      <c r="H48" s="65"/>
-      <c r="I48" s="65"/>
-      <c r="J48" s="65"/>
-      <c r="K48" s="65"/>
-      <c r="L48" s="65"/>
-      <c r="M48" s="65"/>
-      <c r="N48" s="65"/>
-      <c r="O48" s="65"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="67"/>
+      <c r="K48" s="67"/>
+      <c r="L48" s="67"/>
+      <c r="M48" s="67"/>
+      <c r="N48" s="67"/>
+      <c r="O48" s="67"/>
     </row>
     <row r="49" spans="6:15">
-      <c r="F49" s="65"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="65"/>
-      <c r="I49" s="65"/>
-      <c r="J49" s="65"/>
-      <c r="K49" s="65"/>
-      <c r="L49" s="65"/>
-      <c r="M49" s="65"/>
-      <c r="N49" s="65"/>
-      <c r="O49" s="65"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="67"/>
+      <c r="I49" s="67"/>
+      <c r="J49" s="67"/>
+      <c r="K49" s="67"/>
+      <c r="L49" s="67"/>
+      <c r="M49" s="67"/>
+      <c r="N49" s="67"/>
+      <c r="O49" s="67"/>
     </row>
     <row r="50" spans="6:15">
-      <c r="F50" s="65"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="65"/>
-      <c r="I50" s="65"/>
-      <c r="J50" s="65"/>
-      <c r="K50" s="65"/>
-      <c r="L50" s="65"/>
-      <c r="M50" s="65"/>
-      <c r="N50" s="65"/>
-      <c r="O50" s="65"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="67"/>
+      <c r="H50" s="67"/>
+      <c r="I50" s="67"/>
+      <c r="J50" s="67"/>
+      <c r="K50" s="67"/>
+      <c r="L50" s="67"/>
+      <c r="M50" s="67"/>
+      <c r="N50" s="67"/>
+      <c r="O50" s="67"/>
     </row>
     <row r="51" spans="6:15">
-      <c r="F51" s="65"/>
-      <c r="G51" s="65"/>
-      <c r="H51" s="65"/>
-      <c r="I51" s="65"/>
-      <c r="J51" s="65"/>
-      <c r="K51" s="65"/>
-      <c r="L51" s="65"/>
-      <c r="M51" s="65"/>
-      <c r="N51" s="65"/>
-      <c r="O51" s="65"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="67"/>
+      <c r="I51" s="67"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="67"/>
+      <c r="L51" s="67"/>
+      <c r="M51" s="67"/>
+      <c r="N51" s="67"/>
+      <c r="O51" s="67"/>
     </row>
     <row r="52" spans="6:15">
-      <c r="F52" s="65"/>
-      <c r="G52" s="65"/>
-      <c r="H52" s="65"/>
-      <c r="I52" s="65"/>
-      <c r="J52" s="65"/>
-      <c r="K52" s="65"/>
-      <c r="L52" s="65"/>
-      <c r="M52" s="65"/>
-      <c r="N52" s="65"/>
-      <c r="O52" s="65"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67"/>
+      <c r="I52" s="67"/>
+      <c r="J52" s="67"/>
+      <c r="K52" s="67"/>
+      <c r="L52" s="67"/>
+      <c r="M52" s="67"/>
+      <c r="N52" s="67"/>
+      <c r="O52" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>